<commit_message>
updated using settings and removed lines
</commit_message>
<xml_diff>
--- a/Spreadsheets/Capability Matrix.xlsx
+++ b/Spreadsheets/Capability Matrix.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26101"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maraspeli/Documents/Work/Agile/FocusedObjective.Resources/Spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Troy\Dropbox\Private\GitHub\FocusedObjective.Resources\Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2020" yWindow="500" windowWidth="26780" windowHeight="17500"/>
+    <workbookView xWindow="90" yWindow="75" windowWidth="19140" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="6" r:id="rId1"/>
@@ -24,12 +24,7 @@
     <definedName name="Skills_Header" localSheetId="6">Settings!#REF!</definedName>
     <definedName name="Skills_Header">Settings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -317,16 +312,16 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -334,10 +329,10 @@
       <left/>
       <right/>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="double">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -355,7 +350,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -12480,12 +12475,12 @@
   <dimension ref="B1:Q23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:17" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="35" t="s">
         <v>40</v>
       </c>
@@ -12502,12 +12497,12 @@
       <c r="M1" s="35"/>
       <c r="N1" s="35"/>
     </row>
-    <row r="2" spans="2:17" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="P2" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="P4" s="27">
         <v>1</v>
       </c>
@@ -12515,7 +12510,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="P5" s="27">
         <v>1.1000000000000001</v>
       </c>
@@ -12523,58 +12518,58 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="P6" s="27"/>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="P7" s="27"/>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="P8" s="27"/>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="P9" s="27"/>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="P10" s="27"/>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="P11" s="27"/>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="P12" s="27"/>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="P13" s="27"/>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="P14" s="27"/>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="P15" s="27"/>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="P16" s="27"/>
     </row>
-    <row r="17" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P17" s="27"/>
     </row>
-    <row r="18" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P18" s="27"/>
     </row>
-    <row r="19" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P19" s="27"/>
     </row>
-    <row r="20" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P20" s="27"/>
     </row>
-    <row r="21" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P21" s="27"/>
     </row>
-    <row r="22" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P22" s="27"/>
     </row>
-    <row r="23" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P23" s="27"/>
     </row>
   </sheetData>
@@ -12590,24 +12585,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:K22"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" customWidth="1"/>
-    <col min="2" max="2" width="47.1640625" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" customWidth="1"/>
-    <col min="4" max="4" width="56.6640625" customWidth="1"/>
-    <col min="5" max="5" width="6.1640625" customWidth="1"/>
-    <col min="6" max="6" width="5.6640625" customWidth="1"/>
-    <col min="7" max="7" width="39.33203125" customWidth="1"/>
-    <col min="8" max="8" width="5.1640625" customWidth="1"/>
-    <col min="9" max="9" width="48.6640625" customWidth="1"/>
-    <col min="10" max="10" width="5.33203125" customWidth="1"/>
-    <col min="11" max="11" width="23.83203125" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="2" max="2" width="47.140625" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="56.7109375" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" customWidth="1"/>
+    <col min="7" max="7" width="39.28515625" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" customWidth="1"/>
+    <col min="9" max="9" width="48.7109375" customWidth="1"/>
+    <col min="10" max="10" width="5.28515625" customWidth="1"/>
+    <col min="11" max="11" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>28</v>
       </c>
@@ -12624,7 +12621,7 @@
       </c>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="26" t="s">
         <v>5</v>
       </c>
@@ -12638,7 +12635,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
         <v>33</v>
       </c>
@@ -12652,7 +12649,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
         <v>18</v>
       </c>
@@ -12666,7 +12663,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="26"/>
       <c r="D9" s="25"/>
       <c r="G9" s="25" t="s">
@@ -12676,7 +12673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="26"/>
       <c r="D10" s="25"/>
       <c r="G10" s="25" t="s">
@@ -12686,47 +12683,47 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="26"/>
       <c r="D11" s="25"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="26"/>
       <c r="D12" s="25"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="26"/>
       <c r="D13" s="25"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="26"/>
       <c r="D14" s="25"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="26"/>
       <c r="D15" s="25"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="26"/>
       <c r="D16" s="25"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="26"/>
       <c r="D17" s="25"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D18" s="25"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D19" s="25"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D20" s="25"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D21" s="25"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D22" s="25"/>
     </row>
   </sheetData>
@@ -12740,21 +12737,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.5" style="15" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="15" customWidth="1"/>
-    <col min="3" max="4" width="14.33203125" style="15" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="15" customWidth="1"/>
-    <col min="6" max="6" width="15.5" style="15" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="15"/>
+    <col min="1" max="1" width="24.42578125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="15" customWidth="1"/>
+    <col min="3" max="4" width="14.28515625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="15" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="15" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="36" t="s">
         <v>41</v>
       </c>
@@ -12764,7 +12761,7 @@
       <c r="E1" s="36"/>
       <c r="F1" s="36"/>
     </row>
-    <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:6" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
         <v>19</v>
@@ -12785,7 +12782,7 @@
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="14"/>
     </row>
-    <row r="7" spans="1:6" s="22" customFormat="1" ht="34.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" s="22" customFormat="1" ht="34.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="23" t="str">
         <f>Settings!$G$6</f>
         <v>Know nothing</v>
@@ -12994,12 +12991,12 @@
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
     </row>
-    <row r="25" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="31.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="18" customFormat="1" ht="28" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="22"/>
       <c r="B27" s="23" t="str">
         <f>Settings!$I$6</f>
@@ -13227,17 +13224,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="29.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="29.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="35.33203125" customWidth="1"/>
-    <col min="3" max="3" width="32.83203125" customWidth="1"/>
+    <col min="1" max="1" width="32.28515625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" customWidth="1"/>
     <col min="4" max="4" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="30"/>
       <c r="B1" s="31" t="str">
         <f>IF(ISBLANK(Settings!$D6),"",Settings!$D6)</f>
@@ -13308,7 +13307,7 @@
         <v/>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="str">
         <f>IF(ISBLANK(Settings!B6),"",Settings!B6)</f>
         <v>Person 1</v>
@@ -13337,7 +13336,7 @@
       <c r="Q2" s="25"/>
       <c r="R2" s="25"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="str">
         <f>IF(ISBLANK(Settings!B7),"",Settings!B7)</f>
         <v>Person 2</v>
@@ -13366,7 +13365,7 @@
       <c r="Q3" s="25"/>
       <c r="R3" s="25"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="str">
         <f>IF(ISBLANK(Settings!B8),"",Settings!B8)</f>
         <v>Team 1</v>
@@ -13395,7 +13394,7 @@
       <c r="Q4" s="25"/>
       <c r="R4" s="25"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="str">
         <f>IF(ISBLANK(Settings!B9),"",Settings!B9)</f>
         <v/>
@@ -13418,7 +13417,7 @@
       <c r="Q5" s="25"/>
       <c r="R5" s="25"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="str">
         <f>IF(ISBLANK(Settings!B10),"",Settings!B10)</f>
         <v/>
@@ -13441,7 +13440,7 @@
       <c r="Q6" s="25"/>
       <c r="R6" s="25"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="str">
         <f>IF(ISBLANK(Settings!B11),"",Settings!B11)</f>
         <v/>
@@ -13464,7 +13463,7 @@
       <c r="Q7" s="25"/>
       <c r="R7" s="25"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="str">
         <f>IF(ISBLANK(Settings!B12),"",Settings!B12)</f>
         <v/>
@@ -13487,7 +13486,7 @@
       <c r="Q8" s="25"/>
       <c r="R8" s="25"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="str">
         <f>IF(ISBLANK(Settings!B13),"",Settings!B13)</f>
         <v/>
@@ -13510,7 +13509,7 @@
       <c r="Q9" s="25"/>
       <c r="R9" s="25"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="str">
         <f>IF(ISBLANK(Settings!B14),"",Settings!B14)</f>
         <v/>
@@ -13533,7 +13532,7 @@
       <c r="Q10" s="25"/>
       <c r="R10" s="25"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="str">
         <f>IF(ISBLANK(Settings!B15),"",Settings!B15)</f>
         <v/>
@@ -13556,7 +13555,7 @@
       <c r="Q11" s="25"/>
       <c r="R11" s="25"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="str">
         <f>IF(ISBLANK(Settings!B16),"",Settings!B16)</f>
         <v/>
@@ -13579,7 +13578,7 @@
       <c r="Q12" s="25"/>
       <c r="R12" s="25"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="str">
         <f>IF(ISBLANK(Settings!B17),"",Settings!B17)</f>
         <v/>
@@ -13602,13 +13601,13 @@
       <c r="Q13" s="25"/>
       <c r="R13" s="25"/>
     </row>
-    <row r="14" spans="1:18" ht="12.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:18" ht="19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="32"/>
       <c r="B16" s="34" t="str">
         <f>IF(B1&lt;&gt;"",B1,"")</f>
@@ -13679,7 +13678,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
         <v>35</v>
       </c>
@@ -13752,7 +13751,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
         <v>34</v>
       </c>
@@ -13825,7 +13824,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="33" t="s">
         <v>36</v>
       </c>
@@ -13955,12 +13954,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -14033,7 +14032,7 @@
         <v/>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -14106,7 +14105,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -14179,7 +14178,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="str">
         <f>IF('Current Assessment'!B1&lt;&gt;"",'Current Assessment'!B1,"")</f>
         <v>CSS</v>
@@ -14249,7 +14248,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="str">
         <f>'Current Assessment'!A2</f>
         <v>Person 1</v>
@@ -14323,7 +14322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="str">
         <f>'Current Assessment'!A3</f>
         <v>Person 2</v>
@@ -14397,7 +14396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="str">
         <f>'Current Assessment'!A4</f>
         <v>Team 1</v>
@@ -14471,7 +14470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="str">
         <f>'Current Assessment'!A5</f>
         <v/>
@@ -14545,7 +14544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="str">
         <f>'Current Assessment'!A6</f>
         <v/>
@@ -14619,7 +14618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="str">
         <f>'Current Assessment'!A7</f>
         <v/>
@@ -14693,7 +14692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="str">
         <f>'Current Assessment'!A8</f>
         <v/>
@@ -14767,7 +14766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="str">
         <f>'Current Assessment'!A9</f>
         <v/>
@@ -14841,7 +14840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="str">
         <f>'Current Assessment'!A10</f>
         <v/>
@@ -14915,7 +14914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="str">
         <f>'Current Assessment'!A11</f>
         <v/>
@@ -14989,7 +14988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="str">
         <f>'Current Assessment'!A12</f>
         <v/>
@@ -15063,7 +15062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="str">
         <f>'Current Assessment'!A13</f>
         <v/>
@@ -15137,7 +15136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="6">
         <f t="shared" ref="B17:R17" si="3">SUM(B5:B16)</f>
         <v>4</v>
@@ -15207,13 +15206,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:18" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>27</v>
       </c>
@@ -15281,12 +15280,12 @@
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="24.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="24.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.83203125" style="9"/>
+    <col min="1" max="1" width="24.85546875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13"/>
       <c r="B1" s="13" t="str">
         <f>IF('Current Assessment'!B1&lt;&gt;"",'Current Assessment'!B1,"")</f>
@@ -15369,7 +15368,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="str">
         <f>IF('Current Assessment'!A2&lt;&gt;"", 'Current Assessment'!A2, "")</f>
         <v>Person 1</v>
@@ -15401,7 +15400,7 @@
       <c r="T2" s="12"/>
       <c r="U2" s="12"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="str">
         <f>IF('Current Assessment'!A3&lt;&gt;"", 'Current Assessment'!A3, "")</f>
         <v>Person 2</v>
@@ -15429,7 +15428,7 @@
       <c r="T3" s="12"/>
       <c r="U3" s="12"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="str">
         <f>IF('Current Assessment'!A4&lt;&gt;"", 'Current Assessment'!A4, "")</f>
         <v>Team 1</v>
@@ -15455,7 +15454,7 @@
       <c r="T4" s="12"/>
       <c r="U4" s="12"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="str">
         <f>IF('Current Assessment'!A5&lt;&gt;"", 'Current Assessment'!A5, "")</f>
         <v/>
@@ -15481,7 +15480,7 @@
       <c r="T5" s="12"/>
       <c r="U5" s="12"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="str">
         <f>IF('Current Assessment'!A6&lt;&gt;"", 'Current Assessment'!A6, "")</f>
         <v/>
@@ -15507,7 +15506,7 @@
       <c r="T6" s="12"/>
       <c r="U6" s="12"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="str">
         <f>IF('Current Assessment'!A7&lt;&gt;"", 'Current Assessment'!A7, "")</f>
         <v/>
@@ -15533,7 +15532,7 @@
       <c r="T7" s="12"/>
       <c r="U7" s="12"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="str">
         <f>IF('Current Assessment'!A8&lt;&gt;"", 'Current Assessment'!A8, "")</f>
         <v/>
@@ -15559,7 +15558,7 @@
       <c r="T8" s="12"/>
       <c r="U8" s="12"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="str">
         <f>IF('Current Assessment'!A9&lt;&gt;"", 'Current Assessment'!A9, "")</f>
         <v/>
@@ -15585,7 +15584,7 @@
       <c r="T9" s="12"/>
       <c r="U9" s="12"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="str">
         <f>IF('Current Assessment'!A10&lt;&gt;"", 'Current Assessment'!A10, "")</f>
         <v/>
@@ -15611,7 +15610,7 @@
       <c r="T10" s="12"/>
       <c r="U10" s="12"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="str">
         <f>IF('Current Assessment'!A11&lt;&gt;"", 'Current Assessment'!A11, "")</f>
         <v/>
@@ -15637,7 +15636,7 @@
       <c r="T11" s="12"/>
       <c r="U11" s="12"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="str">
         <f>IF('Current Assessment'!A12&lt;&gt;"", 'Current Assessment'!A12, "")</f>
         <v/>
@@ -15663,7 +15662,7 @@
       <c r="T12" s="12"/>
       <c r="U12" s="12"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="str">
         <f>IF('Current Assessment'!A13&lt;&gt;"", 'Current Assessment'!A13, "")</f>
         <v/>
@@ -15689,7 +15688,7 @@
       <c r="T13" s="12"/>
       <c r="U13" s="12"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="e">
         <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
         <v>#REF!</v>
@@ -15715,7 +15714,7 @@
       <c r="T14" s="12"/>
       <c r="U14" s="12"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="e">
         <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
         <v>#REF!</v>
@@ -15741,7 +15740,7 @@
       <c r="T15" s="12"/>
       <c r="U15" s="12"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="e">
         <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
         <v>#REF!</v>
@@ -15767,7 +15766,7 @@
       <c r="T16" s="12"/>
       <c r="U16" s="12"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="e">
         <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
         <v>#REF!</v>
@@ -15793,7 +15792,7 @@
       <c r="T17" s="12"/>
       <c r="U17" s="12"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="e">
         <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
         <v>#REF!</v>
@@ -15819,7 +15818,7 @@
       <c r="T18" s="12"/>
       <c r="U18" s="12"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="e">
         <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
         <v>#REF!</v>
@@ -15845,7 +15844,7 @@
       <c r="T19" s="12"/>
       <c r="U19" s="12"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="e">
         <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
         <v>#REF!</v>
@@ -15871,7 +15870,7 @@
       <c r="T20" s="12"/>
       <c r="U20" s="12"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="e">
         <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
         <v>#REF!</v>
@@ -15897,12 +15896,12 @@
       <c r="T21" s="12"/>
       <c r="U21" s="12"/>
     </row>
-    <row r="23" spans="1:21" ht="19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="3" t="str">
         <f>IF(B1&lt;&gt;"",B1,"")</f>
@@ -15985,7 +15984,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>0</v>
       </c>
@@ -16070,7 +16069,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>17</v>
       </c>
@@ -16155,7 +16154,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>16</v>
       </c>
@@ -16293,15 +16292,15 @@
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.5" customWidth="1"/>
-    <col min="6" max="6" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -16386,7 +16385,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -16471,7 +16470,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -16556,7 +16555,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="str">
         <f>IF('Current Assessment'!B1&lt;&gt;"",'Current Assessment'!B1,"")</f>
         <v>CSS</v>
@@ -16638,7 +16637,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="str">
         <f>'Current Assessment'!A2</f>
         <v>Person 1</v>
@@ -16724,7 +16723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="str">
         <f>'Current Assessment'!A3</f>
         <v>Person 2</v>
@@ -16810,7 +16809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="str">
         <f>'Current Assessment'!A4</f>
         <v>Team 1</v>
@@ -16896,7 +16895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="str">
         <f>'Current Assessment'!A5</f>
         <v/>
@@ -16982,7 +16981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="str">
         <f>'Current Assessment'!A6</f>
         <v/>
@@ -17068,7 +17067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="str">
         <f>'Current Assessment'!A7</f>
         <v/>
@@ -17154,7 +17153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="str">
         <f>'Current Assessment'!A8</f>
         <v/>
@@ -17240,7 +17239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="str">
         <f>'Current Assessment'!A9</f>
         <v/>
@@ -17326,7 +17325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="str">
         <f>'Current Assessment'!A10</f>
         <v/>
@@ -17412,7 +17411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="str">
         <f>'Current Assessment'!A11</f>
         <v/>
@@ -17498,7 +17497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="str">
         <f>'Current Assessment'!A12</f>
         <v/>
@@ -17584,7 +17583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="str">
         <f>'Current Assessment'!A13</f>
         <v/>
@@ -17670,7 +17669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="e">
         <f>'Current Assessment'!#REF!</f>
         <v>#REF!</v>
@@ -17756,7 +17755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="e">
         <f>'Current Assessment'!#REF!</f>
         <v>#REF!</v>
@@ -17842,7 +17841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="e">
         <f>'Current Assessment'!#REF!</f>
         <v>#REF!</v>
@@ -17928,7 +17927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="e">
         <f>'Current Assessment'!#REF!</f>
         <v>#REF!</v>
@@ -18014,7 +18013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="e">
         <f>'Current Assessment'!#REF!</f>
         <v>#REF!</v>
@@ -18100,7 +18099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="e">
         <f>'Current Assessment'!#REF!</f>
         <v>#REF!</v>
@@ -18186,7 +18185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="e">
         <f>'Current Assessment'!#REF!</f>
         <v>#REF!</v>
@@ -18272,7 +18271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="e">
         <f>'Current Assessment'!#REF!</f>
         <v>#REF!</v>
@@ -18358,7 +18357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="6">
         <f>SUM(B5:B24)</f>
         <v>4</v>
@@ -18440,7 +18439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="B5:U24">
     <cfRule type="colorScale" priority="3">

</xml_diff>

<commit_message>
Expanded version supporting 5000 samples rather than 1250
</commit_message>
<xml_diff>
--- a/Spreadsheets/Capability Matrix.xlsx
+++ b/Spreadsheets/Capability Matrix.xlsx
@@ -1,35 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Troy\Dropbox\Private\GitHub\FocusedObjective.Resources\Spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Private\GitHub\FocusedObjective.Resources\Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="90" yWindow="75" windowWidth="19140" windowHeight="9525"/>
+    <workbookView xWindow="90" yWindow="765" windowWidth="19140" windowHeight="9525" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="6" r:id="rId1"/>
     <sheet name="Settings" sheetId="2" r:id="rId2"/>
     <sheet name="Survey Sheet" sheetId="5" r:id="rId3"/>
-    <sheet name="Current Assessment" sheetId="1" r:id="rId4"/>
-    <sheet name="Current_Calcs" sheetId="4" state="hidden" r:id="rId5"/>
-    <sheet name="Willingness" sheetId="3" state="hidden" r:id="rId6"/>
-    <sheet name="Willingness_Calcs" sheetId="7" state="hidden" r:id="rId7"/>
+    <sheet name="Input" sheetId="1" r:id="rId4"/>
+    <sheet name="Heatmap" sheetId="4" r:id="rId5"/>
+    <sheet name="Splitability" sheetId="8" r:id="rId6"/>
+    <sheet name="Willingness" sheetId="3" state="hidden" r:id="rId7"/>
+    <sheet name="Willingness_Calcs" sheetId="7" state="hidden" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="Skills_Header" localSheetId="6">Settings!#REF!</definedName>
+    <definedName name="Skills_Header" localSheetId="7">Settings!#REF!</definedName>
     <definedName name="Skills_Header">Settings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
   <si>
     <t>Willing</t>
   </si>
@@ -49,19 +50,10 @@
     <t>Person 1</t>
   </si>
   <si>
-    <t>Captains: Ability to Create (# &gt;= 3)</t>
-  </si>
-  <si>
-    <t>Players: Ability to Maintain (# &gt;= 2)</t>
-  </si>
-  <si>
     <t>Your Name:</t>
   </si>
   <si>
     <t>Analysis:</t>
-  </si>
-  <si>
-    <t>Bench: Ready to Train Up (# = 1)</t>
   </si>
   <si>
     <t>I'd quit rather than do this…</t>
@@ -101,9 +93,6 @@
   </si>
   <si>
     <t>Can start from nothing and create</t>
-  </si>
-  <si>
-    <t>Expert level</t>
   </si>
   <si>
     <t>For each capability choose from the list of CURRENT skill level values. If in doubt, err low (left)!</t>
@@ -148,19 +137,58 @@
     <t>Initial Version</t>
   </si>
   <si>
-    <t>Made all setting in the Setting tab.</t>
-  </si>
-  <si>
     <t>Staff and Team Capability Matrix</t>
   </si>
   <si>
     <t>Capability Survey For Printing (enter skills in the Settings worksheet)</t>
   </si>
+  <si>
+    <t>Quick Analysis:</t>
+  </si>
+  <si>
+    <t>Can teach others</t>
+  </si>
+  <si>
+    <t>Made all settings definable in the Setting tab.</t>
+  </si>
+  <si>
+    <t>no teacher</t>
+  </si>
+  <si>
+    <t>1 teacher</t>
+  </si>
+  <si>
+    <t>no doer</t>
+  </si>
+  <si>
+    <t>1 doer</t>
+  </si>
+  <si>
+    <t>no novice</t>
+  </si>
+  <si>
+    <t>1 novice</t>
+  </si>
+  <si>
+    <t>no doer. 1 Novice</t>
+  </si>
+  <si>
+    <t>teach novice into doer - URGENT</t>
+  </si>
+  <si>
+    <t>1 doer, 1 novice</t>
+  </si>
+  <si>
+    <t>teach novice into doer - SOON</t>
+  </si>
+  <si>
+    <t>hire teacher level or  external consultant. Create doers, then train one into teacher</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -287,7 +315,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -378,6 +406,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -388,7 +427,7 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -442,6 +481,8 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -11868,7 +11909,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>Novice &amp; LEarner (bench)</a:t>
+            <a:t>Novice &amp; Learner (bench)</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
@@ -11975,75 +12016,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>527685</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>32385</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>59055</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4013835" y="1556385"/>
-          <a:ext cx="6846570" cy="1386840"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFF00"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2400" b="1"/>
-            <a:t>Do not edit this sheet directly. This is the formulas for converting and counting current capability. If you want to add people, do it in the current tab. </a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
       <xdr:colOff>1150620</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
@@ -12116,7 +12088,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -12472,34 +12444,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:Q23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
+      <c r="B1" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
     </row>
     <row r="2" spans="2:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="P2" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
@@ -12507,7 +12480,7 @@
         <v>1</v>
       </c>
       <c r="Q4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
@@ -12583,10 +12556,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="B5:K22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12606,18 +12580,18 @@
   <sheetData>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="K5" s="2"/>
     </row>
@@ -12629,45 +12603,45 @@
         <v>3</v>
       </c>
       <c r="G6" s="25" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I6" s="25" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D7" s="25" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I7" s="25" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I8" s="25" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="26"/>
       <c r="D9" s="25"/>
       <c r="G9" s="25" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I9" s="25" t="s">
         <v>1</v>
@@ -12677,7 +12651,7 @@
       <c r="B10" s="26"/>
       <c r="D10" s="25"/>
       <c r="G10" s="25" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="I10" s="25" t="s">
         <v>2</v>
@@ -12735,10 +12709,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12752,31 +12727,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
+      <c r="A1" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:6" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="20" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -12801,12 +12776,12 @@
       </c>
       <c r="F7" s="23" t="str">
         <f>Settings!$G$10</f>
-        <v>Expert level</v>
+        <v>Can teach others</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="str">
-        <f>IF('Current Assessment'!B1&lt;&gt;"", 'Current Assessment'!B1, "")</f>
+        <f>IF(Input!B1&lt;&gt;"", Input!B1, "")</f>
         <v>CSS</v>
       </c>
       <c r="B8" s="17"/>
@@ -12817,7 +12792,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="str">
-        <f>IF('Current Assessment'!C1&lt;&gt;"", 'Current Assessment'!C1, "")</f>
+        <f>IF(Input!C1&lt;&gt;"", Input!C1, "")</f>
         <v>Javascript</v>
       </c>
       <c r="B9" s="17"/>
@@ -12828,7 +12803,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="str">
-        <f>IF('Current Assessment'!D1&lt;&gt;"", 'Current Assessment'!D1, "")</f>
+        <f>IF(Input!D1&lt;&gt;"", Input!D1, "")</f>
         <v>DB Backup/Restore</v>
       </c>
       <c r="B10" s="17"/>
@@ -12839,7 +12814,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="str">
-        <f>IF('Current Assessment'!E1&lt;&gt;"", 'Current Assessment'!E1, "")</f>
+        <f>IF(Input!E1&lt;&gt;"", Input!E1, "")</f>
         <v/>
       </c>
       <c r="B11" s="17"/>
@@ -12850,7 +12825,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="str">
-        <f>IF('Current Assessment'!F1&lt;&gt;"", 'Current Assessment'!F1, "")</f>
+        <f>IF(Input!F1&lt;&gt;"", Input!F1, "")</f>
         <v/>
       </c>
       <c r="B12" s="17"/>
@@ -12861,7 +12836,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="str">
-        <f>IF('Current Assessment'!G1&lt;&gt;"", 'Current Assessment'!G1, "")</f>
+        <f>IF(Input!G1&lt;&gt;"", Input!G1, "")</f>
         <v/>
       </c>
       <c r="B13" s="17"/>
@@ -12872,7 +12847,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="str">
-        <f>IF('Current Assessment'!H1&lt;&gt;"", 'Current Assessment'!H1, "")</f>
+        <f>IF(Input!H1&lt;&gt;"", Input!H1, "")</f>
         <v/>
       </c>
       <c r="B14" s="17"/>
@@ -12883,7 +12858,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="str">
-        <f>IF('Current Assessment'!I1&lt;&gt;"", 'Current Assessment'!I1, "")</f>
+        <f>IF(Input!I1&lt;&gt;"", Input!I1, "")</f>
         <v/>
       </c>
       <c r="B15" s="17"/>
@@ -12894,7 +12869,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="str">
-        <f>IF('Current Assessment'!J1&lt;&gt;"", 'Current Assessment'!J1, "")</f>
+        <f>IF(Input!J1&lt;&gt;"", Input!J1, "")</f>
         <v/>
       </c>
       <c r="B16" s="17"/>
@@ -12905,7 +12880,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="str">
-        <f>IF('Current Assessment'!K1&lt;&gt;"", 'Current Assessment'!K1, "")</f>
+        <f>IF(Input!K1&lt;&gt;"", Input!K1, "")</f>
         <v/>
       </c>
       <c r="B17" s="17"/>
@@ -12916,7 +12891,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="str">
-        <f>IF('Current Assessment'!L1&lt;&gt;"", 'Current Assessment'!L1, "")</f>
+        <f>IF(Input!L1&lt;&gt;"", Input!L1, "")</f>
         <v/>
       </c>
       <c r="B18" s="17"/>
@@ -12927,7 +12902,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="str">
-        <f>IF('Current Assessment'!M1&lt;&gt;"", 'Current Assessment'!M1, "")</f>
+        <f>IF(Input!M1&lt;&gt;"", Input!M1, "")</f>
         <v/>
       </c>
       <c r="B19" s="17"/>
@@ -12938,7 +12913,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="str">
-        <f>IF('Current Assessment'!N1&lt;&gt;"", 'Current Assessment'!N1, "")</f>
+        <f>IF(Input!N1&lt;&gt;"", Input!N1, "")</f>
         <v/>
       </c>
       <c r="B20" s="17"/>
@@ -12949,7 +12924,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="str">
-        <f>IF('Current Assessment'!O1&lt;&gt;"", 'Current Assessment'!O1, "")</f>
+        <f>IF(Input!O1&lt;&gt;"", Input!O1, "")</f>
         <v/>
       </c>
       <c r="B21" s="17"/>
@@ -12960,7 +12935,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="str">
-        <f>IF('Current Assessment'!P1&lt;&gt;"", 'Current Assessment'!P1, "")</f>
+        <f>IF(Input!P1&lt;&gt;"", Input!P1, "")</f>
         <v/>
       </c>
       <c r="B22" s="17"/>
@@ -12971,7 +12946,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="str">
-        <f>IF('Current Assessment'!Q1&lt;&gt;"", 'Current Assessment'!Q1, "")</f>
+        <f>IF(Input!Q1&lt;&gt;"", Input!Q1, "")</f>
         <v/>
       </c>
       <c r="B23" s="17"/>
@@ -12982,7 +12957,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="str">
-        <f>IF('Current Assessment'!R1&lt;&gt;"", 'Current Assessment'!R1, "")</f>
+        <f>IF(Input!R1&lt;&gt;"", Input!R1, "")</f>
         <v/>
       </c>
       <c r="B24" s="17"/>
@@ -12993,7 +12968,7 @@
     </row>
     <row r="25" spans="1:6" ht="31.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -13021,7 +12996,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="str">
-        <f>IF('Current Assessment'!B16&lt;&gt;"", 'Current Assessment'!B16, "")</f>
+        <f>IF(Input!B16&lt;&gt;"", Input!B16, "")</f>
         <v>CSS</v>
       </c>
       <c r="B28" s="17"/>
@@ -13032,7 +13007,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="str">
-        <f>IF('Current Assessment'!C16&lt;&gt;"", 'Current Assessment'!C16, "")</f>
+        <f>IF(Input!C16&lt;&gt;"", Input!C16, "")</f>
         <v>Javascript</v>
       </c>
       <c r="B29" s="17"/>
@@ -13043,7 +13018,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="16" t="str">
-        <f>IF('Current Assessment'!D16&lt;&gt;"", 'Current Assessment'!D16, "")</f>
+        <f>IF(Input!D16&lt;&gt;"", Input!D16, "")</f>
         <v>DB Backup/Restore</v>
       </c>
       <c r="B30" s="17"/>
@@ -13054,7 +13029,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="str">
-        <f>IF('Current Assessment'!E16&lt;&gt;"", 'Current Assessment'!E16, "")</f>
+        <f>IF(Input!E16&lt;&gt;"", Input!E16, "")</f>
         <v/>
       </c>
       <c r="B31" s="17"/>
@@ -13065,7 +13040,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="16" t="str">
-        <f>IF('Current Assessment'!F16&lt;&gt;"", 'Current Assessment'!F16, "")</f>
+        <f>IF(Input!F16&lt;&gt;"", Input!F16, "")</f>
         <v/>
       </c>
       <c r="B32" s="17"/>
@@ -13076,7 +13051,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="16" t="str">
-        <f>IF('Current Assessment'!G16&lt;&gt;"", 'Current Assessment'!G16, "")</f>
+        <f>IF(Input!G16&lt;&gt;"", Input!G16, "")</f>
         <v/>
       </c>
       <c r="B33" s="17"/>
@@ -13087,7 +13062,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="str">
-        <f>IF('Current Assessment'!H16&lt;&gt;"", 'Current Assessment'!H16, "")</f>
+        <f>IF(Input!H16&lt;&gt;"", Input!H16, "")</f>
         <v/>
       </c>
       <c r="B34" s="17"/>
@@ -13098,7 +13073,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="16" t="str">
-        <f>IF('Current Assessment'!I16&lt;&gt;"", 'Current Assessment'!I16, "")</f>
+        <f>IF(Input!I16&lt;&gt;"", Input!I16, "")</f>
         <v/>
       </c>
       <c r="B35" s="17"/>
@@ -13109,7 +13084,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="16" t="str">
-        <f>IF('Current Assessment'!J16&lt;&gt;"", 'Current Assessment'!J16, "")</f>
+        <f>IF(Input!J16&lt;&gt;"", Input!J16, "")</f>
         <v/>
       </c>
       <c r="B36" s="17"/>
@@ -13120,7 +13095,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="16" t="str">
-        <f>IF('Current Assessment'!K16&lt;&gt;"", 'Current Assessment'!K16, "")</f>
+        <f>IF(Input!K16&lt;&gt;"", Input!K16, "")</f>
         <v/>
       </c>
       <c r="B37" s="17"/>
@@ -13131,7 +13106,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="16" t="str">
-        <f>IF('Current Assessment'!L16&lt;&gt;"", 'Current Assessment'!L16, "")</f>
+        <f>IF(Input!L16&lt;&gt;"", Input!L16, "")</f>
         <v/>
       </c>
       <c r="B38" s="17"/>
@@ -13142,7 +13117,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="16" t="str">
-        <f>IF('Current Assessment'!M16&lt;&gt;"", 'Current Assessment'!M16, "")</f>
+        <f>IF(Input!M16&lt;&gt;"", Input!M16, "")</f>
         <v/>
       </c>
       <c r="B39" s="17"/>
@@ -13153,7 +13128,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="16" t="str">
-        <f>IF('Current Assessment'!N16&lt;&gt;"", 'Current Assessment'!N16, "")</f>
+        <f>IF(Input!N16&lt;&gt;"", Input!N16, "")</f>
         <v/>
       </c>
       <c r="B40" s="17"/>
@@ -13164,7 +13139,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="16" t="str">
-        <f>IF('Current Assessment'!O16&lt;&gt;"", 'Current Assessment'!O16, "")</f>
+        <f>IF(Input!O16&lt;&gt;"", Input!O16, "")</f>
         <v/>
       </c>
       <c r="B41" s="17"/>
@@ -13175,7 +13150,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="16" t="str">
-        <f>IF('Current Assessment'!P16&lt;&gt;"", 'Current Assessment'!P16, "")</f>
+        <f>IF(Input!P16&lt;&gt;"", Input!P16, "")</f>
         <v/>
       </c>
       <c r="B42" s="17"/>
@@ -13186,7 +13161,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="16" t="str">
-        <f>IF('Current Assessment'!Q16&lt;&gt;"", 'Current Assessment'!Q16, "")</f>
+        <f>IF(Input!Q16&lt;&gt;"", Input!Q16, "")</f>
         <v/>
       </c>
       <c r="B43" s="17"/>
@@ -13197,7 +13172,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="16" t="str">
-        <f>IF('Current Assessment'!R16&lt;&gt;"", 'Current Assessment'!R16, "")</f>
+        <f>IF(Input!R16&lt;&gt;"", Input!R16, "")</f>
         <v/>
       </c>
       <c r="B44" s="17"/>
@@ -13222,10 +13197,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R19"/>
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13313,13 +13289,13 @@
         <v>Person 1</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E2" s="25"/>
       <c r="F2" s="25"/>
@@ -13342,13 +13318,13 @@
         <v>Person 2</v>
       </c>
       <c r="B3" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="25" t="s">
-        <v>23</v>
-      </c>
       <c r="D3" s="25" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
@@ -13371,13 +13347,13 @@
         <v>Team 1</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C4" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="25" t="s">
         <v>20</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>23</v>
       </c>
       <c r="E4" s="25"/>
       <c r="F4" s="25"/>
@@ -13604,7 +13580,7 @@
     <row r="14" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -13680,221 +13656,287 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B17" s="28">
-        <f>Current_Calcs!B1</f>
+        <f>Heatmap!B1</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="28">
+        <f>Heatmap!C1</f>
         <v>1</v>
       </c>
-      <c r="C17" s="28">
-        <f>Current_Calcs!C1</f>
+      <c r="D17" s="28">
+        <f>Heatmap!D1</f>
         <v>1</v>
       </c>
-      <c r="D17" s="28">
-        <f>Current_Calcs!D1</f>
-        <v>1</v>
-      </c>
       <c r="E17" s="28" t="str">
-        <f>Current_Calcs!E1</f>
+        <f>Heatmap!E1</f>
         <v/>
       </c>
       <c r="F17" s="29" t="str">
-        <f>Current_Calcs!F1</f>
+        <f>Heatmap!F1</f>
         <v/>
       </c>
       <c r="G17" s="29" t="str">
-        <f>Current_Calcs!G1</f>
+        <f>Heatmap!G1</f>
         <v/>
       </c>
       <c r="H17" s="29" t="str">
-        <f>Current_Calcs!H1</f>
+        <f>Heatmap!H1</f>
         <v/>
       </c>
       <c r="I17" s="29" t="str">
-        <f>Current_Calcs!I1</f>
+        <f>Heatmap!I1</f>
         <v/>
       </c>
       <c r="J17" s="29" t="str">
-        <f>Current_Calcs!J1</f>
+        <f>Heatmap!J1</f>
         <v/>
       </c>
       <c r="K17" s="29" t="str">
-        <f>Current_Calcs!K1</f>
+        <f>Heatmap!K1</f>
         <v/>
       </c>
       <c r="L17" s="29" t="str">
-        <f>Current_Calcs!L1</f>
+        <f>Heatmap!L1</f>
         <v/>
       </c>
       <c r="M17" s="29" t="str">
-        <f>Current_Calcs!M1</f>
+        <f>Heatmap!M1</f>
         <v/>
       </c>
       <c r="N17" s="29" t="str">
-        <f>Current_Calcs!N1</f>
+        <f>Heatmap!N1</f>
         <v/>
       </c>
       <c r="O17" s="29" t="str">
-        <f>Current_Calcs!O1</f>
+        <f>Heatmap!O1</f>
         <v/>
       </c>
       <c r="P17" s="29" t="str">
-        <f>Current_Calcs!P1</f>
+        <f>Heatmap!P1</f>
         <v/>
       </c>
       <c r="Q17" s="29" t="str">
-        <f>Current_Calcs!Q1</f>
+        <f>Heatmap!Q1</f>
         <v/>
       </c>
       <c r="R17" s="29" t="str">
-        <f>Current_Calcs!R1</f>
+        <f>Heatmap!R1</f>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B18" s="28">
-        <f>Current_Calcs!B2</f>
+        <f>Heatmap!B2</f>
         <v>1</v>
       </c>
       <c r="C18" s="28">
-        <f>Current_Calcs!C2</f>
+        <f>Heatmap!C2</f>
         <v>1</v>
       </c>
       <c r="D18" s="28">
-        <f>Current_Calcs!D2</f>
+        <f>Heatmap!D2</f>
         <v>2</v>
       </c>
       <c r="E18" s="28" t="str">
-        <f>Current_Calcs!E2</f>
+        <f>Heatmap!E2</f>
         <v/>
       </c>
       <c r="F18" s="29" t="str">
-        <f>Current_Calcs!F2</f>
+        <f>Heatmap!F2</f>
         <v/>
       </c>
       <c r="G18" s="29" t="str">
-        <f>Current_Calcs!G2</f>
+        <f>Heatmap!G2</f>
         <v/>
       </c>
       <c r="H18" s="29" t="str">
-        <f>Current_Calcs!H2</f>
+        <f>Heatmap!H2</f>
         <v/>
       </c>
       <c r="I18" s="29" t="str">
-        <f>Current_Calcs!I2</f>
+        <f>Heatmap!I2</f>
         <v/>
       </c>
       <c r="J18" s="29" t="str">
-        <f>Current_Calcs!J2</f>
+        <f>Heatmap!J2</f>
         <v/>
       </c>
       <c r="K18" s="29" t="str">
-        <f>Current_Calcs!K2</f>
+        <f>Heatmap!K2</f>
         <v/>
       </c>
       <c r="L18" s="29" t="str">
-        <f>Current_Calcs!L2</f>
+        <f>Heatmap!L2</f>
         <v/>
       </c>
       <c r="M18" s="29" t="str">
-        <f>Current_Calcs!M2</f>
+        <f>Heatmap!M2</f>
         <v/>
       </c>
       <c r="N18" s="29" t="str">
-        <f>Current_Calcs!N2</f>
+        <f>Heatmap!N2</f>
         <v/>
       </c>
       <c r="O18" s="29" t="str">
-        <f>Current_Calcs!O2</f>
+        <f>Heatmap!O2</f>
         <v/>
       </c>
       <c r="P18" s="29" t="str">
-        <f>Current_Calcs!P2</f>
+        <f>Heatmap!P2</f>
         <v/>
       </c>
       <c r="Q18" s="29" t="str">
-        <f>Current_Calcs!Q2</f>
+        <f>Heatmap!Q2</f>
         <v/>
       </c>
       <c r="R18" s="29" t="str">
-        <f>Current_Calcs!R2</f>
+        <f>Heatmap!R2</f>
         <v/>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="33" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B19" s="28">
-        <f>Current_Calcs!B3</f>
+        <f>Heatmap!B3</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="28">
+        <f>Heatmap!C3</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="28">
+        <f>Heatmap!D3</f>
         <v>1</v>
       </c>
-      <c r="C19" s="28">
-        <f>Current_Calcs!C3</f>
-        <v>0</v>
-      </c>
-      <c r="D19" s="28">
-        <f>Current_Calcs!D3</f>
+      <c r="E19" s="28" t="str">
+        <f>Heatmap!E3</f>
+        <v/>
+      </c>
+      <c r="F19" s="29" t="str">
+        <f>Heatmap!F3</f>
+        <v/>
+      </c>
+      <c r="G19" s="29" t="str">
+        <f>Heatmap!G3</f>
+        <v/>
+      </c>
+      <c r="H19" s="29" t="str">
+        <f>Heatmap!H3</f>
+        <v/>
+      </c>
+      <c r="I19" s="29" t="str">
+        <f>Heatmap!I3</f>
+        <v/>
+      </c>
+      <c r="J19" s="29" t="str">
+        <f>Heatmap!J3</f>
+        <v/>
+      </c>
+      <c r="K19" s="29" t="str">
+        <f>Heatmap!K3</f>
+        <v/>
+      </c>
+      <c r="L19" s="29" t="str">
+        <f>Heatmap!L3</f>
+        <v/>
+      </c>
+      <c r="M19" s="29" t="str">
+        <f>Heatmap!M3</f>
+        <v/>
+      </c>
+      <c r="N19" s="29" t="str">
+        <f>Heatmap!N3</f>
+        <v/>
+      </c>
+      <c r="O19" s="29" t="str">
+        <f>Heatmap!O3</f>
+        <v/>
+      </c>
+      <c r="P19" s="29" t="str">
+        <f>Heatmap!P3</f>
+        <v/>
+      </c>
+      <c r="Q19" s="29" t="str">
+        <f>Heatmap!Q3</f>
+        <v/>
+      </c>
+      <c r="R19" s="29" t="str">
+        <f>Heatmap!R3</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30">
         <v>1</v>
       </c>
-      <c r="E19" s="28" t="str">
-        <f>Current_Calcs!E3</f>
-        <v/>
-      </c>
-      <c r="F19" s="29" t="str">
-        <f>Current_Calcs!F3</f>
-        <v/>
-      </c>
-      <c r="G19" s="29" t="str">
-        <f>Current_Calcs!G3</f>
-        <v/>
-      </c>
-      <c r="H19" s="29" t="str">
-        <f>Current_Calcs!H3</f>
-        <v/>
-      </c>
-      <c r="I19" s="29" t="str">
-        <f>Current_Calcs!I3</f>
-        <v/>
-      </c>
-      <c r="J19" s="29" t="str">
-        <f>Current_Calcs!J3</f>
-        <v/>
-      </c>
-      <c r="K19" s="29" t="str">
-        <f>Current_Calcs!K3</f>
-        <v/>
-      </c>
-      <c r="L19" s="29" t="str">
-        <f>Current_Calcs!L3</f>
-        <v/>
-      </c>
-      <c r="M19" s="29" t="str">
-        <f>Current_Calcs!M3</f>
-        <v/>
-      </c>
-      <c r="N19" s="29" t="str">
-        <f>Current_Calcs!N3</f>
-        <v/>
-      </c>
-      <c r="O19" s="29" t="str">
-        <f>Current_Calcs!O3</f>
-        <v/>
-      </c>
-      <c r="P19" s="29" t="str">
-        <f>Current_Calcs!P3</f>
-        <v/>
-      </c>
-      <c r="Q19" s="29" t="str">
-        <f>Current_Calcs!Q3</f>
-        <v/>
-      </c>
-      <c r="R19" s="29" t="str">
-        <f>Current_Calcs!R3</f>
-        <v/>
+      <c r="D30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -13948,24 +13990,28 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R21"/>
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="B1">
-        <f t="shared" ref="B1:R1" si="0">IF(B$4&lt;&gt;"",COUNTIF(B$5:B$16, "&gt;= 3"),"")</f>
-        <v>1</v>
+        <f t="shared" ref="B1:R1" si="0">IF(B$5&lt;&gt;"",COUNTIF(B$6:B$17, "&gt;= 3"),"")</f>
+        <v>0</v>
       </c>
       <c r="C1">
         <f t="shared" si="0"/>
@@ -14034,10 +14080,10 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:R2" si="1">IF(B$4&lt;&gt;"",COUNTIF(B$5:B$16, "&gt;= 2"),"")</f>
+        <f t="shared" ref="B2:R2" si="1">IF(B$5&lt;&gt;"",COUNTIF(B$6:B$17, "&gt;= 2"),"")</f>
         <v>1</v>
       </c>
       <c r="C2">
@@ -14107,11 +14153,11 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:R3" si="2">IF(B$4&lt;&gt;"",COUNTIF(B$5:B$16, "= 1"),"")</f>
-        <v>1</v>
+        <f t="shared" ref="B3:R3" si="2">IF(B$5&lt;&gt;"",COUNTIF(B$6:B$17, "= 1"),"")</f>
+        <v>0</v>
       </c>
       <c r="C3">
         <f t="shared" si="2"/>
@@ -14178,1048 +14224,1051 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="str">
-        <f>IF('Current Assessment'!B1&lt;&gt;"",'Current Assessment'!B1,"")</f>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:18" s="35" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="36" t="str">
+        <f>IF(Input!B1&lt;&gt;"",Input!B1,"")</f>
         <v>CSS</v>
       </c>
-      <c r="C4" s="9" t="str">
-        <f>IF('Current Assessment'!C1&lt;&gt;"",'Current Assessment'!C1,"")</f>
+      <c r="C5" s="36" t="str">
+        <f>IF(Input!C1&lt;&gt;"",Input!C1,"")</f>
         <v>Javascript</v>
       </c>
-      <c r="D4" s="9" t="str">
-        <f>IF('Current Assessment'!D1&lt;&gt;"",'Current Assessment'!D1,"")</f>
+      <c r="D5" s="36" t="str">
+        <f>IF(Input!D1&lt;&gt;"",Input!D1,"")</f>
         <v>DB Backup/Restore</v>
       </c>
-      <c r="E4" s="9" t="str">
-        <f>IF('Current Assessment'!E1&lt;&gt;"",'Current Assessment'!E1,"")</f>
-        <v/>
-      </c>
-      <c r="F4" s="9" t="str">
-        <f>IF('Current Assessment'!F1&lt;&gt;"",'Current Assessment'!F1,"")</f>
-        <v/>
-      </c>
-      <c r="G4" s="9" t="str">
-        <f>IF('Current Assessment'!G1&lt;&gt;"",'Current Assessment'!G1,"")</f>
-        <v/>
-      </c>
-      <c r="H4" s="9" t="str">
-        <f>IF('Current Assessment'!H1&lt;&gt;"",'Current Assessment'!H1,"")</f>
-        <v/>
-      </c>
-      <c r="I4" s="9" t="str">
-        <f>IF('Current Assessment'!I1&lt;&gt;"",'Current Assessment'!I1,"")</f>
-        <v/>
-      </c>
-      <c r="J4" s="9" t="str">
-        <f>IF('Current Assessment'!J1&lt;&gt;"",'Current Assessment'!J1,"")</f>
-        <v/>
-      </c>
-      <c r="K4" s="9" t="str">
-        <f>IF('Current Assessment'!K1&lt;&gt;"",'Current Assessment'!K1,"")</f>
-        <v/>
-      </c>
-      <c r="L4" s="9" t="str">
-        <f>IF('Current Assessment'!L1&lt;&gt;"",'Current Assessment'!L1,"")</f>
-        <v/>
-      </c>
-      <c r="M4" s="9" t="str">
-        <f>IF('Current Assessment'!M1&lt;&gt;"",'Current Assessment'!M1,"")</f>
-        <v/>
-      </c>
-      <c r="N4" s="9" t="str">
-        <f>IF('Current Assessment'!N1&lt;&gt;"",'Current Assessment'!N1,"")</f>
-        <v/>
-      </c>
-      <c r="O4" s="9" t="str">
-        <f>IF('Current Assessment'!O1&lt;&gt;"",'Current Assessment'!O1,"")</f>
-        <v/>
-      </c>
-      <c r="P4" s="9" t="str">
-        <f>IF('Current Assessment'!P1&lt;&gt;"",'Current Assessment'!P1,"")</f>
-        <v/>
-      </c>
-      <c r="Q4" s="9" t="str">
-        <f>IF('Current Assessment'!Q1&lt;&gt;"",'Current Assessment'!Q1,"")</f>
-        <v/>
-      </c>
-      <c r="R4" s="9" t="str">
-        <f>IF('Current Assessment'!R1&lt;&gt;"",'Current Assessment'!R1,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="str">
-        <f>'Current Assessment'!A2</f>
-        <v>Person 1</v>
-      </c>
-      <c r="B5">
-        <f>IFERROR(MATCH('Current Assessment'!B2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <f>IFERROR(MATCH('Current Assessment'!C2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <f>IFERROR(MATCH('Current Assessment'!D2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <f>IFERROR(MATCH('Current Assessment'!E2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <f>IFERROR(MATCH('Current Assessment'!F2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <f>IFERROR(MATCH('Current Assessment'!G2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <f>IFERROR(MATCH('Current Assessment'!H2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <f>IFERROR(MATCH('Current Assessment'!I2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <f>IFERROR(MATCH('Current Assessment'!J2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <f>IFERROR(MATCH('Current Assessment'!K2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <f>IFERROR(MATCH('Current Assessment'!L2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <f>IFERROR(MATCH('Current Assessment'!M2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <f>IFERROR(MATCH('Current Assessment'!N2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <f>IFERROR(MATCH('Current Assessment'!O2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <f>IFERROR(MATCH('Current Assessment'!P2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <f>IFERROR(MATCH('Current Assessment'!Q2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <f>IFERROR(MATCH('Current Assessment'!R2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
+      <c r="E5" s="36" t="str">
+        <f>IF(Input!E1&lt;&gt;"",Input!E1,"")</f>
+        <v/>
+      </c>
+      <c r="F5" s="36" t="str">
+        <f>IF(Input!F1&lt;&gt;"",Input!F1,"")</f>
+        <v/>
+      </c>
+      <c r="G5" s="36" t="str">
+        <f>IF(Input!G1&lt;&gt;"",Input!G1,"")</f>
+        <v/>
+      </c>
+      <c r="H5" s="36" t="str">
+        <f>IF(Input!H1&lt;&gt;"",Input!H1,"")</f>
+        <v/>
+      </c>
+      <c r="I5" s="36" t="str">
+        <f>IF(Input!I1&lt;&gt;"",Input!I1,"")</f>
+        <v/>
+      </c>
+      <c r="J5" s="36" t="str">
+        <f>IF(Input!J1&lt;&gt;"",Input!J1,"")</f>
+        <v/>
+      </c>
+      <c r="K5" s="36" t="str">
+        <f>IF(Input!K1&lt;&gt;"",Input!K1,"")</f>
+        <v/>
+      </c>
+      <c r="L5" s="36" t="str">
+        <f>IF(Input!L1&lt;&gt;"",Input!L1,"")</f>
+        <v/>
+      </c>
+      <c r="M5" s="36" t="str">
+        <f>IF(Input!M1&lt;&gt;"",Input!M1,"")</f>
+        <v/>
+      </c>
+      <c r="N5" s="36" t="str">
+        <f>IF(Input!N1&lt;&gt;"",Input!N1,"")</f>
+        <v/>
+      </c>
+      <c r="O5" s="36" t="str">
+        <f>IF(Input!O1&lt;&gt;"",Input!O1,"")</f>
+        <v/>
+      </c>
+      <c r="P5" s="36" t="str">
+        <f>IF(Input!P1&lt;&gt;"",Input!P1,"")</f>
+        <v/>
+      </c>
+      <c r="Q5" s="36" t="str">
+        <f>IF(Input!Q1&lt;&gt;"",Input!Q1,"")</f>
+        <v/>
+      </c>
+      <c r="R5" s="36" t="str">
+        <f>IF(Input!R1&lt;&gt;"",Input!R1,"")</f>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="str">
-        <f>'Current Assessment'!A3</f>
-        <v>Person 2</v>
+        <f>Input!A2</f>
+        <v>Person 1</v>
       </c>
       <c r="B6">
-        <f>IFERROR(MATCH('Current Assessment'!B3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!B2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="C6">
-        <f>IFERROR(MATCH('Current Assessment'!C3,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>3</v>
+        <f>IFERROR(MATCH(Input!C2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
       </c>
       <c r="D6">
-        <f>IFERROR(MATCH('Current Assessment'!D3,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>2</v>
+        <f>IFERROR(MATCH(Input!D2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>1</v>
       </c>
       <c r="E6">
-        <f>IFERROR(MATCH('Current Assessment'!E3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!E2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F6">
-        <f>IFERROR(MATCH('Current Assessment'!F3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!F2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G6">
-        <f>IFERROR(MATCH('Current Assessment'!G3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!G2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H6">
-        <f>IFERROR(MATCH('Current Assessment'!H3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!H2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I6">
-        <f>IFERROR(MATCH('Current Assessment'!I3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!I2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J6">
-        <f>IFERROR(MATCH('Current Assessment'!J3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!J2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K6">
-        <f>IFERROR(MATCH('Current Assessment'!K3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!K2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L6">
-        <f>IFERROR(MATCH('Current Assessment'!L3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!L2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M6">
-        <f>IFERROR(MATCH('Current Assessment'!M3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!M2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N6">
-        <f>IFERROR(MATCH('Current Assessment'!N3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!N2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O6">
-        <f>IFERROR(MATCH('Current Assessment'!O3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!O2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P6">
-        <f>IFERROR(MATCH('Current Assessment'!P3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!P2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q6">
-        <f>IFERROR(MATCH('Current Assessment'!Q3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!Q2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R6">
-        <f>IFERROR(MATCH('Current Assessment'!R3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!R2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="str">
-        <f>'Current Assessment'!A4</f>
-        <v>Team 1</v>
+        <f>Input!A3</f>
+        <v>Person 2</v>
       </c>
       <c r="B7">
-        <f>IFERROR(MATCH('Current Assessment'!B4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!B3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <f>IFERROR(MATCH(Input!C3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>3</v>
       </c>
-      <c r="C7">
-        <f>IFERROR(MATCH('Current Assessment'!C4,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
       <c r="D7">
-        <f>IFERROR(MATCH('Current Assessment'!D4,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>3</v>
+        <f>IFERROR(MATCH(Input!D3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>2</v>
       </c>
       <c r="E7">
-        <f>IFERROR(MATCH('Current Assessment'!E4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!E3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F7">
-        <f>IFERROR(MATCH('Current Assessment'!F4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!F3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G7">
-        <f>IFERROR(MATCH('Current Assessment'!G4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!G3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H7">
-        <f>IFERROR(MATCH('Current Assessment'!H4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!H3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I7">
-        <f>IFERROR(MATCH('Current Assessment'!I4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!I3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J7">
-        <f>IFERROR(MATCH('Current Assessment'!J4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!J3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K7">
-        <f>IFERROR(MATCH('Current Assessment'!K4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!K3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L7">
-        <f>IFERROR(MATCH('Current Assessment'!L4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!L3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M7">
-        <f>IFERROR(MATCH('Current Assessment'!M4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!M3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N7">
-        <f>IFERROR(MATCH('Current Assessment'!N4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!N3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O7">
-        <f>IFERROR(MATCH('Current Assessment'!O4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!O3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P7">
-        <f>IFERROR(MATCH('Current Assessment'!P4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!P3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q7">
-        <f>IFERROR(MATCH('Current Assessment'!Q4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!Q3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R7">
-        <f>IFERROR(MATCH('Current Assessment'!R4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!R3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="str">
-        <f>'Current Assessment'!A5</f>
-        <v/>
+        <f>Input!A4</f>
+        <v>Team 1</v>
       </c>
       <c r="B8">
-        <f>IFERROR(MATCH('Current Assessment'!B5,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
+        <f>IFERROR(MATCH(Input!B4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>2</v>
       </c>
       <c r="C8">
-        <f>IFERROR(MATCH('Current Assessment'!C5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!C4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="D8">
-        <f>IFERROR(MATCH('Current Assessment'!D5,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
+        <f>IFERROR(MATCH(Input!D4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>3</v>
       </c>
       <c r="E8">
-        <f>IFERROR(MATCH('Current Assessment'!E5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!E4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F8">
-        <f>IFERROR(MATCH('Current Assessment'!F5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!F4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G8">
-        <f>IFERROR(MATCH('Current Assessment'!G5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!G4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H8">
-        <f>IFERROR(MATCH('Current Assessment'!H5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!H4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I8">
-        <f>IFERROR(MATCH('Current Assessment'!I5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!I4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J8">
-        <f>IFERROR(MATCH('Current Assessment'!J5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!J4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K8">
-        <f>IFERROR(MATCH('Current Assessment'!K5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!K4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L8">
-        <f>IFERROR(MATCH('Current Assessment'!L5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!L4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M8">
-        <f>IFERROR(MATCH('Current Assessment'!M5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!M4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N8">
-        <f>IFERROR(MATCH('Current Assessment'!N5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!N4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O8">
-        <f>IFERROR(MATCH('Current Assessment'!O5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!O4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P8">
-        <f>IFERROR(MATCH('Current Assessment'!P5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!P4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q8">
-        <f>IFERROR(MATCH('Current Assessment'!Q5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!Q4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R8">
-        <f>IFERROR(MATCH('Current Assessment'!R5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!R4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="str">
-        <f>'Current Assessment'!A6</f>
+        <f>Input!A5</f>
         <v/>
       </c>
       <c r="B9">
-        <f>IFERROR(MATCH('Current Assessment'!B6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!B5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="C9">
-        <f>IFERROR(MATCH('Current Assessment'!C6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!C5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="D9">
-        <f>IFERROR(MATCH('Current Assessment'!D6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!D5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="E9">
-        <f>IFERROR(MATCH('Current Assessment'!E6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!E5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F9">
-        <f>IFERROR(MATCH('Current Assessment'!F6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!F5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G9">
-        <f>IFERROR(MATCH('Current Assessment'!G6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!G5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H9">
-        <f>IFERROR(MATCH('Current Assessment'!H6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!H5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I9">
-        <f>IFERROR(MATCH('Current Assessment'!I6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!I5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J9">
-        <f>IFERROR(MATCH('Current Assessment'!J6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!J5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K9">
-        <f>IFERROR(MATCH('Current Assessment'!K6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!K5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L9">
-        <f>IFERROR(MATCH('Current Assessment'!L6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!L5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M9">
-        <f>IFERROR(MATCH('Current Assessment'!M6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!M5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N9">
-        <f>IFERROR(MATCH('Current Assessment'!N6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!N5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O9">
-        <f>IFERROR(MATCH('Current Assessment'!O6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!O5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P9">
-        <f>IFERROR(MATCH('Current Assessment'!P6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!P5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q9">
-        <f>IFERROR(MATCH('Current Assessment'!Q6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!Q5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R9">
-        <f>IFERROR(MATCH('Current Assessment'!R6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!R5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="str">
-        <f>'Current Assessment'!A7</f>
+        <f>Input!A6</f>
         <v/>
       </c>
       <c r="B10">
-        <f>IFERROR(MATCH('Current Assessment'!B7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!B6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="C10">
-        <f>IFERROR(MATCH('Current Assessment'!C7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!C6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="D10">
-        <f>IFERROR(MATCH('Current Assessment'!D7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!D6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="E10">
-        <f>IFERROR(MATCH('Current Assessment'!E7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!E6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F10">
-        <f>IFERROR(MATCH('Current Assessment'!F7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!F6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G10">
-        <f>IFERROR(MATCH('Current Assessment'!G7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!G6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H10">
-        <f>IFERROR(MATCH('Current Assessment'!H7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!H6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I10">
-        <f>IFERROR(MATCH('Current Assessment'!I7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!I6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J10">
-        <f>IFERROR(MATCH('Current Assessment'!J7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!J6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K10">
-        <f>IFERROR(MATCH('Current Assessment'!K7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!K6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L10">
-        <f>IFERROR(MATCH('Current Assessment'!L7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!L6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M10">
-        <f>IFERROR(MATCH('Current Assessment'!M7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!M6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N10">
-        <f>IFERROR(MATCH('Current Assessment'!N7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!N6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O10">
-        <f>IFERROR(MATCH('Current Assessment'!O7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!O6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P10">
-        <f>IFERROR(MATCH('Current Assessment'!P7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!P6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q10">
-        <f>IFERROR(MATCH('Current Assessment'!Q7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!Q6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R10">
-        <f>IFERROR(MATCH('Current Assessment'!R7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!R6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="str">
-        <f>'Current Assessment'!A8</f>
+        <f>Input!A7</f>
         <v/>
       </c>
       <c r="B11">
-        <f>IFERROR(MATCH('Current Assessment'!B8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!B7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="C11">
-        <f>IFERROR(MATCH('Current Assessment'!C8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!C7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="D11">
-        <f>IFERROR(MATCH('Current Assessment'!D8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!D7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="E11">
-        <f>IFERROR(MATCH('Current Assessment'!E8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!E7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F11">
-        <f>IFERROR(MATCH('Current Assessment'!F8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!F7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G11">
-        <f>IFERROR(MATCH('Current Assessment'!G8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!G7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H11">
-        <f>IFERROR(MATCH('Current Assessment'!H8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!H7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I11">
-        <f>IFERROR(MATCH('Current Assessment'!I8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!I7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J11">
-        <f>IFERROR(MATCH('Current Assessment'!J8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!J7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K11">
-        <f>IFERROR(MATCH('Current Assessment'!K8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!K7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L11">
-        <f>IFERROR(MATCH('Current Assessment'!L8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!L7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M11">
-        <f>IFERROR(MATCH('Current Assessment'!M8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!M7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N11">
-        <f>IFERROR(MATCH('Current Assessment'!N8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!N7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O11">
-        <f>IFERROR(MATCH('Current Assessment'!O8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!O7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P11">
-        <f>IFERROR(MATCH('Current Assessment'!P8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!P7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q11">
-        <f>IFERROR(MATCH('Current Assessment'!Q8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!Q7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R11">
-        <f>IFERROR(MATCH('Current Assessment'!R8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!R7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="str">
-        <f>'Current Assessment'!A9</f>
+        <f>Input!A8</f>
         <v/>
       </c>
       <c r="B12">
-        <f>IFERROR(MATCH('Current Assessment'!B9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!B8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="C12">
-        <f>IFERROR(MATCH('Current Assessment'!C9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!C8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="D12">
-        <f>IFERROR(MATCH('Current Assessment'!D9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!D8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="E12">
-        <f>IFERROR(MATCH('Current Assessment'!E9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!E8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F12">
-        <f>IFERROR(MATCH('Current Assessment'!F9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!F8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G12">
-        <f>IFERROR(MATCH('Current Assessment'!G9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!G8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H12">
-        <f>IFERROR(MATCH('Current Assessment'!H9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!H8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I12">
-        <f>IFERROR(MATCH('Current Assessment'!I9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!I8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J12">
-        <f>IFERROR(MATCH('Current Assessment'!J9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!J8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K12">
-        <f>IFERROR(MATCH('Current Assessment'!K9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!K8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L12">
-        <f>IFERROR(MATCH('Current Assessment'!L9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!L8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M12">
-        <f>IFERROR(MATCH('Current Assessment'!M9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!M8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N12">
-        <f>IFERROR(MATCH('Current Assessment'!N9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!N8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O12">
-        <f>IFERROR(MATCH('Current Assessment'!O9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!O8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P12">
-        <f>IFERROR(MATCH('Current Assessment'!P9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!P8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q12">
-        <f>IFERROR(MATCH('Current Assessment'!Q9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!Q8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R12">
-        <f>IFERROR(MATCH('Current Assessment'!R9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!R8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="str">
-        <f>'Current Assessment'!A10</f>
+        <f>Input!A9</f>
         <v/>
       </c>
       <c r="B13">
-        <f>IFERROR(MATCH('Current Assessment'!B10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!B9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="C13">
-        <f>IFERROR(MATCH('Current Assessment'!C10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!C9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="D13">
-        <f>IFERROR(MATCH('Current Assessment'!D10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!D9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="E13">
-        <f>IFERROR(MATCH('Current Assessment'!E10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!E9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F13">
-        <f>IFERROR(MATCH('Current Assessment'!F10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!F9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G13">
-        <f>IFERROR(MATCH('Current Assessment'!G10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!G9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H13">
-        <f>IFERROR(MATCH('Current Assessment'!H10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!H9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I13">
-        <f>IFERROR(MATCH('Current Assessment'!I10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!I9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J13">
-        <f>IFERROR(MATCH('Current Assessment'!J10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!J9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K13">
-        <f>IFERROR(MATCH('Current Assessment'!K10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!K9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L13">
-        <f>IFERROR(MATCH('Current Assessment'!L10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!L9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M13">
-        <f>IFERROR(MATCH('Current Assessment'!M10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!M9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N13">
-        <f>IFERROR(MATCH('Current Assessment'!N10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!N9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O13">
-        <f>IFERROR(MATCH('Current Assessment'!O10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!O9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P13">
-        <f>IFERROR(MATCH('Current Assessment'!P10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!P9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q13">
-        <f>IFERROR(MATCH('Current Assessment'!Q10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!Q9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R13">
-        <f>IFERROR(MATCH('Current Assessment'!R10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!R9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="str">
-        <f>'Current Assessment'!A11</f>
+        <f>Input!A10</f>
         <v/>
       </c>
       <c r="B14">
-        <f>IFERROR(MATCH('Current Assessment'!B11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!B10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="C14">
-        <f>IFERROR(MATCH('Current Assessment'!C11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!C10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="D14">
-        <f>IFERROR(MATCH('Current Assessment'!D11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!D10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="E14">
-        <f>IFERROR(MATCH('Current Assessment'!E11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!E10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F14">
-        <f>IFERROR(MATCH('Current Assessment'!F11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!F10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G14">
-        <f>IFERROR(MATCH('Current Assessment'!G11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!G10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H14">
-        <f>IFERROR(MATCH('Current Assessment'!H11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!H10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I14">
-        <f>IFERROR(MATCH('Current Assessment'!I11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!I10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J14">
-        <f>IFERROR(MATCH('Current Assessment'!J11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!J10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K14">
-        <f>IFERROR(MATCH('Current Assessment'!K11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!K10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L14">
-        <f>IFERROR(MATCH('Current Assessment'!L11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!L10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M14">
-        <f>IFERROR(MATCH('Current Assessment'!M11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!M10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N14">
-        <f>IFERROR(MATCH('Current Assessment'!N11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!N10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O14">
-        <f>IFERROR(MATCH('Current Assessment'!O11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!O10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P14">
-        <f>IFERROR(MATCH('Current Assessment'!P11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!P10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q14">
-        <f>IFERROR(MATCH('Current Assessment'!Q11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!Q10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R14">
-        <f>IFERROR(MATCH('Current Assessment'!R11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!R10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="str">
-        <f>'Current Assessment'!A12</f>
+        <f>Input!A11</f>
         <v/>
       </c>
       <c r="B15">
-        <f>IFERROR(MATCH('Current Assessment'!B12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!B11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="C15">
-        <f>IFERROR(MATCH('Current Assessment'!C12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!C11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="D15">
-        <f>IFERROR(MATCH('Current Assessment'!D12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!D11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="E15">
-        <f>IFERROR(MATCH('Current Assessment'!E12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!E11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F15">
-        <f>IFERROR(MATCH('Current Assessment'!F12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!F11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G15">
-        <f>IFERROR(MATCH('Current Assessment'!G12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!G11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H15">
-        <f>IFERROR(MATCH('Current Assessment'!H12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!H11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I15">
-        <f>IFERROR(MATCH('Current Assessment'!I12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!I11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J15">
-        <f>IFERROR(MATCH('Current Assessment'!J12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!J11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K15">
-        <f>IFERROR(MATCH('Current Assessment'!K12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!K11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L15">
-        <f>IFERROR(MATCH('Current Assessment'!L12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!L11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M15">
-        <f>IFERROR(MATCH('Current Assessment'!M12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!M11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N15">
-        <f>IFERROR(MATCH('Current Assessment'!N12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!N11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O15">
-        <f>IFERROR(MATCH('Current Assessment'!O12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!O11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P15">
-        <f>IFERROR(MATCH('Current Assessment'!P12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!P11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q15">
-        <f>IFERROR(MATCH('Current Assessment'!Q12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!Q11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R15">
-        <f>IFERROR(MATCH('Current Assessment'!R12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!R11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="str">
-        <f>'Current Assessment'!A13</f>
+        <f>Input!A12</f>
         <v/>
       </c>
       <c r="B16">
-        <f>IFERROR(MATCH('Current Assessment'!B13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!B12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="C16">
-        <f>IFERROR(MATCH('Current Assessment'!C13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!C12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="D16">
-        <f>IFERROR(MATCH('Current Assessment'!D13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!D12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="E16">
-        <f>IFERROR(MATCH('Current Assessment'!E13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!E12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F16">
-        <f>IFERROR(MATCH('Current Assessment'!F13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!F12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G16">
-        <f>IFERROR(MATCH('Current Assessment'!G13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!G12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H16">
-        <f>IFERROR(MATCH('Current Assessment'!H13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!H12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I16">
-        <f>IFERROR(MATCH('Current Assessment'!I13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!I12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J16">
-        <f>IFERROR(MATCH('Current Assessment'!J13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!J12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K16">
-        <f>IFERROR(MATCH('Current Assessment'!K13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!K12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L16">
-        <f>IFERROR(MATCH('Current Assessment'!L13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!L12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M16">
-        <f>IFERROR(MATCH('Current Assessment'!M13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!M12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N16">
-        <f>IFERROR(MATCH('Current Assessment'!N13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!N12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O16">
-        <f>IFERROR(MATCH('Current Assessment'!O13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!O12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P16">
-        <f>IFERROR(MATCH('Current Assessment'!P13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!P12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q16">
-        <f>IFERROR(MATCH('Current Assessment'!Q13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!Q12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R16">
-        <f>IFERROR(MATCH('Current Assessment'!R13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!R12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="6">
-        <f t="shared" ref="B17:R17" si="3">SUM(B5:B16)</f>
-        <v>4</v>
-      </c>
-      <c r="C17" s="6">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="str">
+        <f>Input!A13</f>
+        <v/>
+      </c>
+      <c r="B17">
+        <f>IFERROR(MATCH(Input!B13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <f>IFERROR(MATCH(Input!C13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <f>IFERROR(MATCH(Input!D13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f>IFERROR(MATCH(Input!E13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <f>IFERROR(MATCH(Input!F13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <f>IFERROR(MATCH(Input!G13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <f>IFERROR(MATCH(Input!H13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f>IFERROR(MATCH(Input!I13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <f>IFERROR(MATCH(Input!J13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <f>IFERROR(MATCH(Input!K13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f>IFERROR(MATCH(Input!L13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <f>IFERROR(MATCH(Input!M13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <f>IFERROR(MATCH(Input!N13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <f>IFERROR(MATCH(Input!O13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <f>IFERROR(MATCH(Input!P13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <f>IFERROR(MATCH(Input!Q13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <f>IFERROR(MATCH(Input!R13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="6">
+        <f t="shared" ref="B18:R18" si="3">SUM(B6:B17)</f>
+        <v>2</v>
+      </c>
+      <c r="C18" s="6">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D18" s="6">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E18" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F18" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G18" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H18" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I18" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J17" s="6">
+      <c r="J18" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K17" s="6">
+      <c r="K18" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L17" s="6">
+      <c r="L18" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M17" s="6">
+      <c r="M18" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N17" s="6">
+      <c r="N18" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O17" s="6">
+      <c r="O18" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P17" s="6">
+      <c r="P18" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Q17" s="6">
+      <c r="Q18" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R17" s="6">
+      <c r="R18" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>27</v>
+    <row r="19" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>27</v>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B17:R17">
-    <cfRule type="colorScale" priority="6">
+  <conditionalFormatting sqref="B18:R18">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -15227,9 +15276,19 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5:R16">
-    <cfRule type="colorScale" priority="8">
+  <conditionalFormatting sqref="B6:R17">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -15239,12 +15298,11 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="7" id="{339E999E-0713-46E1-92D7-78E999ECB110}">
+          <x14:cfRule type="iconSet" priority="8" id="{339E999E-0713-46E1-92D7-78E999ECB110}">
             <x14:iconSet iconSet="4TrafficLights" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -15264,7 +15322,7 @@
               <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>B1:R3</xm:sqref>
+          <xm:sqref>B1:R4</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -15274,6 +15332,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet6"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:U27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15288,99 +15360,99 @@
     <row r="1" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13"/>
       <c r="B1" s="13" t="str">
-        <f>IF('Current Assessment'!B1&lt;&gt;"",'Current Assessment'!B1,"")</f>
+        <f>IF(Input!B1&lt;&gt;"",Input!B1,"")</f>
         <v>CSS</v>
       </c>
       <c r="C1" s="13" t="str">
-        <f>IF('Current Assessment'!C1&lt;&gt;"",'Current Assessment'!C1,"")</f>
+        <f>IF(Input!C1&lt;&gt;"",Input!C1,"")</f>
         <v>Javascript</v>
       </c>
       <c r="D1" s="13" t="str">
-        <f>IF('Current Assessment'!D1&lt;&gt;"",'Current Assessment'!D1,"")</f>
+        <f>IF(Input!D1&lt;&gt;"",Input!D1,"")</f>
         <v>DB Backup/Restore</v>
       </c>
       <c r="E1" s="13" t="str">
-        <f>IF('Current Assessment'!E1&lt;&gt;"",'Current Assessment'!E1,"")</f>
+        <f>IF(Input!E1&lt;&gt;"",Input!E1,"")</f>
         <v/>
       </c>
       <c r="F1" s="13" t="str">
-        <f>IF('Current Assessment'!F1&lt;&gt;"",'Current Assessment'!F1,"")</f>
+        <f>IF(Input!F1&lt;&gt;"",Input!F1,"")</f>
         <v/>
       </c>
       <c r="G1" s="13" t="str">
-        <f>IF('Current Assessment'!G1&lt;&gt;"",'Current Assessment'!G1,"")</f>
+        <f>IF(Input!G1&lt;&gt;"",Input!G1,"")</f>
         <v/>
       </c>
       <c r="H1" s="13" t="str">
-        <f>IF('Current Assessment'!H1&lt;&gt;"",'Current Assessment'!H1,"")</f>
+        <f>IF(Input!H1&lt;&gt;"",Input!H1,"")</f>
         <v/>
       </c>
       <c r="I1" s="13" t="str">
-        <f>IF('Current Assessment'!I1&lt;&gt;"",'Current Assessment'!I1,"")</f>
+        <f>IF(Input!I1&lt;&gt;"",Input!I1,"")</f>
         <v/>
       </c>
       <c r="J1" s="13" t="str">
-        <f>IF('Current Assessment'!J1&lt;&gt;"",'Current Assessment'!J1,"")</f>
+        <f>IF(Input!J1&lt;&gt;"",Input!J1,"")</f>
         <v/>
       </c>
       <c r="K1" s="13" t="str">
-        <f>IF('Current Assessment'!K1&lt;&gt;"",'Current Assessment'!K1,"")</f>
+        <f>IF(Input!K1&lt;&gt;"",Input!K1,"")</f>
         <v/>
       </c>
       <c r="L1" s="13" t="str">
-        <f>IF('Current Assessment'!L1&lt;&gt;"",'Current Assessment'!L1,"")</f>
+        <f>IF(Input!L1&lt;&gt;"",Input!L1,"")</f>
         <v/>
       </c>
       <c r="M1" s="13" t="str">
-        <f>IF('Current Assessment'!M1&lt;&gt;"",'Current Assessment'!M1,"")</f>
+        <f>IF(Input!M1&lt;&gt;"",Input!M1,"")</f>
         <v/>
       </c>
       <c r="N1" s="13" t="str">
-        <f>IF('Current Assessment'!N1&lt;&gt;"",'Current Assessment'!N1,"")</f>
+        <f>IF(Input!N1&lt;&gt;"",Input!N1,"")</f>
         <v/>
       </c>
       <c r="O1" s="13" t="str">
-        <f>IF('Current Assessment'!O1&lt;&gt;"",'Current Assessment'!O1,"")</f>
+        <f>IF(Input!O1&lt;&gt;"",Input!O1,"")</f>
         <v/>
       </c>
       <c r="P1" s="13" t="str">
-        <f>IF('Current Assessment'!P1&lt;&gt;"",'Current Assessment'!P1,"")</f>
+        <f>IF(Input!P1&lt;&gt;"",Input!P1,"")</f>
         <v/>
       </c>
       <c r="Q1" s="13" t="str">
-        <f>IF('Current Assessment'!Q1&lt;&gt;"",'Current Assessment'!Q1,"")</f>
+        <f>IF(Input!Q1&lt;&gt;"",Input!Q1,"")</f>
         <v/>
       </c>
       <c r="R1" s="13" t="str">
-        <f>IF('Current Assessment'!R1&lt;&gt;"",'Current Assessment'!R1,"")</f>
+        <f>IF(Input!R1&lt;&gt;"",Input!R1,"")</f>
         <v/>
       </c>
       <c r="S1" s="13" t="e">
-        <f>IF('Current Assessment'!#REF!&lt;&gt;"",'Current Assessment'!#REF!,"")</f>
+        <f>IF(Input!#REF!&lt;&gt;"",Input!#REF!,"")</f>
         <v>#REF!</v>
       </c>
       <c r="T1" s="13" t="e">
-        <f>IF('Current Assessment'!#REF!&lt;&gt;"",'Current Assessment'!#REF!,"")</f>
+        <f>IF(Input!#REF!&lt;&gt;"",Input!#REF!,"")</f>
         <v>#REF!</v>
       </c>
       <c r="U1" s="13" t="e">
-        <f>IF('Current Assessment'!#REF!&lt;&gt;"",'Current Assessment'!#REF!,"")</f>
+        <f>IF(Input!#REF!&lt;&gt;"",Input!#REF!,"")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="str">
-        <f>IF('Current Assessment'!A2&lt;&gt;"", 'Current Assessment'!A2, "")</f>
+        <f>IF(Input!A2&lt;&gt;"", Input!A2, "")</f>
         <v>Person 1</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
@@ -15402,7 +15474,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="str">
-        <f>IF('Current Assessment'!A3&lt;&gt;"", 'Current Assessment'!A3, "")</f>
+        <f>IF(Input!A3&lt;&gt;"", Input!A3, "")</f>
         <v>Person 2</v>
       </c>
       <c r="B3" s="12"/>
@@ -15430,7 +15502,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="str">
-        <f>IF('Current Assessment'!A4&lt;&gt;"", 'Current Assessment'!A4, "")</f>
+        <f>IF(Input!A4&lt;&gt;"", Input!A4, "")</f>
         <v>Team 1</v>
       </c>
       <c r="B4" s="12"/>
@@ -15456,7 +15528,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="str">
-        <f>IF('Current Assessment'!A5&lt;&gt;"", 'Current Assessment'!A5, "")</f>
+        <f>IF(Input!A5&lt;&gt;"", Input!A5, "")</f>
         <v/>
       </c>
       <c r="B5" s="12"/>
@@ -15482,7 +15554,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="str">
-        <f>IF('Current Assessment'!A6&lt;&gt;"", 'Current Assessment'!A6, "")</f>
+        <f>IF(Input!A6&lt;&gt;"", Input!A6, "")</f>
         <v/>
       </c>
       <c r="B6" s="12"/>
@@ -15508,7 +15580,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="str">
-        <f>IF('Current Assessment'!A7&lt;&gt;"", 'Current Assessment'!A7, "")</f>
+        <f>IF(Input!A7&lt;&gt;"", Input!A7, "")</f>
         <v/>
       </c>
       <c r="B7" s="12"/>
@@ -15534,7 +15606,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="str">
-        <f>IF('Current Assessment'!A8&lt;&gt;"", 'Current Assessment'!A8, "")</f>
+        <f>IF(Input!A8&lt;&gt;"", Input!A8, "")</f>
         <v/>
       </c>
       <c r="B8" s="12"/>
@@ -15560,7 +15632,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="str">
-        <f>IF('Current Assessment'!A9&lt;&gt;"", 'Current Assessment'!A9, "")</f>
+        <f>IF(Input!A9&lt;&gt;"", Input!A9, "")</f>
         <v/>
       </c>
       <c r="B9" s="12"/>
@@ -15586,7 +15658,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="str">
-        <f>IF('Current Assessment'!A10&lt;&gt;"", 'Current Assessment'!A10, "")</f>
+        <f>IF(Input!A10&lt;&gt;"", Input!A10, "")</f>
         <v/>
       </c>
       <c r="B10" s="12"/>
@@ -15612,7 +15684,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="str">
-        <f>IF('Current Assessment'!A11&lt;&gt;"", 'Current Assessment'!A11, "")</f>
+        <f>IF(Input!A11&lt;&gt;"", Input!A11, "")</f>
         <v/>
       </c>
       <c r="B11" s="12"/>
@@ -15638,7 +15710,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="str">
-        <f>IF('Current Assessment'!A12&lt;&gt;"", 'Current Assessment'!A12, "")</f>
+        <f>IF(Input!A12&lt;&gt;"", Input!A12, "")</f>
         <v/>
       </c>
       <c r="B12" s="12"/>
@@ -15664,7 +15736,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="str">
-        <f>IF('Current Assessment'!A13&lt;&gt;"", 'Current Assessment'!A13, "")</f>
+        <f>IF(Input!A13&lt;&gt;"", Input!A13, "")</f>
         <v/>
       </c>
       <c r="B13" s="12"/>
@@ -15690,7 +15762,7 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="e">
-        <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
+        <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
         <v>#REF!</v>
       </c>
       <c r="B14" s="12"/>
@@ -15716,7 +15788,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="e">
-        <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
+        <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
         <v>#REF!</v>
       </c>
       <c r="B15" s="12"/>
@@ -15742,7 +15814,7 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="e">
-        <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
+        <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
         <v>#REF!</v>
       </c>
       <c r="B16" s="12"/>
@@ -15768,7 +15840,7 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="e">
-        <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
+        <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
         <v>#REF!</v>
       </c>
       <c r="B17" s="12"/>
@@ -15794,7 +15866,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="e">
-        <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
+        <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
         <v>#REF!</v>
       </c>
       <c r="B18" s="12"/>
@@ -15820,7 +15892,7 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="e">
-        <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
+        <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
         <v>#REF!</v>
       </c>
       <c r="B19" s="12"/>
@@ -15846,7 +15918,7 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="e">
-        <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
+        <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
         <v>#REF!</v>
       </c>
       <c r="B20" s="12"/>
@@ -15872,7 +15944,7 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="e">
-        <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
+        <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
         <v>#REF!</v>
       </c>
       <c r="B21" s="12"/>
@@ -15898,7 +15970,7 @@
     </row>
     <row r="23" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -16071,7 +16143,7 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B26" s="7">
         <f>Willingness_Calcs!B2</f>
@@ -16156,7 +16228,7 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B27" s="7">
         <f>Willingness_Calcs!B3</f>
@@ -16284,8 +16356,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16302,7 +16375,7 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B1">
         <f>IF(B$4&lt;&gt;"",COUNTIF(B$5:B$24, "&gt;= 3"),"")</f>
@@ -16387,7 +16460,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <f>IF(B$4&lt;&gt;"",COUNTIF(B$5:B$24, "&gt;= 2"),"")</f>
@@ -16472,7 +16545,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <f>IF(B$4&lt;&gt;"",COUNTIF(B$5:B$24, "= 1"),"")</f>
@@ -16557,89 +16630,89 @@
     </row>
     <row r="4" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="str">
-        <f>IF('Current Assessment'!B1&lt;&gt;"",'Current Assessment'!B1,"")</f>
+        <f>IF(Input!B1&lt;&gt;"",Input!B1,"")</f>
         <v>CSS</v>
       </c>
       <c r="C4" s="9" t="str">
-        <f>IF('Current Assessment'!C1&lt;&gt;"",'Current Assessment'!C1,"")</f>
+        <f>IF(Input!C1&lt;&gt;"",Input!C1,"")</f>
         <v>Javascript</v>
       </c>
       <c r="D4" s="9" t="str">
-        <f>IF('Current Assessment'!D1&lt;&gt;"",'Current Assessment'!D1,"")</f>
+        <f>IF(Input!D1&lt;&gt;"",Input!D1,"")</f>
         <v>DB Backup/Restore</v>
       </c>
       <c r="E4" s="9" t="str">
-        <f>IF('Current Assessment'!E1&lt;&gt;"",'Current Assessment'!E1,"")</f>
+        <f>IF(Input!E1&lt;&gt;"",Input!E1,"")</f>
         <v/>
       </c>
       <c r="F4" s="9" t="str">
-        <f>IF('Current Assessment'!F1&lt;&gt;"",'Current Assessment'!F1,"")</f>
+        <f>IF(Input!F1&lt;&gt;"",Input!F1,"")</f>
         <v/>
       </c>
       <c r="G4" s="9" t="str">
-        <f>IF('Current Assessment'!G1&lt;&gt;"",'Current Assessment'!G1,"")</f>
+        <f>IF(Input!G1&lt;&gt;"",Input!G1,"")</f>
         <v/>
       </c>
       <c r="H4" s="9" t="str">
-        <f>IF('Current Assessment'!H1&lt;&gt;"",'Current Assessment'!H1,"")</f>
+        <f>IF(Input!H1&lt;&gt;"",Input!H1,"")</f>
         <v/>
       </c>
       <c r="I4" s="9" t="str">
-        <f>IF('Current Assessment'!I1&lt;&gt;"",'Current Assessment'!I1,"")</f>
+        <f>IF(Input!I1&lt;&gt;"",Input!I1,"")</f>
         <v/>
       </c>
       <c r="J4" s="9" t="str">
-        <f>IF('Current Assessment'!J1&lt;&gt;"",'Current Assessment'!J1,"")</f>
+        <f>IF(Input!J1&lt;&gt;"",Input!J1,"")</f>
         <v/>
       </c>
       <c r="K4" s="9" t="str">
-        <f>IF('Current Assessment'!K1&lt;&gt;"",'Current Assessment'!K1,"")</f>
+        <f>IF(Input!K1&lt;&gt;"",Input!K1,"")</f>
         <v/>
       </c>
       <c r="L4" s="9" t="str">
-        <f>IF('Current Assessment'!L1&lt;&gt;"",'Current Assessment'!L1,"")</f>
+        <f>IF(Input!L1&lt;&gt;"",Input!L1,"")</f>
         <v/>
       </c>
       <c r="M4" s="9" t="str">
-        <f>IF('Current Assessment'!M1&lt;&gt;"",'Current Assessment'!M1,"")</f>
+        <f>IF(Input!M1&lt;&gt;"",Input!M1,"")</f>
         <v/>
       </c>
       <c r="N4" s="9" t="str">
-        <f>IF('Current Assessment'!N1&lt;&gt;"",'Current Assessment'!N1,"")</f>
+        <f>IF(Input!N1&lt;&gt;"",Input!N1,"")</f>
         <v/>
       </c>
       <c r="O4" s="9" t="str">
-        <f>IF('Current Assessment'!O1&lt;&gt;"",'Current Assessment'!O1,"")</f>
+        <f>IF(Input!O1&lt;&gt;"",Input!O1,"")</f>
         <v/>
       </c>
       <c r="P4" s="9" t="str">
-        <f>IF('Current Assessment'!P1&lt;&gt;"",'Current Assessment'!P1,"")</f>
+        <f>IF(Input!P1&lt;&gt;"",Input!P1,"")</f>
         <v/>
       </c>
       <c r="Q4" s="9" t="str">
-        <f>IF('Current Assessment'!Q1&lt;&gt;"",'Current Assessment'!Q1,"")</f>
+        <f>IF(Input!Q1&lt;&gt;"",Input!Q1,"")</f>
         <v/>
       </c>
       <c r="R4" s="9" t="str">
-        <f>IF('Current Assessment'!R1&lt;&gt;"",'Current Assessment'!R1,"")</f>
+        <f>IF(Input!R1&lt;&gt;"",Input!R1,"")</f>
         <v/>
       </c>
       <c r="S4" s="9" t="e">
-        <f>IF('Current Assessment'!#REF!&lt;&gt;"",'Current Assessment'!#REF!,"")</f>
+        <f>IF(Input!#REF!&lt;&gt;"",Input!#REF!,"")</f>
         <v>#REF!</v>
       </c>
       <c r="T4" s="9" t="e">
-        <f>IF('Current Assessment'!#REF!&lt;&gt;"",'Current Assessment'!#REF!,"")</f>
+        <f>IF(Input!#REF!&lt;&gt;"",Input!#REF!,"")</f>
         <v>#REF!</v>
       </c>
       <c r="U4" s="9" t="e">
-        <f>IF('Current Assessment'!#REF!&lt;&gt;"",'Current Assessment'!#REF!,"")</f>
+        <f>IF(Input!#REF!&lt;&gt;"",Input!#REF!,"")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="str">
-        <f>'Current Assessment'!A2</f>
+        <f>Input!A2</f>
         <v>Person 1</v>
       </c>
       <c r="B5">
@@ -16725,7 +16798,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="str">
-        <f>'Current Assessment'!A3</f>
+        <f>Input!A3</f>
         <v>Person 2</v>
       </c>
       <c r="B6">
@@ -16811,7 +16884,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="str">
-        <f>'Current Assessment'!A4</f>
+        <f>Input!A4</f>
         <v>Team 1</v>
       </c>
       <c r="B7">
@@ -16897,7 +16970,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="str">
-        <f>'Current Assessment'!A5</f>
+        <f>Input!A5</f>
         <v/>
       </c>
       <c r="B8">
@@ -16983,7 +17056,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="str">
-        <f>'Current Assessment'!A6</f>
+        <f>Input!A6</f>
         <v/>
       </c>
       <c r="B9">
@@ -17069,7 +17142,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="str">
-        <f>'Current Assessment'!A7</f>
+        <f>Input!A7</f>
         <v/>
       </c>
       <c r="B10">
@@ -17155,7 +17228,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="str">
-        <f>'Current Assessment'!A8</f>
+        <f>Input!A8</f>
         <v/>
       </c>
       <c r="B11">
@@ -17241,7 +17314,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="str">
-        <f>'Current Assessment'!A9</f>
+        <f>Input!A9</f>
         <v/>
       </c>
       <c r="B12">
@@ -17327,7 +17400,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="str">
-        <f>'Current Assessment'!A10</f>
+        <f>Input!A10</f>
         <v/>
       </c>
       <c r="B13">
@@ -17413,7 +17486,7 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="str">
-        <f>'Current Assessment'!A11</f>
+        <f>Input!A11</f>
         <v/>
       </c>
       <c r="B14">
@@ -17499,7 +17572,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="str">
-        <f>'Current Assessment'!A12</f>
+        <f>Input!A12</f>
         <v/>
       </c>
       <c r="B15">
@@ -17585,7 +17658,7 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="str">
-        <f>'Current Assessment'!A13</f>
+        <f>Input!A13</f>
         <v/>
       </c>
       <c r="B16">
@@ -17671,7 +17744,7 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="e">
-        <f>'Current Assessment'!#REF!</f>
+        <f>Input!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B17">
@@ -17757,7 +17830,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="e">
-        <f>'Current Assessment'!#REF!</f>
+        <f>Input!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B18">
@@ -17843,7 +17916,7 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="e">
-        <f>'Current Assessment'!#REF!</f>
+        <f>Input!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B19">
@@ -17929,7 +18002,7 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="e">
-        <f>'Current Assessment'!#REF!</f>
+        <f>Input!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B20">
@@ -18015,7 +18088,7 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="e">
-        <f>'Current Assessment'!#REF!</f>
+        <f>Input!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B21">
@@ -18101,7 +18174,7 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="e">
-        <f>'Current Assessment'!#REF!</f>
+        <f>Input!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B22">
@@ -18187,7 +18260,7 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="e">
-        <f>'Current Assessment'!#REF!</f>
+        <f>Input!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B23">
@@ -18273,7 +18346,7 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="e">
-        <f>'Current Assessment'!#REF!</f>
+        <f>Input!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B24">

</xml_diff>

<commit_message>
Revert "Expanded version supporting 5000 samples rather than 1250"
This reverts commit 6cc5b62711c2ac8b18050b702dc3f5fbe0a9c671.
</commit_message>
<xml_diff>
--- a/Spreadsheets/Capability Matrix.xlsx
+++ b/Spreadsheets/Capability Matrix.xlsx
@@ -1,36 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Private\GitHub\FocusedObjective.Resources\Spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Troy\Dropbox\Private\GitHub\FocusedObjective.Resources\Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="90" yWindow="765" windowWidth="19140" windowHeight="9525" activeTab="3"/>
+    <workbookView xWindow="90" yWindow="75" windowWidth="19140" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="6" r:id="rId1"/>
     <sheet name="Settings" sheetId="2" r:id="rId2"/>
     <sheet name="Survey Sheet" sheetId="5" r:id="rId3"/>
-    <sheet name="Input" sheetId="1" r:id="rId4"/>
-    <sheet name="Heatmap" sheetId="4" r:id="rId5"/>
-    <sheet name="Splitability" sheetId="8" r:id="rId6"/>
-    <sheet name="Willingness" sheetId="3" state="hidden" r:id="rId7"/>
-    <sheet name="Willingness_Calcs" sheetId="7" state="hidden" r:id="rId8"/>
+    <sheet name="Current Assessment" sheetId="1" r:id="rId4"/>
+    <sheet name="Current_Calcs" sheetId="4" state="hidden" r:id="rId5"/>
+    <sheet name="Willingness" sheetId="3" state="hidden" r:id="rId6"/>
+    <sheet name="Willingness_Calcs" sheetId="7" state="hidden" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="Skills_Header" localSheetId="7">Settings!#REF!</definedName>
+    <definedName name="Skills_Header" localSheetId="6">Settings!#REF!</definedName>
     <definedName name="Skills_Header">Settings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t>Willing</t>
   </si>
@@ -50,10 +49,19 @@
     <t>Person 1</t>
   </si>
   <si>
+    <t>Captains: Ability to Create (# &gt;= 3)</t>
+  </si>
+  <si>
+    <t>Players: Ability to Maintain (# &gt;= 2)</t>
+  </si>
+  <si>
     <t>Your Name:</t>
   </si>
   <si>
     <t>Analysis:</t>
+  </si>
+  <si>
+    <t>Bench: Ready to Train Up (# = 1)</t>
   </si>
   <si>
     <t>I'd quit rather than do this…</t>
@@ -93,6 +101,9 @@
   </si>
   <si>
     <t>Can start from nothing and create</t>
+  </si>
+  <si>
+    <t>Expert level</t>
   </si>
   <si>
     <t>For each capability choose from the list of CURRENT skill level values. If in doubt, err low (left)!</t>
@@ -137,58 +148,19 @@
     <t>Initial Version</t>
   </si>
   <si>
+    <t>Made all setting in the Setting tab.</t>
+  </si>
+  <si>
     <t>Staff and Team Capability Matrix</t>
   </si>
   <si>
     <t>Capability Survey For Printing (enter skills in the Settings worksheet)</t>
   </si>
-  <si>
-    <t>Quick Analysis:</t>
-  </si>
-  <si>
-    <t>Can teach others</t>
-  </si>
-  <si>
-    <t>Made all settings definable in the Setting tab.</t>
-  </si>
-  <si>
-    <t>no teacher</t>
-  </si>
-  <si>
-    <t>1 teacher</t>
-  </si>
-  <si>
-    <t>no doer</t>
-  </si>
-  <si>
-    <t>1 doer</t>
-  </si>
-  <si>
-    <t>no novice</t>
-  </si>
-  <si>
-    <t>1 novice</t>
-  </si>
-  <si>
-    <t>no doer. 1 Novice</t>
-  </si>
-  <si>
-    <t>teach novice into doer - URGENT</t>
-  </si>
-  <si>
-    <t>1 doer, 1 novice</t>
-  </si>
-  <si>
-    <t>teach novice into doer - SOON</t>
-  </si>
-  <si>
-    <t>hire teacher level or  external consultant. Create doers, then train one into teacher</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -315,7 +287,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -406,17 +378,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -427,7 +388,7 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -481,8 +442,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -11909,7 +11868,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>Novice &amp; Learner (bench)</a:t>
+            <a:t>Novice &amp; LEarner (bench)</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
@@ -12016,6 +11975,75 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
+      <xdr:colOff>527685</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>32385</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>59055</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4013835" y="1556385"/>
+          <a:ext cx="6846570" cy="1386840"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="1"/>
+            <a:t>Do not edit this sheet directly. This is the formulas for converting and counting current capability. If you want to add people, do it in the current tab. </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>1150620</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
@@ -12088,7 +12116,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -12444,35 +12472,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:Q23"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
+      <c r="B1" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
     </row>
     <row r="2" spans="2:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="P2" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
@@ -12480,7 +12507,7 @@
         <v>1</v>
       </c>
       <c r="Q4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
@@ -12556,11 +12583,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet3"/>
   <dimension ref="B5:K22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12580,18 +12606,18 @@
   <sheetData>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="K5" s="2"/>
     </row>
@@ -12603,45 +12629,45 @@
         <v>3</v>
       </c>
       <c r="G6" s="25" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I6" s="25" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D7" s="25" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="25" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I7" s="25" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I8" s="25" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="26"/>
       <c r="D9" s="25"/>
       <c r="G9" s="25" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I9" s="25" t="s">
         <v>1</v>
@@ -12651,7 +12677,7 @@
       <c r="B10" s="26"/>
       <c r="D10" s="25"/>
       <c r="G10" s="25" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="I10" s="25" t="s">
         <v>2</v>
@@ -12709,11 +12735,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12727,31 +12752,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="A1" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
     </row>
     <row r="2" spans="1:6" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="20" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -12776,12 +12801,12 @@
       </c>
       <c r="F7" s="23" t="str">
         <f>Settings!$G$10</f>
-        <v>Can teach others</v>
+        <v>Expert level</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="str">
-        <f>IF(Input!B1&lt;&gt;"", Input!B1, "")</f>
+        <f>IF('Current Assessment'!B1&lt;&gt;"", 'Current Assessment'!B1, "")</f>
         <v>CSS</v>
       </c>
       <c r="B8" s="17"/>
@@ -12792,7 +12817,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="str">
-        <f>IF(Input!C1&lt;&gt;"", Input!C1, "")</f>
+        <f>IF('Current Assessment'!C1&lt;&gt;"", 'Current Assessment'!C1, "")</f>
         <v>Javascript</v>
       </c>
       <c r="B9" s="17"/>
@@ -12803,7 +12828,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="str">
-        <f>IF(Input!D1&lt;&gt;"", Input!D1, "")</f>
+        <f>IF('Current Assessment'!D1&lt;&gt;"", 'Current Assessment'!D1, "")</f>
         <v>DB Backup/Restore</v>
       </c>
       <c r="B10" s="17"/>
@@ -12814,7 +12839,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="str">
-        <f>IF(Input!E1&lt;&gt;"", Input!E1, "")</f>
+        <f>IF('Current Assessment'!E1&lt;&gt;"", 'Current Assessment'!E1, "")</f>
         <v/>
       </c>
       <c r="B11" s="17"/>
@@ -12825,7 +12850,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="str">
-        <f>IF(Input!F1&lt;&gt;"", Input!F1, "")</f>
+        <f>IF('Current Assessment'!F1&lt;&gt;"", 'Current Assessment'!F1, "")</f>
         <v/>
       </c>
       <c r="B12" s="17"/>
@@ -12836,7 +12861,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="str">
-        <f>IF(Input!G1&lt;&gt;"", Input!G1, "")</f>
+        <f>IF('Current Assessment'!G1&lt;&gt;"", 'Current Assessment'!G1, "")</f>
         <v/>
       </c>
       <c r="B13" s="17"/>
@@ -12847,7 +12872,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="str">
-        <f>IF(Input!H1&lt;&gt;"", Input!H1, "")</f>
+        <f>IF('Current Assessment'!H1&lt;&gt;"", 'Current Assessment'!H1, "")</f>
         <v/>
       </c>
       <c r="B14" s="17"/>
@@ -12858,7 +12883,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="str">
-        <f>IF(Input!I1&lt;&gt;"", Input!I1, "")</f>
+        <f>IF('Current Assessment'!I1&lt;&gt;"", 'Current Assessment'!I1, "")</f>
         <v/>
       </c>
       <c r="B15" s="17"/>
@@ -12869,7 +12894,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="str">
-        <f>IF(Input!J1&lt;&gt;"", Input!J1, "")</f>
+        <f>IF('Current Assessment'!J1&lt;&gt;"", 'Current Assessment'!J1, "")</f>
         <v/>
       </c>
       <c r="B16" s="17"/>
@@ -12880,7 +12905,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="str">
-        <f>IF(Input!K1&lt;&gt;"", Input!K1, "")</f>
+        <f>IF('Current Assessment'!K1&lt;&gt;"", 'Current Assessment'!K1, "")</f>
         <v/>
       </c>
       <c r="B17" s="17"/>
@@ -12891,7 +12916,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="str">
-        <f>IF(Input!L1&lt;&gt;"", Input!L1, "")</f>
+        <f>IF('Current Assessment'!L1&lt;&gt;"", 'Current Assessment'!L1, "")</f>
         <v/>
       </c>
       <c r="B18" s="17"/>
@@ -12902,7 +12927,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="str">
-        <f>IF(Input!M1&lt;&gt;"", Input!M1, "")</f>
+        <f>IF('Current Assessment'!M1&lt;&gt;"", 'Current Assessment'!M1, "")</f>
         <v/>
       </c>
       <c r="B19" s="17"/>
@@ -12913,7 +12938,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="str">
-        <f>IF(Input!N1&lt;&gt;"", Input!N1, "")</f>
+        <f>IF('Current Assessment'!N1&lt;&gt;"", 'Current Assessment'!N1, "")</f>
         <v/>
       </c>
       <c r="B20" s="17"/>
@@ -12924,7 +12949,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="str">
-        <f>IF(Input!O1&lt;&gt;"", Input!O1, "")</f>
+        <f>IF('Current Assessment'!O1&lt;&gt;"", 'Current Assessment'!O1, "")</f>
         <v/>
       </c>
       <c r="B21" s="17"/>
@@ -12935,7 +12960,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="str">
-        <f>IF(Input!P1&lt;&gt;"", Input!P1, "")</f>
+        <f>IF('Current Assessment'!P1&lt;&gt;"", 'Current Assessment'!P1, "")</f>
         <v/>
       </c>
       <c r="B22" s="17"/>
@@ -12946,7 +12971,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="str">
-        <f>IF(Input!Q1&lt;&gt;"", Input!Q1, "")</f>
+        <f>IF('Current Assessment'!Q1&lt;&gt;"", 'Current Assessment'!Q1, "")</f>
         <v/>
       </c>
       <c r="B23" s="17"/>
@@ -12957,7 +12982,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="str">
-        <f>IF(Input!R1&lt;&gt;"", Input!R1, "")</f>
+        <f>IF('Current Assessment'!R1&lt;&gt;"", 'Current Assessment'!R1, "")</f>
         <v/>
       </c>
       <c r="B24" s="17"/>
@@ -12968,7 +12993,7 @@
     </row>
     <row r="25" spans="1:6" ht="31.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -12996,7 +13021,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="str">
-        <f>IF(Input!B16&lt;&gt;"", Input!B16, "")</f>
+        <f>IF('Current Assessment'!B16&lt;&gt;"", 'Current Assessment'!B16, "")</f>
         <v>CSS</v>
       </c>
       <c r="B28" s="17"/>
@@ -13007,7 +13032,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="str">
-        <f>IF(Input!C16&lt;&gt;"", Input!C16, "")</f>
+        <f>IF('Current Assessment'!C16&lt;&gt;"", 'Current Assessment'!C16, "")</f>
         <v>Javascript</v>
       </c>
       <c r="B29" s="17"/>
@@ -13018,7 +13043,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="16" t="str">
-        <f>IF(Input!D16&lt;&gt;"", Input!D16, "")</f>
+        <f>IF('Current Assessment'!D16&lt;&gt;"", 'Current Assessment'!D16, "")</f>
         <v>DB Backup/Restore</v>
       </c>
       <c r="B30" s="17"/>
@@ -13029,7 +13054,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="str">
-        <f>IF(Input!E16&lt;&gt;"", Input!E16, "")</f>
+        <f>IF('Current Assessment'!E16&lt;&gt;"", 'Current Assessment'!E16, "")</f>
         <v/>
       </c>
       <c r="B31" s="17"/>
@@ -13040,7 +13065,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="16" t="str">
-        <f>IF(Input!F16&lt;&gt;"", Input!F16, "")</f>
+        <f>IF('Current Assessment'!F16&lt;&gt;"", 'Current Assessment'!F16, "")</f>
         <v/>
       </c>
       <c r="B32" s="17"/>
@@ -13051,7 +13076,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="16" t="str">
-        <f>IF(Input!G16&lt;&gt;"", Input!G16, "")</f>
+        <f>IF('Current Assessment'!G16&lt;&gt;"", 'Current Assessment'!G16, "")</f>
         <v/>
       </c>
       <c r="B33" s="17"/>
@@ -13062,7 +13087,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="str">
-        <f>IF(Input!H16&lt;&gt;"", Input!H16, "")</f>
+        <f>IF('Current Assessment'!H16&lt;&gt;"", 'Current Assessment'!H16, "")</f>
         <v/>
       </c>
       <c r="B34" s="17"/>
@@ -13073,7 +13098,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="16" t="str">
-        <f>IF(Input!I16&lt;&gt;"", Input!I16, "")</f>
+        <f>IF('Current Assessment'!I16&lt;&gt;"", 'Current Assessment'!I16, "")</f>
         <v/>
       </c>
       <c r="B35" s="17"/>
@@ -13084,7 +13109,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="16" t="str">
-        <f>IF(Input!J16&lt;&gt;"", Input!J16, "")</f>
+        <f>IF('Current Assessment'!J16&lt;&gt;"", 'Current Assessment'!J16, "")</f>
         <v/>
       </c>
       <c r="B36" s="17"/>
@@ -13095,7 +13120,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="16" t="str">
-        <f>IF(Input!K16&lt;&gt;"", Input!K16, "")</f>
+        <f>IF('Current Assessment'!K16&lt;&gt;"", 'Current Assessment'!K16, "")</f>
         <v/>
       </c>
       <c r="B37" s="17"/>
@@ -13106,7 +13131,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="16" t="str">
-        <f>IF(Input!L16&lt;&gt;"", Input!L16, "")</f>
+        <f>IF('Current Assessment'!L16&lt;&gt;"", 'Current Assessment'!L16, "")</f>
         <v/>
       </c>
       <c r="B38" s="17"/>
@@ -13117,7 +13142,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="16" t="str">
-        <f>IF(Input!M16&lt;&gt;"", Input!M16, "")</f>
+        <f>IF('Current Assessment'!M16&lt;&gt;"", 'Current Assessment'!M16, "")</f>
         <v/>
       </c>
       <c r="B39" s="17"/>
@@ -13128,7 +13153,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="16" t="str">
-        <f>IF(Input!N16&lt;&gt;"", Input!N16, "")</f>
+        <f>IF('Current Assessment'!N16&lt;&gt;"", 'Current Assessment'!N16, "")</f>
         <v/>
       </c>
       <c r="B40" s="17"/>
@@ -13139,7 +13164,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="16" t="str">
-        <f>IF(Input!O16&lt;&gt;"", Input!O16, "")</f>
+        <f>IF('Current Assessment'!O16&lt;&gt;"", 'Current Assessment'!O16, "")</f>
         <v/>
       </c>
       <c r="B41" s="17"/>
@@ -13150,7 +13175,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="16" t="str">
-        <f>IF(Input!P16&lt;&gt;"", Input!P16, "")</f>
+        <f>IF('Current Assessment'!P16&lt;&gt;"", 'Current Assessment'!P16, "")</f>
         <v/>
       </c>
       <c r="B42" s="17"/>
@@ -13161,7 +13186,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="16" t="str">
-        <f>IF(Input!Q16&lt;&gt;"", Input!Q16, "")</f>
+        <f>IF('Current Assessment'!Q16&lt;&gt;"", 'Current Assessment'!Q16, "")</f>
         <v/>
       </c>
       <c r="B43" s="17"/>
@@ -13172,7 +13197,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="16" t="str">
-        <f>IF(Input!R16&lt;&gt;"", Input!R16, "")</f>
+        <f>IF('Current Assessment'!R16&lt;&gt;"", 'Current Assessment'!R16, "")</f>
         <v/>
       </c>
       <c r="B44" s="17"/>
@@ -13197,11 +13222,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:R33"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13289,13 +13313,13 @@
         <v>Person 1</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E2" s="25"/>
       <c r="F2" s="25"/>
@@ -13318,13 +13342,13 @@
         <v>Person 2</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
@@ -13347,13 +13371,13 @@
         <v>Team 1</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E4" s="25"/>
       <c r="F4" s="25"/>
@@ -13580,7 +13604,7 @@
     <row r="14" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -13656,287 +13680,221 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B17" s="28">
-        <f>Heatmap!B1</f>
-        <v>0</v>
+        <f>Current_Calcs!B1</f>
+        <v>1</v>
       </c>
       <c r="C17" s="28">
-        <f>Heatmap!C1</f>
+        <f>Current_Calcs!C1</f>
         <v>1</v>
       </c>
       <c r="D17" s="28">
-        <f>Heatmap!D1</f>
+        <f>Current_Calcs!D1</f>
         <v>1</v>
       </c>
       <c r="E17" s="28" t="str">
-        <f>Heatmap!E1</f>
+        <f>Current_Calcs!E1</f>
         <v/>
       </c>
       <c r="F17" s="29" t="str">
-        <f>Heatmap!F1</f>
+        <f>Current_Calcs!F1</f>
         <v/>
       </c>
       <c r="G17" s="29" t="str">
-        <f>Heatmap!G1</f>
+        <f>Current_Calcs!G1</f>
         <v/>
       </c>
       <c r="H17" s="29" t="str">
-        <f>Heatmap!H1</f>
+        <f>Current_Calcs!H1</f>
         <v/>
       </c>
       <c r="I17" s="29" t="str">
-        <f>Heatmap!I1</f>
+        <f>Current_Calcs!I1</f>
         <v/>
       </c>
       <c r="J17" s="29" t="str">
-        <f>Heatmap!J1</f>
+        <f>Current_Calcs!J1</f>
         <v/>
       </c>
       <c r="K17" s="29" t="str">
-        <f>Heatmap!K1</f>
+        <f>Current_Calcs!K1</f>
         <v/>
       </c>
       <c r="L17" s="29" t="str">
-        <f>Heatmap!L1</f>
+        <f>Current_Calcs!L1</f>
         <v/>
       </c>
       <c r="M17" s="29" t="str">
-        <f>Heatmap!M1</f>
+        <f>Current_Calcs!M1</f>
         <v/>
       </c>
       <c r="N17" s="29" t="str">
-        <f>Heatmap!N1</f>
+        <f>Current_Calcs!N1</f>
         <v/>
       </c>
       <c r="O17" s="29" t="str">
-        <f>Heatmap!O1</f>
+        <f>Current_Calcs!O1</f>
         <v/>
       </c>
       <c r="P17" s="29" t="str">
-        <f>Heatmap!P1</f>
+        <f>Current_Calcs!P1</f>
         <v/>
       </c>
       <c r="Q17" s="29" t="str">
-        <f>Heatmap!Q1</f>
+        <f>Current_Calcs!Q1</f>
         <v/>
       </c>
       <c r="R17" s="29" t="str">
-        <f>Heatmap!R1</f>
+        <f>Current_Calcs!R1</f>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B18" s="28">
-        <f>Heatmap!B2</f>
+        <f>Current_Calcs!B2</f>
         <v>1</v>
       </c>
       <c r="C18" s="28">
-        <f>Heatmap!C2</f>
+        <f>Current_Calcs!C2</f>
         <v>1</v>
       </c>
       <c r="D18" s="28">
-        <f>Heatmap!D2</f>
+        <f>Current_Calcs!D2</f>
         <v>2</v>
       </c>
       <c r="E18" s="28" t="str">
-        <f>Heatmap!E2</f>
+        <f>Current_Calcs!E2</f>
         <v/>
       </c>
       <c r="F18" s="29" t="str">
-        <f>Heatmap!F2</f>
+        <f>Current_Calcs!F2</f>
         <v/>
       </c>
       <c r="G18" s="29" t="str">
-        <f>Heatmap!G2</f>
+        <f>Current_Calcs!G2</f>
         <v/>
       </c>
       <c r="H18" s="29" t="str">
-        <f>Heatmap!H2</f>
+        <f>Current_Calcs!H2</f>
         <v/>
       </c>
       <c r="I18" s="29" t="str">
-        <f>Heatmap!I2</f>
+        <f>Current_Calcs!I2</f>
         <v/>
       </c>
       <c r="J18" s="29" t="str">
-        <f>Heatmap!J2</f>
+        <f>Current_Calcs!J2</f>
         <v/>
       </c>
       <c r="K18" s="29" t="str">
-        <f>Heatmap!K2</f>
+        <f>Current_Calcs!K2</f>
         <v/>
       </c>
       <c r="L18" s="29" t="str">
-        <f>Heatmap!L2</f>
+        <f>Current_Calcs!L2</f>
         <v/>
       </c>
       <c r="M18" s="29" t="str">
-        <f>Heatmap!M2</f>
+        <f>Current_Calcs!M2</f>
         <v/>
       </c>
       <c r="N18" s="29" t="str">
-        <f>Heatmap!N2</f>
+        <f>Current_Calcs!N2</f>
         <v/>
       </c>
       <c r="O18" s="29" t="str">
-        <f>Heatmap!O2</f>
+        <f>Current_Calcs!O2</f>
         <v/>
       </c>
       <c r="P18" s="29" t="str">
-        <f>Heatmap!P2</f>
+        <f>Current_Calcs!P2</f>
         <v/>
       </c>
       <c r="Q18" s="29" t="str">
-        <f>Heatmap!Q2</f>
+        <f>Current_Calcs!Q2</f>
         <v/>
       </c>
       <c r="R18" s="29" t="str">
-        <f>Heatmap!R2</f>
+        <f>Current_Calcs!R2</f>
         <v/>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="33" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B19" s="28">
-        <f>Heatmap!B3</f>
-        <v>0</v>
+        <f>Current_Calcs!B3</f>
+        <v>1</v>
       </c>
       <c r="C19" s="28">
-        <f>Heatmap!C3</f>
+        <f>Current_Calcs!C3</f>
         <v>0</v>
       </c>
       <c r="D19" s="28">
-        <f>Heatmap!D3</f>
+        <f>Current_Calcs!D3</f>
         <v>1</v>
       </c>
       <c r="E19" s="28" t="str">
-        <f>Heatmap!E3</f>
+        <f>Current_Calcs!E3</f>
         <v/>
       </c>
       <c r="F19" s="29" t="str">
-        <f>Heatmap!F3</f>
+        <f>Current_Calcs!F3</f>
         <v/>
       </c>
       <c r="G19" s="29" t="str">
-        <f>Heatmap!G3</f>
+        <f>Current_Calcs!G3</f>
         <v/>
       </c>
       <c r="H19" s="29" t="str">
-        <f>Heatmap!H3</f>
+        <f>Current_Calcs!H3</f>
         <v/>
       </c>
       <c r="I19" s="29" t="str">
-        <f>Heatmap!I3</f>
+        <f>Current_Calcs!I3</f>
         <v/>
       </c>
       <c r="J19" s="29" t="str">
-        <f>Heatmap!J3</f>
+        <f>Current_Calcs!J3</f>
         <v/>
       </c>
       <c r="K19" s="29" t="str">
-        <f>Heatmap!K3</f>
+        <f>Current_Calcs!K3</f>
         <v/>
       </c>
       <c r="L19" s="29" t="str">
-        <f>Heatmap!L3</f>
+        <f>Current_Calcs!L3</f>
         <v/>
       </c>
       <c r="M19" s="29" t="str">
-        <f>Heatmap!M3</f>
+        <f>Current_Calcs!M3</f>
         <v/>
       </c>
       <c r="N19" s="29" t="str">
-        <f>Heatmap!N3</f>
+        <f>Current_Calcs!N3</f>
         <v/>
       </c>
       <c r="O19" s="29" t="str">
-        <f>Heatmap!O3</f>
+        <f>Current_Calcs!O3</f>
         <v/>
       </c>
       <c r="P19" s="29" t="str">
-        <f>Heatmap!P3</f>
+        <f>Current_Calcs!P3</f>
         <v/>
       </c>
       <c r="Q19" s="29" t="str">
-        <f>Heatmap!Q3</f>
+        <f>Current_Calcs!Q3</f>
         <v/>
       </c>
       <c r="R19" s="29" t="str">
-        <f>Heatmap!R3</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28">
-        <v>3</v>
-      </c>
-      <c r="D28" t="s">
-        <v>40</v>
-      </c>
-      <c r="E28" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29">
-        <v>6</v>
-      </c>
-      <c r="D29" t="s">
-        <v>46</v>
-      </c>
-      <c r="E29" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="D30" t="s">
-        <v>48</v>
-      </c>
-      <c r="E30" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33">
-        <v>5</v>
+        <f>Current_Calcs!R3</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -13990,28 +13948,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:R22"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="B1">
-        <f t="shared" ref="B1:R1" si="0">IF(B$5&lt;&gt;"",COUNTIF(B$6:B$17, "&gt;= 3"),"")</f>
-        <v>0</v>
+        <f t="shared" ref="B1:R1" si="0">IF(B$4&lt;&gt;"",COUNTIF(B$5:B$16, "&gt;= 3"),"")</f>
+        <v>1</v>
       </c>
       <c r="C1">
         <f t="shared" si="0"/>
@@ -14080,10 +14034,10 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:R2" si="1">IF(B$5&lt;&gt;"",COUNTIF(B$6:B$17, "&gt;= 2"),"")</f>
+        <f t="shared" ref="B2:R2" si="1">IF(B$4&lt;&gt;"",COUNTIF(B$5:B$16, "&gt;= 2"),"")</f>
         <v>1</v>
       </c>
       <c r="C2">
@@ -14153,11 +14107,11 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:R3" si="2">IF(B$5&lt;&gt;"",COUNTIF(B$6:B$17, "= 1"),"")</f>
-        <v>0</v>
+        <f t="shared" ref="B3:R3" si="2">IF(B$4&lt;&gt;"",COUNTIF(B$5:B$16, "= 1"),"")</f>
+        <v>1</v>
       </c>
       <c r="C3">
         <f t="shared" si="2"/>
@@ -14224,1051 +14178,1048 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+    <row r="4" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="str">
+        <f>IF('Current Assessment'!B1&lt;&gt;"",'Current Assessment'!B1,"")</f>
+        <v>CSS</v>
+      </c>
+      <c r="C4" s="9" t="str">
+        <f>IF('Current Assessment'!C1&lt;&gt;"",'Current Assessment'!C1,"")</f>
+        <v>Javascript</v>
+      </c>
+      <c r="D4" s="9" t="str">
+        <f>IF('Current Assessment'!D1&lt;&gt;"",'Current Assessment'!D1,"")</f>
+        <v>DB Backup/Restore</v>
+      </c>
+      <c r="E4" s="9" t="str">
+        <f>IF('Current Assessment'!E1&lt;&gt;"",'Current Assessment'!E1,"")</f>
+        <v/>
+      </c>
+      <c r="F4" s="9" t="str">
+        <f>IF('Current Assessment'!F1&lt;&gt;"",'Current Assessment'!F1,"")</f>
+        <v/>
+      </c>
+      <c r="G4" s="9" t="str">
+        <f>IF('Current Assessment'!G1&lt;&gt;"",'Current Assessment'!G1,"")</f>
+        <v/>
+      </c>
+      <c r="H4" s="9" t="str">
+        <f>IF('Current Assessment'!H1&lt;&gt;"",'Current Assessment'!H1,"")</f>
+        <v/>
+      </c>
+      <c r="I4" s="9" t="str">
+        <f>IF('Current Assessment'!I1&lt;&gt;"",'Current Assessment'!I1,"")</f>
+        <v/>
+      </c>
+      <c r="J4" s="9" t="str">
+        <f>IF('Current Assessment'!J1&lt;&gt;"",'Current Assessment'!J1,"")</f>
+        <v/>
+      </c>
+      <c r="K4" s="9" t="str">
+        <f>IF('Current Assessment'!K1&lt;&gt;"",'Current Assessment'!K1,"")</f>
+        <v/>
+      </c>
+      <c r="L4" s="9" t="str">
+        <f>IF('Current Assessment'!L1&lt;&gt;"",'Current Assessment'!L1,"")</f>
+        <v/>
+      </c>
+      <c r="M4" s="9" t="str">
+        <f>IF('Current Assessment'!M1&lt;&gt;"",'Current Assessment'!M1,"")</f>
+        <v/>
+      </c>
+      <c r="N4" s="9" t="str">
+        <f>IF('Current Assessment'!N1&lt;&gt;"",'Current Assessment'!N1,"")</f>
+        <v/>
+      </c>
+      <c r="O4" s="9" t="str">
+        <f>IF('Current Assessment'!O1&lt;&gt;"",'Current Assessment'!O1,"")</f>
+        <v/>
+      </c>
+      <c r="P4" s="9" t="str">
+        <f>IF('Current Assessment'!P1&lt;&gt;"",'Current Assessment'!P1,"")</f>
+        <v/>
+      </c>
+      <c r="Q4" s="9" t="str">
+        <f>IF('Current Assessment'!Q1&lt;&gt;"",'Current Assessment'!Q1,"")</f>
+        <v/>
+      </c>
+      <c r="R4" s="9" t="str">
+        <f>IF('Current Assessment'!R1&lt;&gt;"",'Current Assessment'!R1,"")</f>
+        <v/>
+      </c>
     </row>
-    <row r="5" spans="1:18" s="35" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="36" t="str">
-        <f>IF(Input!B1&lt;&gt;"",Input!B1,"")</f>
-        <v>CSS</v>
-      </c>
-      <c r="C5" s="36" t="str">
-        <f>IF(Input!C1&lt;&gt;"",Input!C1,"")</f>
-        <v>Javascript</v>
-      </c>
-      <c r="D5" s="36" t="str">
-        <f>IF(Input!D1&lt;&gt;"",Input!D1,"")</f>
-        <v>DB Backup/Restore</v>
-      </c>
-      <c r="E5" s="36" t="str">
-        <f>IF(Input!E1&lt;&gt;"",Input!E1,"")</f>
-        <v/>
-      </c>
-      <c r="F5" s="36" t="str">
-        <f>IF(Input!F1&lt;&gt;"",Input!F1,"")</f>
-        <v/>
-      </c>
-      <c r="G5" s="36" t="str">
-        <f>IF(Input!G1&lt;&gt;"",Input!G1,"")</f>
-        <v/>
-      </c>
-      <c r="H5" s="36" t="str">
-        <f>IF(Input!H1&lt;&gt;"",Input!H1,"")</f>
-        <v/>
-      </c>
-      <c r="I5" s="36" t="str">
-        <f>IF(Input!I1&lt;&gt;"",Input!I1,"")</f>
-        <v/>
-      </c>
-      <c r="J5" s="36" t="str">
-        <f>IF(Input!J1&lt;&gt;"",Input!J1,"")</f>
-        <v/>
-      </c>
-      <c r="K5" s="36" t="str">
-        <f>IF(Input!K1&lt;&gt;"",Input!K1,"")</f>
-        <v/>
-      </c>
-      <c r="L5" s="36" t="str">
-        <f>IF(Input!L1&lt;&gt;"",Input!L1,"")</f>
-        <v/>
-      </c>
-      <c r="M5" s="36" t="str">
-        <f>IF(Input!M1&lt;&gt;"",Input!M1,"")</f>
-        <v/>
-      </c>
-      <c r="N5" s="36" t="str">
-        <f>IF(Input!N1&lt;&gt;"",Input!N1,"")</f>
-        <v/>
-      </c>
-      <c r="O5" s="36" t="str">
-        <f>IF(Input!O1&lt;&gt;"",Input!O1,"")</f>
-        <v/>
-      </c>
-      <c r="P5" s="36" t="str">
-        <f>IF(Input!P1&lt;&gt;"",Input!P1,"")</f>
-        <v/>
-      </c>
-      <c r="Q5" s="36" t="str">
-        <f>IF(Input!Q1&lt;&gt;"",Input!Q1,"")</f>
-        <v/>
-      </c>
-      <c r="R5" s="36" t="str">
-        <f>IF(Input!R1&lt;&gt;"",Input!R1,"")</f>
-        <v/>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="str">
+        <f>'Current Assessment'!A2</f>
+        <v>Person 1</v>
+      </c>
+      <c r="B5">
+        <f>IFERROR(MATCH('Current Assessment'!B2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <f>IFERROR(MATCH('Current Assessment'!C2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <f>IFERROR(MATCH('Current Assessment'!D2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f>IFERROR(MATCH('Current Assessment'!E2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f>IFERROR(MATCH('Current Assessment'!F2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f>IFERROR(MATCH('Current Assessment'!G2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <f>IFERROR(MATCH('Current Assessment'!H2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f>IFERROR(MATCH('Current Assessment'!I2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <f>IFERROR(MATCH('Current Assessment'!J2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <f>IFERROR(MATCH('Current Assessment'!K2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <f>IFERROR(MATCH('Current Assessment'!L2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <f>IFERROR(MATCH('Current Assessment'!M2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <f>IFERROR(MATCH('Current Assessment'!N2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f>IFERROR(MATCH('Current Assessment'!O2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <f>IFERROR(MATCH('Current Assessment'!P2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <f>IFERROR(MATCH('Current Assessment'!Q2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <f>IFERROR(MATCH('Current Assessment'!R2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="str">
-        <f>Input!A2</f>
-        <v>Person 1</v>
+        <f>'Current Assessment'!A3</f>
+        <v>Person 2</v>
       </c>
       <c r="B6">
-        <f>IFERROR(MATCH(Input!B2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!B3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="C6">
-        <f>IFERROR(MATCH(Input!C2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
+        <f>IFERROR(MATCH('Current Assessment'!C3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>3</v>
       </c>
       <c r="D6">
-        <f>IFERROR(MATCH(Input!D2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>1</v>
+        <f>IFERROR(MATCH('Current Assessment'!D3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>2</v>
       </c>
       <c r="E6">
-        <f>IFERROR(MATCH(Input!E2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!E3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F6">
-        <f>IFERROR(MATCH(Input!F2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!F3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G6">
-        <f>IFERROR(MATCH(Input!G2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!G3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H6">
-        <f>IFERROR(MATCH(Input!H2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!H3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I6">
-        <f>IFERROR(MATCH(Input!I2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!I3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J6">
-        <f>IFERROR(MATCH(Input!J2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!J3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K6">
-        <f>IFERROR(MATCH(Input!K2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!K3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L6">
-        <f>IFERROR(MATCH(Input!L2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!L3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M6">
-        <f>IFERROR(MATCH(Input!M2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!M3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N6">
-        <f>IFERROR(MATCH(Input!N2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!N3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O6">
-        <f>IFERROR(MATCH(Input!O2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!O3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P6">
-        <f>IFERROR(MATCH(Input!P2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!P3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q6">
-        <f>IFERROR(MATCH(Input!Q2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!Q3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R6">
-        <f>IFERROR(MATCH(Input!R2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!R3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="str">
-        <f>Input!A3</f>
-        <v>Person 2</v>
+        <f>'Current Assessment'!A4</f>
+        <v>Team 1</v>
       </c>
       <c r="B7">
-        <f>IFERROR(MATCH(Input!B3,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
+        <f>IFERROR(MATCH('Current Assessment'!B4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>3</v>
       </c>
       <c r="C7">
-        <f>IFERROR(MATCH(Input!C3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!C4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f>IFERROR(MATCH('Current Assessment'!D4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>3</v>
       </c>
-      <c r="D7">
-        <f>IFERROR(MATCH(Input!D3,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>2</v>
-      </c>
       <c r="E7">
-        <f>IFERROR(MATCH(Input!E3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!E4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F7">
-        <f>IFERROR(MATCH(Input!F3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!F4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G7">
-        <f>IFERROR(MATCH(Input!G3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!G4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H7">
-        <f>IFERROR(MATCH(Input!H3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!H4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I7">
-        <f>IFERROR(MATCH(Input!I3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!I4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J7">
-        <f>IFERROR(MATCH(Input!J3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!J4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K7">
-        <f>IFERROR(MATCH(Input!K3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!K4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L7">
-        <f>IFERROR(MATCH(Input!L3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!L4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M7">
-        <f>IFERROR(MATCH(Input!M3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!M4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N7">
-        <f>IFERROR(MATCH(Input!N3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!N4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O7">
-        <f>IFERROR(MATCH(Input!O3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!O4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P7">
-        <f>IFERROR(MATCH(Input!P3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!P4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q7">
-        <f>IFERROR(MATCH(Input!Q3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!Q4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R7">
-        <f>IFERROR(MATCH(Input!R3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!R4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="str">
-        <f>Input!A4</f>
-        <v>Team 1</v>
+        <f>'Current Assessment'!A5</f>
+        <v/>
       </c>
       <c r="B8">
-        <f>IFERROR(MATCH(Input!B4,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>2</v>
+        <f>IFERROR(MATCH('Current Assessment'!B5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
       </c>
       <c r="C8">
-        <f>IFERROR(MATCH(Input!C4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!C5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="D8">
-        <f>IFERROR(MATCH(Input!D4,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>3</v>
+        <f>IFERROR(MATCH('Current Assessment'!D5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
       </c>
       <c r="E8">
-        <f>IFERROR(MATCH(Input!E4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!E5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F8">
-        <f>IFERROR(MATCH(Input!F4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!F5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G8">
-        <f>IFERROR(MATCH(Input!G4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!G5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H8">
-        <f>IFERROR(MATCH(Input!H4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!H5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I8">
-        <f>IFERROR(MATCH(Input!I4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!I5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J8">
-        <f>IFERROR(MATCH(Input!J4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!J5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K8">
-        <f>IFERROR(MATCH(Input!K4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!K5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L8">
-        <f>IFERROR(MATCH(Input!L4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!L5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M8">
-        <f>IFERROR(MATCH(Input!M4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!M5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N8">
-        <f>IFERROR(MATCH(Input!N4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!N5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O8">
-        <f>IFERROR(MATCH(Input!O4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!O5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P8">
-        <f>IFERROR(MATCH(Input!P4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!P5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q8">
-        <f>IFERROR(MATCH(Input!Q4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!Q5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R8">
-        <f>IFERROR(MATCH(Input!R4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!R5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="str">
-        <f>Input!A5</f>
+        <f>'Current Assessment'!A6</f>
         <v/>
       </c>
       <c r="B9">
-        <f>IFERROR(MATCH(Input!B5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!B6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="C9">
-        <f>IFERROR(MATCH(Input!C5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!C6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="D9">
-        <f>IFERROR(MATCH(Input!D5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!D6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="E9">
-        <f>IFERROR(MATCH(Input!E5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!E6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F9">
-        <f>IFERROR(MATCH(Input!F5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!F6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G9">
-        <f>IFERROR(MATCH(Input!G5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!G6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H9">
-        <f>IFERROR(MATCH(Input!H5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!H6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I9">
-        <f>IFERROR(MATCH(Input!I5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!I6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J9">
-        <f>IFERROR(MATCH(Input!J5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!J6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K9">
-        <f>IFERROR(MATCH(Input!K5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!K6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L9">
-        <f>IFERROR(MATCH(Input!L5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!L6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M9">
-        <f>IFERROR(MATCH(Input!M5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!M6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N9">
-        <f>IFERROR(MATCH(Input!N5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!N6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O9">
-        <f>IFERROR(MATCH(Input!O5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!O6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P9">
-        <f>IFERROR(MATCH(Input!P5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!P6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q9">
-        <f>IFERROR(MATCH(Input!Q5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!Q6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R9">
-        <f>IFERROR(MATCH(Input!R5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!R6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="str">
-        <f>Input!A6</f>
+        <f>'Current Assessment'!A7</f>
         <v/>
       </c>
       <c r="B10">
-        <f>IFERROR(MATCH(Input!B6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!B7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="C10">
-        <f>IFERROR(MATCH(Input!C6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!C7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="D10">
-        <f>IFERROR(MATCH(Input!D6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!D7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="E10">
-        <f>IFERROR(MATCH(Input!E6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!E7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F10">
-        <f>IFERROR(MATCH(Input!F6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!F7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G10">
-        <f>IFERROR(MATCH(Input!G6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!G7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H10">
-        <f>IFERROR(MATCH(Input!H6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!H7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I10">
-        <f>IFERROR(MATCH(Input!I6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!I7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J10">
-        <f>IFERROR(MATCH(Input!J6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!J7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K10">
-        <f>IFERROR(MATCH(Input!K6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!K7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L10">
-        <f>IFERROR(MATCH(Input!L6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!L7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M10">
-        <f>IFERROR(MATCH(Input!M6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!M7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N10">
-        <f>IFERROR(MATCH(Input!N6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!N7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O10">
-        <f>IFERROR(MATCH(Input!O6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!O7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P10">
-        <f>IFERROR(MATCH(Input!P6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!P7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q10">
-        <f>IFERROR(MATCH(Input!Q6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!Q7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R10">
-        <f>IFERROR(MATCH(Input!R6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!R7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="str">
-        <f>Input!A7</f>
+        <f>'Current Assessment'!A8</f>
         <v/>
       </c>
       <c r="B11">
-        <f>IFERROR(MATCH(Input!B7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!B8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="C11">
-        <f>IFERROR(MATCH(Input!C7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!C8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="D11">
-        <f>IFERROR(MATCH(Input!D7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!D8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="E11">
-        <f>IFERROR(MATCH(Input!E7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!E8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F11">
-        <f>IFERROR(MATCH(Input!F7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!F8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G11">
-        <f>IFERROR(MATCH(Input!G7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!G8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H11">
-        <f>IFERROR(MATCH(Input!H7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!H8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I11">
-        <f>IFERROR(MATCH(Input!I7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!I8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J11">
-        <f>IFERROR(MATCH(Input!J7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!J8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K11">
-        <f>IFERROR(MATCH(Input!K7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!K8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L11">
-        <f>IFERROR(MATCH(Input!L7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!L8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M11">
-        <f>IFERROR(MATCH(Input!M7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!M8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N11">
-        <f>IFERROR(MATCH(Input!N7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!N8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O11">
-        <f>IFERROR(MATCH(Input!O7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!O8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P11">
-        <f>IFERROR(MATCH(Input!P7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!P8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q11">
-        <f>IFERROR(MATCH(Input!Q7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!Q8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R11">
-        <f>IFERROR(MATCH(Input!R7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!R8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="str">
-        <f>Input!A8</f>
+        <f>'Current Assessment'!A9</f>
         <v/>
       </c>
       <c r="B12">
-        <f>IFERROR(MATCH(Input!B8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!B9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="C12">
-        <f>IFERROR(MATCH(Input!C8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!C9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="D12">
-        <f>IFERROR(MATCH(Input!D8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!D9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="E12">
-        <f>IFERROR(MATCH(Input!E8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!E9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F12">
-        <f>IFERROR(MATCH(Input!F8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!F9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G12">
-        <f>IFERROR(MATCH(Input!G8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!G9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H12">
-        <f>IFERROR(MATCH(Input!H8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!H9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I12">
-        <f>IFERROR(MATCH(Input!I8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!I9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J12">
-        <f>IFERROR(MATCH(Input!J8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!J9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K12">
-        <f>IFERROR(MATCH(Input!K8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!K9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L12">
-        <f>IFERROR(MATCH(Input!L8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!L9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M12">
-        <f>IFERROR(MATCH(Input!M8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!M9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N12">
-        <f>IFERROR(MATCH(Input!N8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!N9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O12">
-        <f>IFERROR(MATCH(Input!O8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!O9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P12">
-        <f>IFERROR(MATCH(Input!P8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!P9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q12">
-        <f>IFERROR(MATCH(Input!Q8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!Q9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R12">
-        <f>IFERROR(MATCH(Input!R8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!R9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="str">
-        <f>Input!A9</f>
+        <f>'Current Assessment'!A10</f>
         <v/>
       </c>
       <c r="B13">
-        <f>IFERROR(MATCH(Input!B9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!B10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="C13">
-        <f>IFERROR(MATCH(Input!C9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!C10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="D13">
-        <f>IFERROR(MATCH(Input!D9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!D10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="E13">
-        <f>IFERROR(MATCH(Input!E9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!E10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F13">
-        <f>IFERROR(MATCH(Input!F9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!F10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G13">
-        <f>IFERROR(MATCH(Input!G9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!G10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H13">
-        <f>IFERROR(MATCH(Input!H9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!H10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I13">
-        <f>IFERROR(MATCH(Input!I9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!I10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J13">
-        <f>IFERROR(MATCH(Input!J9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!J10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K13">
-        <f>IFERROR(MATCH(Input!K9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!K10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L13">
-        <f>IFERROR(MATCH(Input!L9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!L10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M13">
-        <f>IFERROR(MATCH(Input!M9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!M10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N13">
-        <f>IFERROR(MATCH(Input!N9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!N10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O13">
-        <f>IFERROR(MATCH(Input!O9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!O10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P13">
-        <f>IFERROR(MATCH(Input!P9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!P10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q13">
-        <f>IFERROR(MATCH(Input!Q9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!Q10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R13">
-        <f>IFERROR(MATCH(Input!R9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!R10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="str">
-        <f>Input!A10</f>
+        <f>'Current Assessment'!A11</f>
         <v/>
       </c>
       <c r="B14">
-        <f>IFERROR(MATCH(Input!B10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!B11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="C14">
-        <f>IFERROR(MATCH(Input!C10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!C11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="D14">
-        <f>IFERROR(MATCH(Input!D10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!D11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="E14">
-        <f>IFERROR(MATCH(Input!E10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!E11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F14">
-        <f>IFERROR(MATCH(Input!F10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!F11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G14">
-        <f>IFERROR(MATCH(Input!G10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!G11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H14">
-        <f>IFERROR(MATCH(Input!H10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!H11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I14">
-        <f>IFERROR(MATCH(Input!I10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!I11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J14">
-        <f>IFERROR(MATCH(Input!J10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!J11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K14">
-        <f>IFERROR(MATCH(Input!K10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!K11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L14">
-        <f>IFERROR(MATCH(Input!L10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!L11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M14">
-        <f>IFERROR(MATCH(Input!M10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!M11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N14">
-        <f>IFERROR(MATCH(Input!N10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!N11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O14">
-        <f>IFERROR(MATCH(Input!O10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!O11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P14">
-        <f>IFERROR(MATCH(Input!P10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!P11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q14">
-        <f>IFERROR(MATCH(Input!Q10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!Q11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R14">
-        <f>IFERROR(MATCH(Input!R10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!R11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="str">
-        <f>Input!A11</f>
+        <f>'Current Assessment'!A12</f>
         <v/>
       </c>
       <c r="B15">
-        <f>IFERROR(MATCH(Input!B11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!B12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="C15">
-        <f>IFERROR(MATCH(Input!C11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!C12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="D15">
-        <f>IFERROR(MATCH(Input!D11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!D12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="E15">
-        <f>IFERROR(MATCH(Input!E11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!E12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F15">
-        <f>IFERROR(MATCH(Input!F11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!F12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G15">
-        <f>IFERROR(MATCH(Input!G11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!G12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H15">
-        <f>IFERROR(MATCH(Input!H11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!H12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I15">
-        <f>IFERROR(MATCH(Input!I11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!I12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J15">
-        <f>IFERROR(MATCH(Input!J11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!J12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K15">
-        <f>IFERROR(MATCH(Input!K11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!K12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L15">
-        <f>IFERROR(MATCH(Input!L11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!L12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M15">
-        <f>IFERROR(MATCH(Input!M11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!M12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N15">
-        <f>IFERROR(MATCH(Input!N11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!N12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O15">
-        <f>IFERROR(MATCH(Input!O11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!O12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P15">
-        <f>IFERROR(MATCH(Input!P11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!P12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q15">
-        <f>IFERROR(MATCH(Input!Q11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!Q12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R15">
-        <f>IFERROR(MATCH(Input!R11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!R12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="str">
-        <f>Input!A12</f>
+        <f>'Current Assessment'!A13</f>
         <v/>
       </c>
       <c r="B16">
-        <f>IFERROR(MATCH(Input!B12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!B13,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="C16">
-        <f>IFERROR(MATCH(Input!C12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!C13,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="D16">
-        <f>IFERROR(MATCH(Input!D12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!D13,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="E16">
-        <f>IFERROR(MATCH(Input!E12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!E13,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F16">
-        <f>IFERROR(MATCH(Input!F12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!F13,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G16">
-        <f>IFERROR(MATCH(Input!G12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!G13,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H16">
-        <f>IFERROR(MATCH(Input!H12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!H13,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I16">
-        <f>IFERROR(MATCH(Input!I12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!I13,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J16">
-        <f>IFERROR(MATCH(Input!J12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!J13,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K16">
-        <f>IFERROR(MATCH(Input!K12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!K13,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L16">
-        <f>IFERROR(MATCH(Input!L12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!L13,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M16">
-        <f>IFERROR(MATCH(Input!M12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!M13,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N16">
-        <f>IFERROR(MATCH(Input!N12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!N13,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O16">
-        <f>IFERROR(MATCH(Input!O12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!O13,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P16">
-        <f>IFERROR(MATCH(Input!P12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!P13,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q16">
-        <f>IFERROR(MATCH(Input!Q12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!Q13,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R16">
-        <f>IFERROR(MATCH(Input!R12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH('Current Assessment'!R13,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="str">
-        <f>Input!A13</f>
-        <v/>
-      </c>
-      <c r="B17">
-        <f>IFERROR(MATCH(Input!B13,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <f>IFERROR(MATCH(Input!C13,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <f>IFERROR(MATCH(Input!D13,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <f>IFERROR(MATCH(Input!E13,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <f>IFERROR(MATCH(Input!F13,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <f>IFERROR(MATCH(Input!G13,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <f>IFERROR(MATCH(Input!H13,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <f>IFERROR(MATCH(Input!I13,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <f>IFERROR(MATCH(Input!J13,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <f>IFERROR(MATCH(Input!K13,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <f>IFERROR(MATCH(Input!L13,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <f>IFERROR(MATCH(Input!M13,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="N17">
-        <f>IFERROR(MATCH(Input!N13,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="O17">
-        <f>IFERROR(MATCH(Input!O13,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="P17">
-        <f>IFERROR(MATCH(Input!P13,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <f>IFERROR(MATCH(Input!Q13,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="R17">
-        <f>IFERROR(MATCH(Input!R13,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="6">
-        <f t="shared" ref="B18:R18" si="3">SUM(B6:B17)</f>
-        <v>2</v>
-      </c>
-      <c r="C18" s="6">
+    <row r="17" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="6">
+        <f t="shared" ref="B17:R17" si="3">SUM(B5:B16)</f>
+        <v>4</v>
+      </c>
+      <c r="C17" s="6">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D17" s="6">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E17" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F17" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G17" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H17" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I17" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J18" s="6">
+      <c r="J17" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K18" s="6">
+      <c r="K17" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L18" s="6">
+      <c r="L17" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M18" s="6">
+      <c r="M17" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N18" s="6">
+      <c r="N17" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O18" s="6">
+      <c r="O17" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P18" s="6">
+      <c r="P17" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Q18" s="6">
+      <c r="Q17" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R18" s="6">
+      <c r="R17" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>23</v>
+    <row r="18" spans="2:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>23</v>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B18:R18">
-    <cfRule type="colorScale" priority="7">
+  <conditionalFormatting sqref="B17:R17">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -15276,19 +15227,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:R17">
-    <cfRule type="colorScale" priority="9">
+  <conditionalFormatting sqref="B5:R16">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -15298,11 +15239,12 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="8" id="{339E999E-0713-46E1-92D7-78E999ECB110}">
+          <x14:cfRule type="iconSet" priority="7" id="{339E999E-0713-46E1-92D7-78E999ECB110}">
             <x14:iconSet iconSet="4TrafficLights" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -15322,7 +15264,7 @@
               <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>B1:R4</xm:sqref>
+          <xm:sqref>B1:R3</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -15332,20 +15274,6 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:U27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15360,99 +15288,99 @@
     <row r="1" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13"/>
       <c r="B1" s="13" t="str">
-        <f>IF(Input!B1&lt;&gt;"",Input!B1,"")</f>
+        <f>IF('Current Assessment'!B1&lt;&gt;"",'Current Assessment'!B1,"")</f>
         <v>CSS</v>
       </c>
       <c r="C1" s="13" t="str">
-        <f>IF(Input!C1&lt;&gt;"",Input!C1,"")</f>
+        <f>IF('Current Assessment'!C1&lt;&gt;"",'Current Assessment'!C1,"")</f>
         <v>Javascript</v>
       </c>
       <c r="D1" s="13" t="str">
-        <f>IF(Input!D1&lt;&gt;"",Input!D1,"")</f>
+        <f>IF('Current Assessment'!D1&lt;&gt;"",'Current Assessment'!D1,"")</f>
         <v>DB Backup/Restore</v>
       </c>
       <c r="E1" s="13" t="str">
-        <f>IF(Input!E1&lt;&gt;"",Input!E1,"")</f>
+        <f>IF('Current Assessment'!E1&lt;&gt;"",'Current Assessment'!E1,"")</f>
         <v/>
       </c>
       <c r="F1" s="13" t="str">
-        <f>IF(Input!F1&lt;&gt;"",Input!F1,"")</f>
+        <f>IF('Current Assessment'!F1&lt;&gt;"",'Current Assessment'!F1,"")</f>
         <v/>
       </c>
       <c r="G1" s="13" t="str">
-        <f>IF(Input!G1&lt;&gt;"",Input!G1,"")</f>
+        <f>IF('Current Assessment'!G1&lt;&gt;"",'Current Assessment'!G1,"")</f>
         <v/>
       </c>
       <c r="H1" s="13" t="str">
-        <f>IF(Input!H1&lt;&gt;"",Input!H1,"")</f>
+        <f>IF('Current Assessment'!H1&lt;&gt;"",'Current Assessment'!H1,"")</f>
         <v/>
       </c>
       <c r="I1" s="13" t="str">
-        <f>IF(Input!I1&lt;&gt;"",Input!I1,"")</f>
+        <f>IF('Current Assessment'!I1&lt;&gt;"",'Current Assessment'!I1,"")</f>
         <v/>
       </c>
       <c r="J1" s="13" t="str">
-        <f>IF(Input!J1&lt;&gt;"",Input!J1,"")</f>
+        <f>IF('Current Assessment'!J1&lt;&gt;"",'Current Assessment'!J1,"")</f>
         <v/>
       </c>
       <c r="K1" s="13" t="str">
-        <f>IF(Input!K1&lt;&gt;"",Input!K1,"")</f>
+        <f>IF('Current Assessment'!K1&lt;&gt;"",'Current Assessment'!K1,"")</f>
         <v/>
       </c>
       <c r="L1" s="13" t="str">
-        <f>IF(Input!L1&lt;&gt;"",Input!L1,"")</f>
+        <f>IF('Current Assessment'!L1&lt;&gt;"",'Current Assessment'!L1,"")</f>
         <v/>
       </c>
       <c r="M1" s="13" t="str">
-        <f>IF(Input!M1&lt;&gt;"",Input!M1,"")</f>
+        <f>IF('Current Assessment'!M1&lt;&gt;"",'Current Assessment'!M1,"")</f>
         <v/>
       </c>
       <c r="N1" s="13" t="str">
-        <f>IF(Input!N1&lt;&gt;"",Input!N1,"")</f>
+        <f>IF('Current Assessment'!N1&lt;&gt;"",'Current Assessment'!N1,"")</f>
         <v/>
       </c>
       <c r="O1" s="13" t="str">
-        <f>IF(Input!O1&lt;&gt;"",Input!O1,"")</f>
+        <f>IF('Current Assessment'!O1&lt;&gt;"",'Current Assessment'!O1,"")</f>
         <v/>
       </c>
       <c r="P1" s="13" t="str">
-        <f>IF(Input!P1&lt;&gt;"",Input!P1,"")</f>
+        <f>IF('Current Assessment'!P1&lt;&gt;"",'Current Assessment'!P1,"")</f>
         <v/>
       </c>
       <c r="Q1" s="13" t="str">
-        <f>IF(Input!Q1&lt;&gt;"",Input!Q1,"")</f>
+        <f>IF('Current Assessment'!Q1&lt;&gt;"",'Current Assessment'!Q1,"")</f>
         <v/>
       </c>
       <c r="R1" s="13" t="str">
-        <f>IF(Input!R1&lt;&gt;"",Input!R1,"")</f>
+        <f>IF('Current Assessment'!R1&lt;&gt;"",'Current Assessment'!R1,"")</f>
         <v/>
       </c>
       <c r="S1" s="13" t="e">
-        <f>IF(Input!#REF!&lt;&gt;"",Input!#REF!,"")</f>
+        <f>IF('Current Assessment'!#REF!&lt;&gt;"",'Current Assessment'!#REF!,"")</f>
         <v>#REF!</v>
       </c>
       <c r="T1" s="13" t="e">
-        <f>IF(Input!#REF!&lt;&gt;"",Input!#REF!,"")</f>
+        <f>IF('Current Assessment'!#REF!&lt;&gt;"",'Current Assessment'!#REF!,"")</f>
         <v>#REF!</v>
       </c>
       <c r="U1" s="13" t="e">
-        <f>IF(Input!#REF!&lt;&gt;"",Input!#REF!,"")</f>
+        <f>IF('Current Assessment'!#REF!&lt;&gt;"",'Current Assessment'!#REF!,"")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="str">
-        <f>IF(Input!A2&lt;&gt;"", Input!A2, "")</f>
+        <f>IF('Current Assessment'!A2&lt;&gt;"", 'Current Assessment'!A2, "")</f>
         <v>Person 1</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
@@ -15474,7 +15402,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="str">
-        <f>IF(Input!A3&lt;&gt;"", Input!A3, "")</f>
+        <f>IF('Current Assessment'!A3&lt;&gt;"", 'Current Assessment'!A3, "")</f>
         <v>Person 2</v>
       </c>
       <c r="B3" s="12"/>
@@ -15502,7 +15430,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="str">
-        <f>IF(Input!A4&lt;&gt;"", Input!A4, "")</f>
+        <f>IF('Current Assessment'!A4&lt;&gt;"", 'Current Assessment'!A4, "")</f>
         <v>Team 1</v>
       </c>
       <c r="B4" s="12"/>
@@ -15528,7 +15456,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="str">
-        <f>IF(Input!A5&lt;&gt;"", Input!A5, "")</f>
+        <f>IF('Current Assessment'!A5&lt;&gt;"", 'Current Assessment'!A5, "")</f>
         <v/>
       </c>
       <c r="B5" s="12"/>
@@ -15554,7 +15482,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="str">
-        <f>IF(Input!A6&lt;&gt;"", Input!A6, "")</f>
+        <f>IF('Current Assessment'!A6&lt;&gt;"", 'Current Assessment'!A6, "")</f>
         <v/>
       </c>
       <c r="B6" s="12"/>
@@ -15580,7 +15508,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="str">
-        <f>IF(Input!A7&lt;&gt;"", Input!A7, "")</f>
+        <f>IF('Current Assessment'!A7&lt;&gt;"", 'Current Assessment'!A7, "")</f>
         <v/>
       </c>
       <c r="B7" s="12"/>
@@ -15606,7 +15534,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="str">
-        <f>IF(Input!A8&lt;&gt;"", Input!A8, "")</f>
+        <f>IF('Current Assessment'!A8&lt;&gt;"", 'Current Assessment'!A8, "")</f>
         <v/>
       </c>
       <c r="B8" s="12"/>
@@ -15632,7 +15560,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="str">
-        <f>IF(Input!A9&lt;&gt;"", Input!A9, "")</f>
+        <f>IF('Current Assessment'!A9&lt;&gt;"", 'Current Assessment'!A9, "")</f>
         <v/>
       </c>
       <c r="B9" s="12"/>
@@ -15658,7 +15586,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="str">
-        <f>IF(Input!A10&lt;&gt;"", Input!A10, "")</f>
+        <f>IF('Current Assessment'!A10&lt;&gt;"", 'Current Assessment'!A10, "")</f>
         <v/>
       </c>
       <c r="B10" s="12"/>
@@ -15684,7 +15612,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="str">
-        <f>IF(Input!A11&lt;&gt;"", Input!A11, "")</f>
+        <f>IF('Current Assessment'!A11&lt;&gt;"", 'Current Assessment'!A11, "")</f>
         <v/>
       </c>
       <c r="B11" s="12"/>
@@ -15710,7 +15638,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="str">
-        <f>IF(Input!A12&lt;&gt;"", Input!A12, "")</f>
+        <f>IF('Current Assessment'!A12&lt;&gt;"", 'Current Assessment'!A12, "")</f>
         <v/>
       </c>
       <c r="B12" s="12"/>
@@ -15736,7 +15664,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="str">
-        <f>IF(Input!A13&lt;&gt;"", Input!A13, "")</f>
+        <f>IF('Current Assessment'!A13&lt;&gt;"", 'Current Assessment'!A13, "")</f>
         <v/>
       </c>
       <c r="B13" s="12"/>
@@ -15762,7 +15690,7 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="e">
-        <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
+        <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
         <v>#REF!</v>
       </c>
       <c r="B14" s="12"/>
@@ -15788,7 +15716,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="e">
-        <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
+        <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
         <v>#REF!</v>
       </c>
       <c r="B15" s="12"/>
@@ -15814,7 +15742,7 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="e">
-        <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
+        <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
         <v>#REF!</v>
       </c>
       <c r="B16" s="12"/>
@@ -15840,7 +15768,7 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="e">
-        <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
+        <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
         <v>#REF!</v>
       </c>
       <c r="B17" s="12"/>
@@ -15866,7 +15794,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="e">
-        <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
+        <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
         <v>#REF!</v>
       </c>
       <c r="B18" s="12"/>
@@ -15892,7 +15820,7 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="e">
-        <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
+        <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
         <v>#REF!</v>
       </c>
       <c r="B19" s="12"/>
@@ -15918,7 +15846,7 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="e">
-        <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
+        <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
         <v>#REF!</v>
       </c>
       <c r="B20" s="12"/>
@@ -15944,7 +15872,7 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="e">
-        <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
+        <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
         <v>#REF!</v>
       </c>
       <c r="B21" s="12"/>
@@ -15970,7 +15898,7 @@
     </row>
     <row r="23" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -16143,7 +16071,7 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B26" s="7">
         <f>Willingness_Calcs!B2</f>
@@ -16228,7 +16156,7 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B27" s="7">
         <f>Willingness_Calcs!B3</f>
@@ -16356,9 +16284,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16375,7 +16302,7 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B1">
         <f>IF(B$4&lt;&gt;"",COUNTIF(B$5:B$24, "&gt;= 3"),"")</f>
@@ -16460,7 +16387,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <f>IF(B$4&lt;&gt;"",COUNTIF(B$5:B$24, "&gt;= 2"),"")</f>
@@ -16545,7 +16472,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <f>IF(B$4&lt;&gt;"",COUNTIF(B$5:B$24, "= 1"),"")</f>
@@ -16630,89 +16557,89 @@
     </row>
     <row r="4" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="str">
-        <f>IF(Input!B1&lt;&gt;"",Input!B1,"")</f>
+        <f>IF('Current Assessment'!B1&lt;&gt;"",'Current Assessment'!B1,"")</f>
         <v>CSS</v>
       </c>
       <c r="C4" s="9" t="str">
-        <f>IF(Input!C1&lt;&gt;"",Input!C1,"")</f>
+        <f>IF('Current Assessment'!C1&lt;&gt;"",'Current Assessment'!C1,"")</f>
         <v>Javascript</v>
       </c>
       <c r="D4" s="9" t="str">
-        <f>IF(Input!D1&lt;&gt;"",Input!D1,"")</f>
+        <f>IF('Current Assessment'!D1&lt;&gt;"",'Current Assessment'!D1,"")</f>
         <v>DB Backup/Restore</v>
       </c>
       <c r="E4" s="9" t="str">
-        <f>IF(Input!E1&lt;&gt;"",Input!E1,"")</f>
+        <f>IF('Current Assessment'!E1&lt;&gt;"",'Current Assessment'!E1,"")</f>
         <v/>
       </c>
       <c r="F4" s="9" t="str">
-        <f>IF(Input!F1&lt;&gt;"",Input!F1,"")</f>
+        <f>IF('Current Assessment'!F1&lt;&gt;"",'Current Assessment'!F1,"")</f>
         <v/>
       </c>
       <c r="G4" s="9" t="str">
-        <f>IF(Input!G1&lt;&gt;"",Input!G1,"")</f>
+        <f>IF('Current Assessment'!G1&lt;&gt;"",'Current Assessment'!G1,"")</f>
         <v/>
       </c>
       <c r="H4" s="9" t="str">
-        <f>IF(Input!H1&lt;&gt;"",Input!H1,"")</f>
+        <f>IF('Current Assessment'!H1&lt;&gt;"",'Current Assessment'!H1,"")</f>
         <v/>
       </c>
       <c r="I4" s="9" t="str">
-        <f>IF(Input!I1&lt;&gt;"",Input!I1,"")</f>
+        <f>IF('Current Assessment'!I1&lt;&gt;"",'Current Assessment'!I1,"")</f>
         <v/>
       </c>
       <c r="J4" s="9" t="str">
-        <f>IF(Input!J1&lt;&gt;"",Input!J1,"")</f>
+        <f>IF('Current Assessment'!J1&lt;&gt;"",'Current Assessment'!J1,"")</f>
         <v/>
       </c>
       <c r="K4" s="9" t="str">
-        <f>IF(Input!K1&lt;&gt;"",Input!K1,"")</f>
+        <f>IF('Current Assessment'!K1&lt;&gt;"",'Current Assessment'!K1,"")</f>
         <v/>
       </c>
       <c r="L4" s="9" t="str">
-        <f>IF(Input!L1&lt;&gt;"",Input!L1,"")</f>
+        <f>IF('Current Assessment'!L1&lt;&gt;"",'Current Assessment'!L1,"")</f>
         <v/>
       </c>
       <c r="M4" s="9" t="str">
-        <f>IF(Input!M1&lt;&gt;"",Input!M1,"")</f>
+        <f>IF('Current Assessment'!M1&lt;&gt;"",'Current Assessment'!M1,"")</f>
         <v/>
       </c>
       <c r="N4" s="9" t="str">
-        <f>IF(Input!N1&lt;&gt;"",Input!N1,"")</f>
+        <f>IF('Current Assessment'!N1&lt;&gt;"",'Current Assessment'!N1,"")</f>
         <v/>
       </c>
       <c r="O4" s="9" t="str">
-        <f>IF(Input!O1&lt;&gt;"",Input!O1,"")</f>
+        <f>IF('Current Assessment'!O1&lt;&gt;"",'Current Assessment'!O1,"")</f>
         <v/>
       </c>
       <c r="P4" s="9" t="str">
-        <f>IF(Input!P1&lt;&gt;"",Input!P1,"")</f>
+        <f>IF('Current Assessment'!P1&lt;&gt;"",'Current Assessment'!P1,"")</f>
         <v/>
       </c>
       <c r="Q4" s="9" t="str">
-        <f>IF(Input!Q1&lt;&gt;"",Input!Q1,"")</f>
+        <f>IF('Current Assessment'!Q1&lt;&gt;"",'Current Assessment'!Q1,"")</f>
         <v/>
       </c>
       <c r="R4" s="9" t="str">
-        <f>IF(Input!R1&lt;&gt;"",Input!R1,"")</f>
+        <f>IF('Current Assessment'!R1&lt;&gt;"",'Current Assessment'!R1,"")</f>
         <v/>
       </c>
       <c r="S4" s="9" t="e">
-        <f>IF(Input!#REF!&lt;&gt;"",Input!#REF!,"")</f>
+        <f>IF('Current Assessment'!#REF!&lt;&gt;"",'Current Assessment'!#REF!,"")</f>
         <v>#REF!</v>
       </c>
       <c r="T4" s="9" t="e">
-        <f>IF(Input!#REF!&lt;&gt;"",Input!#REF!,"")</f>
+        <f>IF('Current Assessment'!#REF!&lt;&gt;"",'Current Assessment'!#REF!,"")</f>
         <v>#REF!</v>
       </c>
       <c r="U4" s="9" t="e">
-        <f>IF(Input!#REF!&lt;&gt;"",Input!#REF!,"")</f>
+        <f>IF('Current Assessment'!#REF!&lt;&gt;"",'Current Assessment'!#REF!,"")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="str">
-        <f>Input!A2</f>
+        <f>'Current Assessment'!A2</f>
         <v>Person 1</v>
       </c>
       <c r="B5">
@@ -16798,7 +16725,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="str">
-        <f>Input!A3</f>
+        <f>'Current Assessment'!A3</f>
         <v>Person 2</v>
       </c>
       <c r="B6">
@@ -16884,7 +16811,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="str">
-        <f>Input!A4</f>
+        <f>'Current Assessment'!A4</f>
         <v>Team 1</v>
       </c>
       <c r="B7">
@@ -16970,7 +16897,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="str">
-        <f>Input!A5</f>
+        <f>'Current Assessment'!A5</f>
         <v/>
       </c>
       <c r="B8">
@@ -17056,7 +16983,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="str">
-        <f>Input!A6</f>
+        <f>'Current Assessment'!A6</f>
         <v/>
       </c>
       <c r="B9">
@@ -17142,7 +17069,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="str">
-        <f>Input!A7</f>
+        <f>'Current Assessment'!A7</f>
         <v/>
       </c>
       <c r="B10">
@@ -17228,7 +17155,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="str">
-        <f>Input!A8</f>
+        <f>'Current Assessment'!A8</f>
         <v/>
       </c>
       <c r="B11">
@@ -17314,7 +17241,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="str">
-        <f>Input!A9</f>
+        <f>'Current Assessment'!A9</f>
         <v/>
       </c>
       <c r="B12">
@@ -17400,7 +17327,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="str">
-        <f>Input!A10</f>
+        <f>'Current Assessment'!A10</f>
         <v/>
       </c>
       <c r="B13">
@@ -17486,7 +17413,7 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="str">
-        <f>Input!A11</f>
+        <f>'Current Assessment'!A11</f>
         <v/>
       </c>
       <c r="B14">
@@ -17572,7 +17499,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="str">
-        <f>Input!A12</f>
+        <f>'Current Assessment'!A12</f>
         <v/>
       </c>
       <c r="B15">
@@ -17658,7 +17585,7 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="str">
-        <f>Input!A13</f>
+        <f>'Current Assessment'!A13</f>
         <v/>
       </c>
       <c r="B16">
@@ -17744,7 +17671,7 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="e">
-        <f>Input!#REF!</f>
+        <f>'Current Assessment'!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B17">
@@ -17830,7 +17757,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="e">
-        <f>Input!#REF!</f>
+        <f>'Current Assessment'!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B18">
@@ -17916,7 +17843,7 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="e">
-        <f>Input!#REF!</f>
+        <f>'Current Assessment'!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B19">
@@ -18002,7 +17929,7 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="e">
-        <f>Input!#REF!</f>
+        <f>'Current Assessment'!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B20">
@@ -18088,7 +18015,7 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="e">
-        <f>Input!#REF!</f>
+        <f>'Current Assessment'!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B21">
@@ -18174,7 +18101,7 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="e">
-        <f>Input!#REF!</f>
+        <f>'Current Assessment'!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B22">
@@ -18260,7 +18187,7 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="e">
-        <f>Input!#REF!</f>
+        <f>'Current Assessment'!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B23">
@@ -18346,7 +18273,7 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="e">
-        <f>Input!#REF!</f>
+        <f>'Current Assessment'!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B24">

</xml_diff>

<commit_message>
Revert "Revert "Expanded version supporting 5000 samples rather than 1250""
This reverts commit 2a8b180e1479d258f796cc11b6f4ad6aa11a68e3.
</commit_message>
<xml_diff>
--- a/Spreadsheets/Capability Matrix.xlsx
+++ b/Spreadsheets/Capability Matrix.xlsx
@@ -1,35 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Troy\Dropbox\Private\GitHub\FocusedObjective.Resources\Spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Private\GitHub\FocusedObjective.Resources\Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="90" yWindow="75" windowWidth="19140" windowHeight="9525"/>
+    <workbookView xWindow="90" yWindow="765" windowWidth="19140" windowHeight="9525" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="6" r:id="rId1"/>
     <sheet name="Settings" sheetId="2" r:id="rId2"/>
     <sheet name="Survey Sheet" sheetId="5" r:id="rId3"/>
-    <sheet name="Current Assessment" sheetId="1" r:id="rId4"/>
-    <sheet name="Current_Calcs" sheetId="4" state="hidden" r:id="rId5"/>
-    <sheet name="Willingness" sheetId="3" state="hidden" r:id="rId6"/>
-    <sheet name="Willingness_Calcs" sheetId="7" state="hidden" r:id="rId7"/>
+    <sheet name="Input" sheetId="1" r:id="rId4"/>
+    <sheet name="Heatmap" sheetId="4" r:id="rId5"/>
+    <sheet name="Splitability" sheetId="8" r:id="rId6"/>
+    <sheet name="Willingness" sheetId="3" state="hidden" r:id="rId7"/>
+    <sheet name="Willingness_Calcs" sheetId="7" state="hidden" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="Skills_Header" localSheetId="6">Settings!#REF!</definedName>
+    <definedName name="Skills_Header" localSheetId="7">Settings!#REF!</definedName>
     <definedName name="Skills_Header">Settings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
   <si>
     <t>Willing</t>
   </si>
@@ -49,19 +50,10 @@
     <t>Person 1</t>
   </si>
   <si>
-    <t>Captains: Ability to Create (# &gt;= 3)</t>
-  </si>
-  <si>
-    <t>Players: Ability to Maintain (# &gt;= 2)</t>
-  </si>
-  <si>
     <t>Your Name:</t>
   </si>
   <si>
     <t>Analysis:</t>
-  </si>
-  <si>
-    <t>Bench: Ready to Train Up (# = 1)</t>
   </si>
   <si>
     <t>I'd quit rather than do this…</t>
@@ -101,9 +93,6 @@
   </si>
   <si>
     <t>Can start from nothing and create</t>
-  </si>
-  <si>
-    <t>Expert level</t>
   </si>
   <si>
     <t>For each capability choose from the list of CURRENT skill level values. If in doubt, err low (left)!</t>
@@ -148,19 +137,58 @@
     <t>Initial Version</t>
   </si>
   <si>
-    <t>Made all setting in the Setting tab.</t>
-  </si>
-  <si>
     <t>Staff and Team Capability Matrix</t>
   </si>
   <si>
     <t>Capability Survey For Printing (enter skills in the Settings worksheet)</t>
   </si>
+  <si>
+    <t>Quick Analysis:</t>
+  </si>
+  <si>
+    <t>Can teach others</t>
+  </si>
+  <si>
+    <t>Made all settings definable in the Setting tab.</t>
+  </si>
+  <si>
+    <t>no teacher</t>
+  </si>
+  <si>
+    <t>1 teacher</t>
+  </si>
+  <si>
+    <t>no doer</t>
+  </si>
+  <si>
+    <t>1 doer</t>
+  </si>
+  <si>
+    <t>no novice</t>
+  </si>
+  <si>
+    <t>1 novice</t>
+  </si>
+  <si>
+    <t>no doer. 1 Novice</t>
+  </si>
+  <si>
+    <t>teach novice into doer - URGENT</t>
+  </si>
+  <si>
+    <t>1 doer, 1 novice</t>
+  </si>
+  <si>
+    <t>teach novice into doer - SOON</t>
+  </si>
+  <si>
+    <t>hire teacher level or  external consultant. Create doers, then train one into teacher</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -287,7 +315,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -378,6 +406,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -388,7 +427,7 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -442,6 +481,8 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -11868,7 +11909,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>Novice &amp; LEarner (bench)</a:t>
+            <a:t>Novice &amp; Learner (bench)</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
@@ -11975,75 +12016,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>527685</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>32385</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>59055</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4013835" y="1556385"/>
-          <a:ext cx="6846570" cy="1386840"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFF00"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2400" b="1"/>
-            <a:t>Do not edit this sheet directly. This is the formulas for converting and counting current capability. If you want to add people, do it in the current tab. </a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
       <xdr:colOff>1150620</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
@@ -12116,7 +12088,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -12472,34 +12444,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:Q23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
+      <c r="B1" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
     </row>
     <row r="2" spans="2:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="P2" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
@@ -12507,7 +12480,7 @@
         <v>1</v>
       </c>
       <c r="Q4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
@@ -12583,10 +12556,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="B5:K22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12606,18 +12580,18 @@
   <sheetData>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="K5" s="2"/>
     </row>
@@ -12629,45 +12603,45 @@
         <v>3</v>
       </c>
       <c r="G6" s="25" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I6" s="25" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D7" s="25" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I7" s="25" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I8" s="25" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="26"/>
       <c r="D9" s="25"/>
       <c r="G9" s="25" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I9" s="25" t="s">
         <v>1</v>
@@ -12677,7 +12651,7 @@
       <c r="B10" s="26"/>
       <c r="D10" s="25"/>
       <c r="G10" s="25" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="I10" s="25" t="s">
         <v>2</v>
@@ -12735,10 +12709,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12752,31 +12727,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
+      <c r="A1" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:6" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="20" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -12801,12 +12776,12 @@
       </c>
       <c r="F7" s="23" t="str">
         <f>Settings!$G$10</f>
-        <v>Expert level</v>
+        <v>Can teach others</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="str">
-        <f>IF('Current Assessment'!B1&lt;&gt;"", 'Current Assessment'!B1, "")</f>
+        <f>IF(Input!B1&lt;&gt;"", Input!B1, "")</f>
         <v>CSS</v>
       </c>
       <c r="B8" s="17"/>
@@ -12817,7 +12792,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="str">
-        <f>IF('Current Assessment'!C1&lt;&gt;"", 'Current Assessment'!C1, "")</f>
+        <f>IF(Input!C1&lt;&gt;"", Input!C1, "")</f>
         <v>Javascript</v>
       </c>
       <c r="B9" s="17"/>
@@ -12828,7 +12803,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="str">
-        <f>IF('Current Assessment'!D1&lt;&gt;"", 'Current Assessment'!D1, "")</f>
+        <f>IF(Input!D1&lt;&gt;"", Input!D1, "")</f>
         <v>DB Backup/Restore</v>
       </c>
       <c r="B10" s="17"/>
@@ -12839,7 +12814,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="str">
-        <f>IF('Current Assessment'!E1&lt;&gt;"", 'Current Assessment'!E1, "")</f>
+        <f>IF(Input!E1&lt;&gt;"", Input!E1, "")</f>
         <v/>
       </c>
       <c r="B11" s="17"/>
@@ -12850,7 +12825,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="str">
-        <f>IF('Current Assessment'!F1&lt;&gt;"", 'Current Assessment'!F1, "")</f>
+        <f>IF(Input!F1&lt;&gt;"", Input!F1, "")</f>
         <v/>
       </c>
       <c r="B12" s="17"/>
@@ -12861,7 +12836,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="str">
-        <f>IF('Current Assessment'!G1&lt;&gt;"", 'Current Assessment'!G1, "")</f>
+        <f>IF(Input!G1&lt;&gt;"", Input!G1, "")</f>
         <v/>
       </c>
       <c r="B13" s="17"/>
@@ -12872,7 +12847,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="str">
-        <f>IF('Current Assessment'!H1&lt;&gt;"", 'Current Assessment'!H1, "")</f>
+        <f>IF(Input!H1&lt;&gt;"", Input!H1, "")</f>
         <v/>
       </c>
       <c r="B14" s="17"/>
@@ -12883,7 +12858,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="str">
-        <f>IF('Current Assessment'!I1&lt;&gt;"", 'Current Assessment'!I1, "")</f>
+        <f>IF(Input!I1&lt;&gt;"", Input!I1, "")</f>
         <v/>
       </c>
       <c r="B15" s="17"/>
@@ -12894,7 +12869,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="str">
-        <f>IF('Current Assessment'!J1&lt;&gt;"", 'Current Assessment'!J1, "")</f>
+        <f>IF(Input!J1&lt;&gt;"", Input!J1, "")</f>
         <v/>
       </c>
       <c r="B16" s="17"/>
@@ -12905,7 +12880,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="str">
-        <f>IF('Current Assessment'!K1&lt;&gt;"", 'Current Assessment'!K1, "")</f>
+        <f>IF(Input!K1&lt;&gt;"", Input!K1, "")</f>
         <v/>
       </c>
       <c r="B17" s="17"/>
@@ -12916,7 +12891,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="str">
-        <f>IF('Current Assessment'!L1&lt;&gt;"", 'Current Assessment'!L1, "")</f>
+        <f>IF(Input!L1&lt;&gt;"", Input!L1, "")</f>
         <v/>
       </c>
       <c r="B18" s="17"/>
@@ -12927,7 +12902,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="str">
-        <f>IF('Current Assessment'!M1&lt;&gt;"", 'Current Assessment'!M1, "")</f>
+        <f>IF(Input!M1&lt;&gt;"", Input!M1, "")</f>
         <v/>
       </c>
       <c r="B19" s="17"/>
@@ -12938,7 +12913,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="str">
-        <f>IF('Current Assessment'!N1&lt;&gt;"", 'Current Assessment'!N1, "")</f>
+        <f>IF(Input!N1&lt;&gt;"", Input!N1, "")</f>
         <v/>
       </c>
       <c r="B20" s="17"/>
@@ -12949,7 +12924,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="str">
-        <f>IF('Current Assessment'!O1&lt;&gt;"", 'Current Assessment'!O1, "")</f>
+        <f>IF(Input!O1&lt;&gt;"", Input!O1, "")</f>
         <v/>
       </c>
       <c r="B21" s="17"/>
@@ -12960,7 +12935,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="str">
-        <f>IF('Current Assessment'!P1&lt;&gt;"", 'Current Assessment'!P1, "")</f>
+        <f>IF(Input!P1&lt;&gt;"", Input!P1, "")</f>
         <v/>
       </c>
       <c r="B22" s="17"/>
@@ -12971,7 +12946,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="str">
-        <f>IF('Current Assessment'!Q1&lt;&gt;"", 'Current Assessment'!Q1, "")</f>
+        <f>IF(Input!Q1&lt;&gt;"", Input!Q1, "")</f>
         <v/>
       </c>
       <c r="B23" s="17"/>
@@ -12982,7 +12957,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="str">
-        <f>IF('Current Assessment'!R1&lt;&gt;"", 'Current Assessment'!R1, "")</f>
+        <f>IF(Input!R1&lt;&gt;"", Input!R1, "")</f>
         <v/>
       </c>
       <c r="B24" s="17"/>
@@ -12993,7 +12968,7 @@
     </row>
     <row r="25" spans="1:6" ht="31.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -13021,7 +12996,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="str">
-        <f>IF('Current Assessment'!B16&lt;&gt;"", 'Current Assessment'!B16, "")</f>
+        <f>IF(Input!B16&lt;&gt;"", Input!B16, "")</f>
         <v>CSS</v>
       </c>
       <c r="B28" s="17"/>
@@ -13032,7 +13007,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="str">
-        <f>IF('Current Assessment'!C16&lt;&gt;"", 'Current Assessment'!C16, "")</f>
+        <f>IF(Input!C16&lt;&gt;"", Input!C16, "")</f>
         <v>Javascript</v>
       </c>
       <c r="B29" s="17"/>
@@ -13043,7 +13018,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="16" t="str">
-        <f>IF('Current Assessment'!D16&lt;&gt;"", 'Current Assessment'!D16, "")</f>
+        <f>IF(Input!D16&lt;&gt;"", Input!D16, "")</f>
         <v>DB Backup/Restore</v>
       </c>
       <c r="B30" s="17"/>
@@ -13054,7 +13029,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="str">
-        <f>IF('Current Assessment'!E16&lt;&gt;"", 'Current Assessment'!E16, "")</f>
+        <f>IF(Input!E16&lt;&gt;"", Input!E16, "")</f>
         <v/>
       </c>
       <c r="B31" s="17"/>
@@ -13065,7 +13040,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="16" t="str">
-        <f>IF('Current Assessment'!F16&lt;&gt;"", 'Current Assessment'!F16, "")</f>
+        <f>IF(Input!F16&lt;&gt;"", Input!F16, "")</f>
         <v/>
       </c>
       <c r="B32" s="17"/>
@@ -13076,7 +13051,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="16" t="str">
-        <f>IF('Current Assessment'!G16&lt;&gt;"", 'Current Assessment'!G16, "")</f>
+        <f>IF(Input!G16&lt;&gt;"", Input!G16, "")</f>
         <v/>
       </c>
       <c r="B33" s="17"/>
@@ -13087,7 +13062,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="str">
-        <f>IF('Current Assessment'!H16&lt;&gt;"", 'Current Assessment'!H16, "")</f>
+        <f>IF(Input!H16&lt;&gt;"", Input!H16, "")</f>
         <v/>
       </c>
       <c r="B34" s="17"/>
@@ -13098,7 +13073,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="16" t="str">
-        <f>IF('Current Assessment'!I16&lt;&gt;"", 'Current Assessment'!I16, "")</f>
+        <f>IF(Input!I16&lt;&gt;"", Input!I16, "")</f>
         <v/>
       </c>
       <c r="B35" s="17"/>
@@ -13109,7 +13084,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="16" t="str">
-        <f>IF('Current Assessment'!J16&lt;&gt;"", 'Current Assessment'!J16, "")</f>
+        <f>IF(Input!J16&lt;&gt;"", Input!J16, "")</f>
         <v/>
       </c>
       <c r="B36" s="17"/>
@@ -13120,7 +13095,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="16" t="str">
-        <f>IF('Current Assessment'!K16&lt;&gt;"", 'Current Assessment'!K16, "")</f>
+        <f>IF(Input!K16&lt;&gt;"", Input!K16, "")</f>
         <v/>
       </c>
       <c r="B37" s="17"/>
@@ -13131,7 +13106,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="16" t="str">
-        <f>IF('Current Assessment'!L16&lt;&gt;"", 'Current Assessment'!L16, "")</f>
+        <f>IF(Input!L16&lt;&gt;"", Input!L16, "")</f>
         <v/>
       </c>
       <c r="B38" s="17"/>
@@ -13142,7 +13117,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="16" t="str">
-        <f>IF('Current Assessment'!M16&lt;&gt;"", 'Current Assessment'!M16, "")</f>
+        <f>IF(Input!M16&lt;&gt;"", Input!M16, "")</f>
         <v/>
       </c>
       <c r="B39" s="17"/>
@@ -13153,7 +13128,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="16" t="str">
-        <f>IF('Current Assessment'!N16&lt;&gt;"", 'Current Assessment'!N16, "")</f>
+        <f>IF(Input!N16&lt;&gt;"", Input!N16, "")</f>
         <v/>
       </c>
       <c r="B40" s="17"/>
@@ -13164,7 +13139,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="16" t="str">
-        <f>IF('Current Assessment'!O16&lt;&gt;"", 'Current Assessment'!O16, "")</f>
+        <f>IF(Input!O16&lt;&gt;"", Input!O16, "")</f>
         <v/>
       </c>
       <c r="B41" s="17"/>
@@ -13175,7 +13150,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="16" t="str">
-        <f>IF('Current Assessment'!P16&lt;&gt;"", 'Current Assessment'!P16, "")</f>
+        <f>IF(Input!P16&lt;&gt;"", Input!P16, "")</f>
         <v/>
       </c>
       <c r="B42" s="17"/>
@@ -13186,7 +13161,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="16" t="str">
-        <f>IF('Current Assessment'!Q16&lt;&gt;"", 'Current Assessment'!Q16, "")</f>
+        <f>IF(Input!Q16&lt;&gt;"", Input!Q16, "")</f>
         <v/>
       </c>
       <c r="B43" s="17"/>
@@ -13197,7 +13172,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="16" t="str">
-        <f>IF('Current Assessment'!R16&lt;&gt;"", 'Current Assessment'!R16, "")</f>
+        <f>IF(Input!R16&lt;&gt;"", Input!R16, "")</f>
         <v/>
       </c>
       <c r="B44" s="17"/>
@@ -13222,10 +13197,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R19"/>
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13313,13 +13289,13 @@
         <v>Person 1</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E2" s="25"/>
       <c r="F2" s="25"/>
@@ -13342,13 +13318,13 @@
         <v>Person 2</v>
       </c>
       <c r="B3" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="25" t="s">
-        <v>23</v>
-      </c>
       <c r="D3" s="25" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
@@ -13371,13 +13347,13 @@
         <v>Team 1</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C4" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="25" t="s">
         <v>20</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>23</v>
       </c>
       <c r="E4" s="25"/>
       <c r="F4" s="25"/>
@@ -13604,7 +13580,7 @@
     <row r="14" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -13680,221 +13656,287 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B17" s="28">
-        <f>Current_Calcs!B1</f>
+        <f>Heatmap!B1</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="28">
+        <f>Heatmap!C1</f>
         <v>1</v>
       </c>
-      <c r="C17" s="28">
-        <f>Current_Calcs!C1</f>
+      <c r="D17" s="28">
+        <f>Heatmap!D1</f>
         <v>1</v>
       </c>
-      <c r="D17" s="28">
-        <f>Current_Calcs!D1</f>
-        <v>1</v>
-      </c>
       <c r="E17" s="28" t="str">
-        <f>Current_Calcs!E1</f>
+        <f>Heatmap!E1</f>
         <v/>
       </c>
       <c r="F17" s="29" t="str">
-        <f>Current_Calcs!F1</f>
+        <f>Heatmap!F1</f>
         <v/>
       </c>
       <c r="G17" s="29" t="str">
-        <f>Current_Calcs!G1</f>
+        <f>Heatmap!G1</f>
         <v/>
       </c>
       <c r="H17" s="29" t="str">
-        <f>Current_Calcs!H1</f>
+        <f>Heatmap!H1</f>
         <v/>
       </c>
       <c r="I17" s="29" t="str">
-        <f>Current_Calcs!I1</f>
+        <f>Heatmap!I1</f>
         <v/>
       </c>
       <c r="J17" s="29" t="str">
-        <f>Current_Calcs!J1</f>
+        <f>Heatmap!J1</f>
         <v/>
       </c>
       <c r="K17" s="29" t="str">
-        <f>Current_Calcs!K1</f>
+        <f>Heatmap!K1</f>
         <v/>
       </c>
       <c r="L17" s="29" t="str">
-        <f>Current_Calcs!L1</f>
+        <f>Heatmap!L1</f>
         <v/>
       </c>
       <c r="M17" s="29" t="str">
-        <f>Current_Calcs!M1</f>
+        <f>Heatmap!M1</f>
         <v/>
       </c>
       <c r="N17" s="29" t="str">
-        <f>Current_Calcs!N1</f>
+        <f>Heatmap!N1</f>
         <v/>
       </c>
       <c r="O17" s="29" t="str">
-        <f>Current_Calcs!O1</f>
+        <f>Heatmap!O1</f>
         <v/>
       </c>
       <c r="P17" s="29" t="str">
-        <f>Current_Calcs!P1</f>
+        <f>Heatmap!P1</f>
         <v/>
       </c>
       <c r="Q17" s="29" t="str">
-        <f>Current_Calcs!Q1</f>
+        <f>Heatmap!Q1</f>
         <v/>
       </c>
       <c r="R17" s="29" t="str">
-        <f>Current_Calcs!R1</f>
+        <f>Heatmap!R1</f>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B18" s="28">
-        <f>Current_Calcs!B2</f>
+        <f>Heatmap!B2</f>
         <v>1</v>
       </c>
       <c r="C18" s="28">
-        <f>Current_Calcs!C2</f>
+        <f>Heatmap!C2</f>
         <v>1</v>
       </c>
       <c r="D18" s="28">
-        <f>Current_Calcs!D2</f>
+        <f>Heatmap!D2</f>
         <v>2</v>
       </c>
       <c r="E18" s="28" t="str">
-        <f>Current_Calcs!E2</f>
+        <f>Heatmap!E2</f>
         <v/>
       </c>
       <c r="F18" s="29" t="str">
-        <f>Current_Calcs!F2</f>
+        <f>Heatmap!F2</f>
         <v/>
       </c>
       <c r="G18" s="29" t="str">
-        <f>Current_Calcs!G2</f>
+        <f>Heatmap!G2</f>
         <v/>
       </c>
       <c r="H18" s="29" t="str">
-        <f>Current_Calcs!H2</f>
+        <f>Heatmap!H2</f>
         <v/>
       </c>
       <c r="I18" s="29" t="str">
-        <f>Current_Calcs!I2</f>
+        <f>Heatmap!I2</f>
         <v/>
       </c>
       <c r="J18" s="29" t="str">
-        <f>Current_Calcs!J2</f>
+        <f>Heatmap!J2</f>
         <v/>
       </c>
       <c r="K18" s="29" t="str">
-        <f>Current_Calcs!K2</f>
+        <f>Heatmap!K2</f>
         <v/>
       </c>
       <c r="L18" s="29" t="str">
-        <f>Current_Calcs!L2</f>
+        <f>Heatmap!L2</f>
         <v/>
       </c>
       <c r="M18" s="29" t="str">
-        <f>Current_Calcs!M2</f>
+        <f>Heatmap!M2</f>
         <v/>
       </c>
       <c r="N18" s="29" t="str">
-        <f>Current_Calcs!N2</f>
+        <f>Heatmap!N2</f>
         <v/>
       </c>
       <c r="O18" s="29" t="str">
-        <f>Current_Calcs!O2</f>
+        <f>Heatmap!O2</f>
         <v/>
       </c>
       <c r="P18" s="29" t="str">
-        <f>Current_Calcs!P2</f>
+        <f>Heatmap!P2</f>
         <v/>
       </c>
       <c r="Q18" s="29" t="str">
-        <f>Current_Calcs!Q2</f>
+        <f>Heatmap!Q2</f>
         <v/>
       </c>
       <c r="R18" s="29" t="str">
-        <f>Current_Calcs!R2</f>
+        <f>Heatmap!R2</f>
         <v/>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="33" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B19" s="28">
-        <f>Current_Calcs!B3</f>
+        <f>Heatmap!B3</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="28">
+        <f>Heatmap!C3</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="28">
+        <f>Heatmap!D3</f>
         <v>1</v>
       </c>
-      <c r="C19" s="28">
-        <f>Current_Calcs!C3</f>
-        <v>0</v>
-      </c>
-      <c r="D19" s="28">
-        <f>Current_Calcs!D3</f>
+      <c r="E19" s="28" t="str">
+        <f>Heatmap!E3</f>
+        <v/>
+      </c>
+      <c r="F19" s="29" t="str">
+        <f>Heatmap!F3</f>
+        <v/>
+      </c>
+      <c r="G19" s="29" t="str">
+        <f>Heatmap!G3</f>
+        <v/>
+      </c>
+      <c r="H19" s="29" t="str">
+        <f>Heatmap!H3</f>
+        <v/>
+      </c>
+      <c r="I19" s="29" t="str">
+        <f>Heatmap!I3</f>
+        <v/>
+      </c>
+      <c r="J19" s="29" t="str">
+        <f>Heatmap!J3</f>
+        <v/>
+      </c>
+      <c r="K19" s="29" t="str">
+        <f>Heatmap!K3</f>
+        <v/>
+      </c>
+      <c r="L19" s="29" t="str">
+        <f>Heatmap!L3</f>
+        <v/>
+      </c>
+      <c r="M19" s="29" t="str">
+        <f>Heatmap!M3</f>
+        <v/>
+      </c>
+      <c r="N19" s="29" t="str">
+        <f>Heatmap!N3</f>
+        <v/>
+      </c>
+      <c r="O19" s="29" t="str">
+        <f>Heatmap!O3</f>
+        <v/>
+      </c>
+      <c r="P19" s="29" t="str">
+        <f>Heatmap!P3</f>
+        <v/>
+      </c>
+      <c r="Q19" s="29" t="str">
+        <f>Heatmap!Q3</f>
+        <v/>
+      </c>
+      <c r="R19" s="29" t="str">
+        <f>Heatmap!R3</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30">
         <v>1</v>
       </c>
-      <c r="E19" s="28" t="str">
-        <f>Current_Calcs!E3</f>
-        <v/>
-      </c>
-      <c r="F19" s="29" t="str">
-        <f>Current_Calcs!F3</f>
-        <v/>
-      </c>
-      <c r="G19" s="29" t="str">
-        <f>Current_Calcs!G3</f>
-        <v/>
-      </c>
-      <c r="H19" s="29" t="str">
-        <f>Current_Calcs!H3</f>
-        <v/>
-      </c>
-      <c r="I19" s="29" t="str">
-        <f>Current_Calcs!I3</f>
-        <v/>
-      </c>
-      <c r="J19" s="29" t="str">
-        <f>Current_Calcs!J3</f>
-        <v/>
-      </c>
-      <c r="K19" s="29" t="str">
-        <f>Current_Calcs!K3</f>
-        <v/>
-      </c>
-      <c r="L19" s="29" t="str">
-        <f>Current_Calcs!L3</f>
-        <v/>
-      </c>
-      <c r="M19" s="29" t="str">
-        <f>Current_Calcs!M3</f>
-        <v/>
-      </c>
-      <c r="N19" s="29" t="str">
-        <f>Current_Calcs!N3</f>
-        <v/>
-      </c>
-      <c r="O19" s="29" t="str">
-        <f>Current_Calcs!O3</f>
-        <v/>
-      </c>
-      <c r="P19" s="29" t="str">
-        <f>Current_Calcs!P3</f>
-        <v/>
-      </c>
-      <c r="Q19" s="29" t="str">
-        <f>Current_Calcs!Q3</f>
-        <v/>
-      </c>
-      <c r="R19" s="29" t="str">
-        <f>Current_Calcs!R3</f>
-        <v/>
+      <c r="D30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -13948,24 +13990,28 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R21"/>
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="B1">
-        <f t="shared" ref="B1:R1" si="0">IF(B$4&lt;&gt;"",COUNTIF(B$5:B$16, "&gt;= 3"),"")</f>
-        <v>1</v>
+        <f t="shared" ref="B1:R1" si="0">IF(B$5&lt;&gt;"",COUNTIF(B$6:B$17, "&gt;= 3"),"")</f>
+        <v>0</v>
       </c>
       <c r="C1">
         <f t="shared" si="0"/>
@@ -14034,10 +14080,10 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:R2" si="1">IF(B$4&lt;&gt;"",COUNTIF(B$5:B$16, "&gt;= 2"),"")</f>
+        <f t="shared" ref="B2:R2" si="1">IF(B$5&lt;&gt;"",COUNTIF(B$6:B$17, "&gt;= 2"),"")</f>
         <v>1</v>
       </c>
       <c r="C2">
@@ -14107,11 +14153,11 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:R3" si="2">IF(B$4&lt;&gt;"",COUNTIF(B$5:B$16, "= 1"),"")</f>
-        <v>1</v>
+        <f t="shared" ref="B3:R3" si="2">IF(B$5&lt;&gt;"",COUNTIF(B$6:B$17, "= 1"),"")</f>
+        <v>0</v>
       </c>
       <c r="C3">
         <f t="shared" si="2"/>
@@ -14178,1048 +14224,1051 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="str">
-        <f>IF('Current Assessment'!B1&lt;&gt;"",'Current Assessment'!B1,"")</f>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:18" s="35" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="36" t="str">
+        <f>IF(Input!B1&lt;&gt;"",Input!B1,"")</f>
         <v>CSS</v>
       </c>
-      <c r="C4" s="9" t="str">
-        <f>IF('Current Assessment'!C1&lt;&gt;"",'Current Assessment'!C1,"")</f>
+      <c r="C5" s="36" t="str">
+        <f>IF(Input!C1&lt;&gt;"",Input!C1,"")</f>
         <v>Javascript</v>
       </c>
-      <c r="D4" s="9" t="str">
-        <f>IF('Current Assessment'!D1&lt;&gt;"",'Current Assessment'!D1,"")</f>
+      <c r="D5" s="36" t="str">
+        <f>IF(Input!D1&lt;&gt;"",Input!D1,"")</f>
         <v>DB Backup/Restore</v>
       </c>
-      <c r="E4" s="9" t="str">
-        <f>IF('Current Assessment'!E1&lt;&gt;"",'Current Assessment'!E1,"")</f>
-        <v/>
-      </c>
-      <c r="F4" s="9" t="str">
-        <f>IF('Current Assessment'!F1&lt;&gt;"",'Current Assessment'!F1,"")</f>
-        <v/>
-      </c>
-      <c r="G4" s="9" t="str">
-        <f>IF('Current Assessment'!G1&lt;&gt;"",'Current Assessment'!G1,"")</f>
-        <v/>
-      </c>
-      <c r="H4" s="9" t="str">
-        <f>IF('Current Assessment'!H1&lt;&gt;"",'Current Assessment'!H1,"")</f>
-        <v/>
-      </c>
-      <c r="I4" s="9" t="str">
-        <f>IF('Current Assessment'!I1&lt;&gt;"",'Current Assessment'!I1,"")</f>
-        <v/>
-      </c>
-      <c r="J4" s="9" t="str">
-        <f>IF('Current Assessment'!J1&lt;&gt;"",'Current Assessment'!J1,"")</f>
-        <v/>
-      </c>
-      <c r="K4" s="9" t="str">
-        <f>IF('Current Assessment'!K1&lt;&gt;"",'Current Assessment'!K1,"")</f>
-        <v/>
-      </c>
-      <c r="L4" s="9" t="str">
-        <f>IF('Current Assessment'!L1&lt;&gt;"",'Current Assessment'!L1,"")</f>
-        <v/>
-      </c>
-      <c r="M4" s="9" t="str">
-        <f>IF('Current Assessment'!M1&lt;&gt;"",'Current Assessment'!M1,"")</f>
-        <v/>
-      </c>
-      <c r="N4" s="9" t="str">
-        <f>IF('Current Assessment'!N1&lt;&gt;"",'Current Assessment'!N1,"")</f>
-        <v/>
-      </c>
-      <c r="O4" s="9" t="str">
-        <f>IF('Current Assessment'!O1&lt;&gt;"",'Current Assessment'!O1,"")</f>
-        <v/>
-      </c>
-      <c r="P4" s="9" t="str">
-        <f>IF('Current Assessment'!P1&lt;&gt;"",'Current Assessment'!P1,"")</f>
-        <v/>
-      </c>
-      <c r="Q4" s="9" t="str">
-        <f>IF('Current Assessment'!Q1&lt;&gt;"",'Current Assessment'!Q1,"")</f>
-        <v/>
-      </c>
-      <c r="R4" s="9" t="str">
-        <f>IF('Current Assessment'!R1&lt;&gt;"",'Current Assessment'!R1,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="str">
-        <f>'Current Assessment'!A2</f>
-        <v>Person 1</v>
-      </c>
-      <c r="B5">
-        <f>IFERROR(MATCH('Current Assessment'!B2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <f>IFERROR(MATCH('Current Assessment'!C2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <f>IFERROR(MATCH('Current Assessment'!D2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <f>IFERROR(MATCH('Current Assessment'!E2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <f>IFERROR(MATCH('Current Assessment'!F2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <f>IFERROR(MATCH('Current Assessment'!G2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <f>IFERROR(MATCH('Current Assessment'!H2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <f>IFERROR(MATCH('Current Assessment'!I2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <f>IFERROR(MATCH('Current Assessment'!J2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <f>IFERROR(MATCH('Current Assessment'!K2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <f>IFERROR(MATCH('Current Assessment'!L2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <f>IFERROR(MATCH('Current Assessment'!M2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <f>IFERROR(MATCH('Current Assessment'!N2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <f>IFERROR(MATCH('Current Assessment'!O2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <f>IFERROR(MATCH('Current Assessment'!P2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <f>IFERROR(MATCH('Current Assessment'!Q2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <f>IFERROR(MATCH('Current Assessment'!R2,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
+      <c r="E5" s="36" t="str">
+        <f>IF(Input!E1&lt;&gt;"",Input!E1,"")</f>
+        <v/>
+      </c>
+      <c r="F5" s="36" t="str">
+        <f>IF(Input!F1&lt;&gt;"",Input!F1,"")</f>
+        <v/>
+      </c>
+      <c r="G5" s="36" t="str">
+        <f>IF(Input!G1&lt;&gt;"",Input!G1,"")</f>
+        <v/>
+      </c>
+      <c r="H5" s="36" t="str">
+        <f>IF(Input!H1&lt;&gt;"",Input!H1,"")</f>
+        <v/>
+      </c>
+      <c r="I5" s="36" t="str">
+        <f>IF(Input!I1&lt;&gt;"",Input!I1,"")</f>
+        <v/>
+      </c>
+      <c r="J5" s="36" t="str">
+        <f>IF(Input!J1&lt;&gt;"",Input!J1,"")</f>
+        <v/>
+      </c>
+      <c r="K5" s="36" t="str">
+        <f>IF(Input!K1&lt;&gt;"",Input!K1,"")</f>
+        <v/>
+      </c>
+      <c r="L5" s="36" t="str">
+        <f>IF(Input!L1&lt;&gt;"",Input!L1,"")</f>
+        <v/>
+      </c>
+      <c r="M5" s="36" t="str">
+        <f>IF(Input!M1&lt;&gt;"",Input!M1,"")</f>
+        <v/>
+      </c>
+      <c r="N5" s="36" t="str">
+        <f>IF(Input!N1&lt;&gt;"",Input!N1,"")</f>
+        <v/>
+      </c>
+      <c r="O5" s="36" t="str">
+        <f>IF(Input!O1&lt;&gt;"",Input!O1,"")</f>
+        <v/>
+      </c>
+      <c r="P5" s="36" t="str">
+        <f>IF(Input!P1&lt;&gt;"",Input!P1,"")</f>
+        <v/>
+      </c>
+      <c r="Q5" s="36" t="str">
+        <f>IF(Input!Q1&lt;&gt;"",Input!Q1,"")</f>
+        <v/>
+      </c>
+      <c r="R5" s="36" t="str">
+        <f>IF(Input!R1&lt;&gt;"",Input!R1,"")</f>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="str">
-        <f>'Current Assessment'!A3</f>
-        <v>Person 2</v>
+        <f>Input!A2</f>
+        <v>Person 1</v>
       </c>
       <c r="B6">
-        <f>IFERROR(MATCH('Current Assessment'!B3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!B2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="C6">
-        <f>IFERROR(MATCH('Current Assessment'!C3,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>3</v>
+        <f>IFERROR(MATCH(Input!C2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
       </c>
       <c r="D6">
-        <f>IFERROR(MATCH('Current Assessment'!D3,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>2</v>
+        <f>IFERROR(MATCH(Input!D2,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>1</v>
       </c>
       <c r="E6">
-        <f>IFERROR(MATCH('Current Assessment'!E3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!E2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F6">
-        <f>IFERROR(MATCH('Current Assessment'!F3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!F2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G6">
-        <f>IFERROR(MATCH('Current Assessment'!G3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!G2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H6">
-        <f>IFERROR(MATCH('Current Assessment'!H3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!H2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I6">
-        <f>IFERROR(MATCH('Current Assessment'!I3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!I2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J6">
-        <f>IFERROR(MATCH('Current Assessment'!J3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!J2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K6">
-        <f>IFERROR(MATCH('Current Assessment'!K3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!K2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L6">
-        <f>IFERROR(MATCH('Current Assessment'!L3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!L2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M6">
-        <f>IFERROR(MATCH('Current Assessment'!M3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!M2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N6">
-        <f>IFERROR(MATCH('Current Assessment'!N3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!N2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O6">
-        <f>IFERROR(MATCH('Current Assessment'!O3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!O2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P6">
-        <f>IFERROR(MATCH('Current Assessment'!P3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!P2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q6">
-        <f>IFERROR(MATCH('Current Assessment'!Q3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!Q2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R6">
-        <f>IFERROR(MATCH('Current Assessment'!R3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!R2,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="str">
-        <f>'Current Assessment'!A4</f>
-        <v>Team 1</v>
+        <f>Input!A3</f>
+        <v>Person 2</v>
       </c>
       <c r="B7">
-        <f>IFERROR(MATCH('Current Assessment'!B4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!B3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <f>IFERROR(MATCH(Input!C3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>3</v>
       </c>
-      <c r="C7">
-        <f>IFERROR(MATCH('Current Assessment'!C4,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
-      </c>
       <c r="D7">
-        <f>IFERROR(MATCH('Current Assessment'!D4,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>3</v>
+        <f>IFERROR(MATCH(Input!D3,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>2</v>
       </c>
       <c r="E7">
-        <f>IFERROR(MATCH('Current Assessment'!E4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!E3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F7">
-        <f>IFERROR(MATCH('Current Assessment'!F4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!F3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G7">
-        <f>IFERROR(MATCH('Current Assessment'!G4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!G3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H7">
-        <f>IFERROR(MATCH('Current Assessment'!H4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!H3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I7">
-        <f>IFERROR(MATCH('Current Assessment'!I4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!I3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J7">
-        <f>IFERROR(MATCH('Current Assessment'!J4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!J3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K7">
-        <f>IFERROR(MATCH('Current Assessment'!K4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!K3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L7">
-        <f>IFERROR(MATCH('Current Assessment'!L4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!L3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M7">
-        <f>IFERROR(MATCH('Current Assessment'!M4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!M3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N7">
-        <f>IFERROR(MATCH('Current Assessment'!N4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!N3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O7">
-        <f>IFERROR(MATCH('Current Assessment'!O4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!O3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P7">
-        <f>IFERROR(MATCH('Current Assessment'!P4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!P3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q7">
-        <f>IFERROR(MATCH('Current Assessment'!Q4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!Q3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R7">
-        <f>IFERROR(MATCH('Current Assessment'!R4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!R3,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="str">
-        <f>'Current Assessment'!A5</f>
-        <v/>
+        <f>Input!A4</f>
+        <v>Team 1</v>
       </c>
       <c r="B8">
-        <f>IFERROR(MATCH('Current Assessment'!B5,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
+        <f>IFERROR(MATCH(Input!B4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>2</v>
       </c>
       <c r="C8">
-        <f>IFERROR(MATCH('Current Assessment'!C5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!C4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="D8">
-        <f>IFERROR(MATCH('Current Assessment'!D5,Settings!$G$6:$G$10,0)-1, 0)</f>
-        <v>0</v>
+        <f>IFERROR(MATCH(Input!D4,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>3</v>
       </c>
       <c r="E8">
-        <f>IFERROR(MATCH('Current Assessment'!E5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!E4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F8">
-        <f>IFERROR(MATCH('Current Assessment'!F5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!F4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G8">
-        <f>IFERROR(MATCH('Current Assessment'!G5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!G4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H8">
-        <f>IFERROR(MATCH('Current Assessment'!H5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!H4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I8">
-        <f>IFERROR(MATCH('Current Assessment'!I5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!I4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J8">
-        <f>IFERROR(MATCH('Current Assessment'!J5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!J4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K8">
-        <f>IFERROR(MATCH('Current Assessment'!K5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!K4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L8">
-        <f>IFERROR(MATCH('Current Assessment'!L5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!L4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M8">
-        <f>IFERROR(MATCH('Current Assessment'!M5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!M4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N8">
-        <f>IFERROR(MATCH('Current Assessment'!N5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!N4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O8">
-        <f>IFERROR(MATCH('Current Assessment'!O5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!O4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P8">
-        <f>IFERROR(MATCH('Current Assessment'!P5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!P4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q8">
-        <f>IFERROR(MATCH('Current Assessment'!Q5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!Q4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R8">
-        <f>IFERROR(MATCH('Current Assessment'!R5,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!R4,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="str">
-        <f>'Current Assessment'!A6</f>
+        <f>Input!A5</f>
         <v/>
       </c>
       <c r="B9">
-        <f>IFERROR(MATCH('Current Assessment'!B6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!B5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="C9">
-        <f>IFERROR(MATCH('Current Assessment'!C6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!C5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="D9">
-        <f>IFERROR(MATCH('Current Assessment'!D6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!D5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="E9">
-        <f>IFERROR(MATCH('Current Assessment'!E6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!E5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F9">
-        <f>IFERROR(MATCH('Current Assessment'!F6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!F5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G9">
-        <f>IFERROR(MATCH('Current Assessment'!G6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!G5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H9">
-        <f>IFERROR(MATCH('Current Assessment'!H6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!H5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I9">
-        <f>IFERROR(MATCH('Current Assessment'!I6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!I5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J9">
-        <f>IFERROR(MATCH('Current Assessment'!J6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!J5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K9">
-        <f>IFERROR(MATCH('Current Assessment'!K6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!K5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L9">
-        <f>IFERROR(MATCH('Current Assessment'!L6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!L5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M9">
-        <f>IFERROR(MATCH('Current Assessment'!M6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!M5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N9">
-        <f>IFERROR(MATCH('Current Assessment'!N6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!N5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O9">
-        <f>IFERROR(MATCH('Current Assessment'!O6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!O5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P9">
-        <f>IFERROR(MATCH('Current Assessment'!P6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!P5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q9">
-        <f>IFERROR(MATCH('Current Assessment'!Q6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!Q5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R9">
-        <f>IFERROR(MATCH('Current Assessment'!R6,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!R5,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="str">
-        <f>'Current Assessment'!A7</f>
+        <f>Input!A6</f>
         <v/>
       </c>
       <c r="B10">
-        <f>IFERROR(MATCH('Current Assessment'!B7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!B6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="C10">
-        <f>IFERROR(MATCH('Current Assessment'!C7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!C6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="D10">
-        <f>IFERROR(MATCH('Current Assessment'!D7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!D6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="E10">
-        <f>IFERROR(MATCH('Current Assessment'!E7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!E6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F10">
-        <f>IFERROR(MATCH('Current Assessment'!F7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!F6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G10">
-        <f>IFERROR(MATCH('Current Assessment'!G7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!G6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H10">
-        <f>IFERROR(MATCH('Current Assessment'!H7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!H6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I10">
-        <f>IFERROR(MATCH('Current Assessment'!I7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!I6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J10">
-        <f>IFERROR(MATCH('Current Assessment'!J7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!J6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K10">
-        <f>IFERROR(MATCH('Current Assessment'!K7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!K6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L10">
-        <f>IFERROR(MATCH('Current Assessment'!L7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!L6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M10">
-        <f>IFERROR(MATCH('Current Assessment'!M7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!M6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N10">
-        <f>IFERROR(MATCH('Current Assessment'!N7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!N6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O10">
-        <f>IFERROR(MATCH('Current Assessment'!O7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!O6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P10">
-        <f>IFERROR(MATCH('Current Assessment'!P7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!P6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q10">
-        <f>IFERROR(MATCH('Current Assessment'!Q7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!Q6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R10">
-        <f>IFERROR(MATCH('Current Assessment'!R7,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!R6,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="str">
-        <f>'Current Assessment'!A8</f>
+        <f>Input!A7</f>
         <v/>
       </c>
       <c r="B11">
-        <f>IFERROR(MATCH('Current Assessment'!B8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!B7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="C11">
-        <f>IFERROR(MATCH('Current Assessment'!C8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!C7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="D11">
-        <f>IFERROR(MATCH('Current Assessment'!D8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!D7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="E11">
-        <f>IFERROR(MATCH('Current Assessment'!E8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!E7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F11">
-        <f>IFERROR(MATCH('Current Assessment'!F8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!F7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G11">
-        <f>IFERROR(MATCH('Current Assessment'!G8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!G7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H11">
-        <f>IFERROR(MATCH('Current Assessment'!H8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!H7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I11">
-        <f>IFERROR(MATCH('Current Assessment'!I8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!I7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J11">
-        <f>IFERROR(MATCH('Current Assessment'!J8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!J7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K11">
-        <f>IFERROR(MATCH('Current Assessment'!K8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!K7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L11">
-        <f>IFERROR(MATCH('Current Assessment'!L8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!L7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M11">
-        <f>IFERROR(MATCH('Current Assessment'!M8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!M7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N11">
-        <f>IFERROR(MATCH('Current Assessment'!N8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!N7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O11">
-        <f>IFERROR(MATCH('Current Assessment'!O8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!O7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P11">
-        <f>IFERROR(MATCH('Current Assessment'!P8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!P7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q11">
-        <f>IFERROR(MATCH('Current Assessment'!Q8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!Q7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R11">
-        <f>IFERROR(MATCH('Current Assessment'!R8,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!R7,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="str">
-        <f>'Current Assessment'!A9</f>
+        <f>Input!A8</f>
         <v/>
       </c>
       <c r="B12">
-        <f>IFERROR(MATCH('Current Assessment'!B9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!B8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="C12">
-        <f>IFERROR(MATCH('Current Assessment'!C9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!C8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="D12">
-        <f>IFERROR(MATCH('Current Assessment'!D9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!D8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="E12">
-        <f>IFERROR(MATCH('Current Assessment'!E9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!E8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F12">
-        <f>IFERROR(MATCH('Current Assessment'!F9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!F8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G12">
-        <f>IFERROR(MATCH('Current Assessment'!G9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!G8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H12">
-        <f>IFERROR(MATCH('Current Assessment'!H9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!H8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I12">
-        <f>IFERROR(MATCH('Current Assessment'!I9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!I8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J12">
-        <f>IFERROR(MATCH('Current Assessment'!J9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!J8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K12">
-        <f>IFERROR(MATCH('Current Assessment'!K9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!K8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L12">
-        <f>IFERROR(MATCH('Current Assessment'!L9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!L8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M12">
-        <f>IFERROR(MATCH('Current Assessment'!M9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!M8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N12">
-        <f>IFERROR(MATCH('Current Assessment'!N9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!N8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O12">
-        <f>IFERROR(MATCH('Current Assessment'!O9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!O8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P12">
-        <f>IFERROR(MATCH('Current Assessment'!P9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!P8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q12">
-        <f>IFERROR(MATCH('Current Assessment'!Q9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!Q8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R12">
-        <f>IFERROR(MATCH('Current Assessment'!R9,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!R8,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="str">
-        <f>'Current Assessment'!A10</f>
+        <f>Input!A9</f>
         <v/>
       </c>
       <c r="B13">
-        <f>IFERROR(MATCH('Current Assessment'!B10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!B9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="C13">
-        <f>IFERROR(MATCH('Current Assessment'!C10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!C9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="D13">
-        <f>IFERROR(MATCH('Current Assessment'!D10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!D9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="E13">
-        <f>IFERROR(MATCH('Current Assessment'!E10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!E9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F13">
-        <f>IFERROR(MATCH('Current Assessment'!F10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!F9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G13">
-        <f>IFERROR(MATCH('Current Assessment'!G10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!G9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H13">
-        <f>IFERROR(MATCH('Current Assessment'!H10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!H9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I13">
-        <f>IFERROR(MATCH('Current Assessment'!I10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!I9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J13">
-        <f>IFERROR(MATCH('Current Assessment'!J10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!J9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K13">
-        <f>IFERROR(MATCH('Current Assessment'!K10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!K9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L13">
-        <f>IFERROR(MATCH('Current Assessment'!L10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!L9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M13">
-        <f>IFERROR(MATCH('Current Assessment'!M10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!M9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N13">
-        <f>IFERROR(MATCH('Current Assessment'!N10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!N9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O13">
-        <f>IFERROR(MATCH('Current Assessment'!O10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!O9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P13">
-        <f>IFERROR(MATCH('Current Assessment'!P10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!P9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q13">
-        <f>IFERROR(MATCH('Current Assessment'!Q10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!Q9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R13">
-        <f>IFERROR(MATCH('Current Assessment'!R10,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!R9,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="str">
-        <f>'Current Assessment'!A11</f>
+        <f>Input!A10</f>
         <v/>
       </c>
       <c r="B14">
-        <f>IFERROR(MATCH('Current Assessment'!B11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!B10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="C14">
-        <f>IFERROR(MATCH('Current Assessment'!C11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!C10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="D14">
-        <f>IFERROR(MATCH('Current Assessment'!D11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!D10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="E14">
-        <f>IFERROR(MATCH('Current Assessment'!E11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!E10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F14">
-        <f>IFERROR(MATCH('Current Assessment'!F11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!F10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G14">
-        <f>IFERROR(MATCH('Current Assessment'!G11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!G10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H14">
-        <f>IFERROR(MATCH('Current Assessment'!H11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!H10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I14">
-        <f>IFERROR(MATCH('Current Assessment'!I11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!I10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J14">
-        <f>IFERROR(MATCH('Current Assessment'!J11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!J10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K14">
-        <f>IFERROR(MATCH('Current Assessment'!K11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!K10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L14">
-        <f>IFERROR(MATCH('Current Assessment'!L11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!L10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M14">
-        <f>IFERROR(MATCH('Current Assessment'!M11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!M10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N14">
-        <f>IFERROR(MATCH('Current Assessment'!N11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!N10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O14">
-        <f>IFERROR(MATCH('Current Assessment'!O11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!O10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P14">
-        <f>IFERROR(MATCH('Current Assessment'!P11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!P10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q14">
-        <f>IFERROR(MATCH('Current Assessment'!Q11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!Q10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R14">
-        <f>IFERROR(MATCH('Current Assessment'!R11,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!R10,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="str">
-        <f>'Current Assessment'!A12</f>
+        <f>Input!A11</f>
         <v/>
       </c>
       <c r="B15">
-        <f>IFERROR(MATCH('Current Assessment'!B12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!B11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="C15">
-        <f>IFERROR(MATCH('Current Assessment'!C12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!C11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="D15">
-        <f>IFERROR(MATCH('Current Assessment'!D12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!D11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="E15">
-        <f>IFERROR(MATCH('Current Assessment'!E12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!E11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F15">
-        <f>IFERROR(MATCH('Current Assessment'!F12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!F11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G15">
-        <f>IFERROR(MATCH('Current Assessment'!G12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!G11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H15">
-        <f>IFERROR(MATCH('Current Assessment'!H12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!H11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I15">
-        <f>IFERROR(MATCH('Current Assessment'!I12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!I11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J15">
-        <f>IFERROR(MATCH('Current Assessment'!J12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!J11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K15">
-        <f>IFERROR(MATCH('Current Assessment'!K12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!K11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L15">
-        <f>IFERROR(MATCH('Current Assessment'!L12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!L11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M15">
-        <f>IFERROR(MATCH('Current Assessment'!M12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!M11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N15">
-        <f>IFERROR(MATCH('Current Assessment'!N12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!N11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O15">
-        <f>IFERROR(MATCH('Current Assessment'!O12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!O11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P15">
-        <f>IFERROR(MATCH('Current Assessment'!P12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!P11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q15">
-        <f>IFERROR(MATCH('Current Assessment'!Q12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!Q11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R15">
-        <f>IFERROR(MATCH('Current Assessment'!R12,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!R11,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="str">
-        <f>'Current Assessment'!A13</f>
+        <f>Input!A12</f>
         <v/>
       </c>
       <c r="B16">
-        <f>IFERROR(MATCH('Current Assessment'!B13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!B12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="C16">
-        <f>IFERROR(MATCH('Current Assessment'!C13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!C12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="D16">
-        <f>IFERROR(MATCH('Current Assessment'!D13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!D12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="E16">
-        <f>IFERROR(MATCH('Current Assessment'!E13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!E12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="F16">
-        <f>IFERROR(MATCH('Current Assessment'!F13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!F12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="G16">
-        <f>IFERROR(MATCH('Current Assessment'!G13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!G12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="H16">
-        <f>IFERROR(MATCH('Current Assessment'!H13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!H12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="I16">
-        <f>IFERROR(MATCH('Current Assessment'!I13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!I12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="J16">
-        <f>IFERROR(MATCH('Current Assessment'!J13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!J12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="K16">
-        <f>IFERROR(MATCH('Current Assessment'!K13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!K12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="L16">
-        <f>IFERROR(MATCH('Current Assessment'!L13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!L12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="M16">
-        <f>IFERROR(MATCH('Current Assessment'!M13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!M12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="N16">
-        <f>IFERROR(MATCH('Current Assessment'!N13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!N12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="O16">
-        <f>IFERROR(MATCH('Current Assessment'!O13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!O12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="P16">
-        <f>IFERROR(MATCH('Current Assessment'!P13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!P12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q16">
-        <f>IFERROR(MATCH('Current Assessment'!Q13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!Q12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
       <c r="R16">
-        <f>IFERROR(MATCH('Current Assessment'!R13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <f>IFERROR(MATCH(Input!R12,Settings!$G$6:$G$10,0)-1, 0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="6">
-        <f t="shared" ref="B17:R17" si="3">SUM(B5:B16)</f>
-        <v>4</v>
-      </c>
-      <c r="C17" s="6">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="str">
+        <f>Input!A13</f>
+        <v/>
+      </c>
+      <c r="B17">
+        <f>IFERROR(MATCH(Input!B13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <f>IFERROR(MATCH(Input!C13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <f>IFERROR(MATCH(Input!D13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f>IFERROR(MATCH(Input!E13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <f>IFERROR(MATCH(Input!F13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <f>IFERROR(MATCH(Input!G13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <f>IFERROR(MATCH(Input!H13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f>IFERROR(MATCH(Input!I13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <f>IFERROR(MATCH(Input!J13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <f>IFERROR(MATCH(Input!K13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f>IFERROR(MATCH(Input!L13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <f>IFERROR(MATCH(Input!M13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <f>IFERROR(MATCH(Input!N13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <f>IFERROR(MATCH(Input!O13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <f>IFERROR(MATCH(Input!P13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <f>IFERROR(MATCH(Input!Q13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <f>IFERROR(MATCH(Input!R13,Settings!$G$6:$G$10,0)-1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="6">
+        <f t="shared" ref="B18:R18" si="3">SUM(B6:B17)</f>
+        <v>2</v>
+      </c>
+      <c r="C18" s="6">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D18" s="6">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E18" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F18" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G18" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H18" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I18" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J17" s="6">
+      <c r="J18" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K17" s="6">
+      <c r="K18" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L17" s="6">
+      <c r="L18" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M17" s="6">
+      <c r="M18" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N17" s="6">
+      <c r="N18" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O17" s="6">
+      <c r="O18" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P17" s="6">
+      <c r="P18" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Q17" s="6">
+      <c r="Q18" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R17" s="6">
+      <c r="R18" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>27</v>
+    <row r="19" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>27</v>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B17:R17">
-    <cfRule type="colorScale" priority="6">
+  <conditionalFormatting sqref="B18:R18">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -15227,9 +15276,19 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5:R16">
-    <cfRule type="colorScale" priority="8">
+  <conditionalFormatting sqref="B6:R17">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -15239,12 +15298,11 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="7" id="{339E999E-0713-46E1-92D7-78E999ECB110}">
+          <x14:cfRule type="iconSet" priority="8" id="{339E999E-0713-46E1-92D7-78E999ECB110}">
             <x14:iconSet iconSet="4TrafficLights" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -15264,7 +15322,7 @@
               <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>B1:R3</xm:sqref>
+          <xm:sqref>B1:R4</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -15274,6 +15332,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet6"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:U27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15288,99 +15360,99 @@
     <row r="1" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13"/>
       <c r="B1" s="13" t="str">
-        <f>IF('Current Assessment'!B1&lt;&gt;"",'Current Assessment'!B1,"")</f>
+        <f>IF(Input!B1&lt;&gt;"",Input!B1,"")</f>
         <v>CSS</v>
       </c>
       <c r="C1" s="13" t="str">
-        <f>IF('Current Assessment'!C1&lt;&gt;"",'Current Assessment'!C1,"")</f>
+        <f>IF(Input!C1&lt;&gt;"",Input!C1,"")</f>
         <v>Javascript</v>
       </c>
       <c r="D1" s="13" t="str">
-        <f>IF('Current Assessment'!D1&lt;&gt;"",'Current Assessment'!D1,"")</f>
+        <f>IF(Input!D1&lt;&gt;"",Input!D1,"")</f>
         <v>DB Backup/Restore</v>
       </c>
       <c r="E1" s="13" t="str">
-        <f>IF('Current Assessment'!E1&lt;&gt;"",'Current Assessment'!E1,"")</f>
+        <f>IF(Input!E1&lt;&gt;"",Input!E1,"")</f>
         <v/>
       </c>
       <c r="F1" s="13" t="str">
-        <f>IF('Current Assessment'!F1&lt;&gt;"",'Current Assessment'!F1,"")</f>
+        <f>IF(Input!F1&lt;&gt;"",Input!F1,"")</f>
         <v/>
       </c>
       <c r="G1" s="13" t="str">
-        <f>IF('Current Assessment'!G1&lt;&gt;"",'Current Assessment'!G1,"")</f>
+        <f>IF(Input!G1&lt;&gt;"",Input!G1,"")</f>
         <v/>
       </c>
       <c r="H1" s="13" t="str">
-        <f>IF('Current Assessment'!H1&lt;&gt;"",'Current Assessment'!H1,"")</f>
+        <f>IF(Input!H1&lt;&gt;"",Input!H1,"")</f>
         <v/>
       </c>
       <c r="I1" s="13" t="str">
-        <f>IF('Current Assessment'!I1&lt;&gt;"",'Current Assessment'!I1,"")</f>
+        <f>IF(Input!I1&lt;&gt;"",Input!I1,"")</f>
         <v/>
       </c>
       <c r="J1" s="13" t="str">
-        <f>IF('Current Assessment'!J1&lt;&gt;"",'Current Assessment'!J1,"")</f>
+        <f>IF(Input!J1&lt;&gt;"",Input!J1,"")</f>
         <v/>
       </c>
       <c r="K1" s="13" t="str">
-        <f>IF('Current Assessment'!K1&lt;&gt;"",'Current Assessment'!K1,"")</f>
+        <f>IF(Input!K1&lt;&gt;"",Input!K1,"")</f>
         <v/>
       </c>
       <c r="L1" s="13" t="str">
-        <f>IF('Current Assessment'!L1&lt;&gt;"",'Current Assessment'!L1,"")</f>
+        <f>IF(Input!L1&lt;&gt;"",Input!L1,"")</f>
         <v/>
       </c>
       <c r="M1" s="13" t="str">
-        <f>IF('Current Assessment'!M1&lt;&gt;"",'Current Assessment'!M1,"")</f>
+        <f>IF(Input!M1&lt;&gt;"",Input!M1,"")</f>
         <v/>
       </c>
       <c r="N1" s="13" t="str">
-        <f>IF('Current Assessment'!N1&lt;&gt;"",'Current Assessment'!N1,"")</f>
+        <f>IF(Input!N1&lt;&gt;"",Input!N1,"")</f>
         <v/>
       </c>
       <c r="O1" s="13" t="str">
-        <f>IF('Current Assessment'!O1&lt;&gt;"",'Current Assessment'!O1,"")</f>
+        <f>IF(Input!O1&lt;&gt;"",Input!O1,"")</f>
         <v/>
       </c>
       <c r="P1" s="13" t="str">
-        <f>IF('Current Assessment'!P1&lt;&gt;"",'Current Assessment'!P1,"")</f>
+        <f>IF(Input!P1&lt;&gt;"",Input!P1,"")</f>
         <v/>
       </c>
       <c r="Q1" s="13" t="str">
-        <f>IF('Current Assessment'!Q1&lt;&gt;"",'Current Assessment'!Q1,"")</f>
+        <f>IF(Input!Q1&lt;&gt;"",Input!Q1,"")</f>
         <v/>
       </c>
       <c r="R1" s="13" t="str">
-        <f>IF('Current Assessment'!R1&lt;&gt;"",'Current Assessment'!R1,"")</f>
+        <f>IF(Input!R1&lt;&gt;"",Input!R1,"")</f>
         <v/>
       </c>
       <c r="S1" s="13" t="e">
-        <f>IF('Current Assessment'!#REF!&lt;&gt;"",'Current Assessment'!#REF!,"")</f>
+        <f>IF(Input!#REF!&lt;&gt;"",Input!#REF!,"")</f>
         <v>#REF!</v>
       </c>
       <c r="T1" s="13" t="e">
-        <f>IF('Current Assessment'!#REF!&lt;&gt;"",'Current Assessment'!#REF!,"")</f>
+        <f>IF(Input!#REF!&lt;&gt;"",Input!#REF!,"")</f>
         <v>#REF!</v>
       </c>
       <c r="U1" s="13" t="e">
-        <f>IF('Current Assessment'!#REF!&lt;&gt;"",'Current Assessment'!#REF!,"")</f>
+        <f>IF(Input!#REF!&lt;&gt;"",Input!#REF!,"")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="str">
-        <f>IF('Current Assessment'!A2&lt;&gt;"", 'Current Assessment'!A2, "")</f>
+        <f>IF(Input!A2&lt;&gt;"", Input!A2, "")</f>
         <v>Person 1</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
@@ -15402,7 +15474,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="str">
-        <f>IF('Current Assessment'!A3&lt;&gt;"", 'Current Assessment'!A3, "")</f>
+        <f>IF(Input!A3&lt;&gt;"", Input!A3, "")</f>
         <v>Person 2</v>
       </c>
       <c r="B3" s="12"/>
@@ -15430,7 +15502,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="str">
-        <f>IF('Current Assessment'!A4&lt;&gt;"", 'Current Assessment'!A4, "")</f>
+        <f>IF(Input!A4&lt;&gt;"", Input!A4, "")</f>
         <v>Team 1</v>
       </c>
       <c r="B4" s="12"/>
@@ -15456,7 +15528,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="str">
-        <f>IF('Current Assessment'!A5&lt;&gt;"", 'Current Assessment'!A5, "")</f>
+        <f>IF(Input!A5&lt;&gt;"", Input!A5, "")</f>
         <v/>
       </c>
       <c r="B5" s="12"/>
@@ -15482,7 +15554,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="str">
-        <f>IF('Current Assessment'!A6&lt;&gt;"", 'Current Assessment'!A6, "")</f>
+        <f>IF(Input!A6&lt;&gt;"", Input!A6, "")</f>
         <v/>
       </c>
       <c r="B6" s="12"/>
@@ -15508,7 +15580,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="str">
-        <f>IF('Current Assessment'!A7&lt;&gt;"", 'Current Assessment'!A7, "")</f>
+        <f>IF(Input!A7&lt;&gt;"", Input!A7, "")</f>
         <v/>
       </c>
       <c r="B7" s="12"/>
@@ -15534,7 +15606,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="str">
-        <f>IF('Current Assessment'!A8&lt;&gt;"", 'Current Assessment'!A8, "")</f>
+        <f>IF(Input!A8&lt;&gt;"", Input!A8, "")</f>
         <v/>
       </c>
       <c r="B8" s="12"/>
@@ -15560,7 +15632,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="str">
-        <f>IF('Current Assessment'!A9&lt;&gt;"", 'Current Assessment'!A9, "")</f>
+        <f>IF(Input!A9&lt;&gt;"", Input!A9, "")</f>
         <v/>
       </c>
       <c r="B9" s="12"/>
@@ -15586,7 +15658,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="str">
-        <f>IF('Current Assessment'!A10&lt;&gt;"", 'Current Assessment'!A10, "")</f>
+        <f>IF(Input!A10&lt;&gt;"", Input!A10, "")</f>
         <v/>
       </c>
       <c r="B10" s="12"/>
@@ -15612,7 +15684,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="str">
-        <f>IF('Current Assessment'!A11&lt;&gt;"", 'Current Assessment'!A11, "")</f>
+        <f>IF(Input!A11&lt;&gt;"", Input!A11, "")</f>
         <v/>
       </c>
       <c r="B11" s="12"/>
@@ -15638,7 +15710,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="str">
-        <f>IF('Current Assessment'!A12&lt;&gt;"", 'Current Assessment'!A12, "")</f>
+        <f>IF(Input!A12&lt;&gt;"", Input!A12, "")</f>
         <v/>
       </c>
       <c r="B12" s="12"/>
@@ -15664,7 +15736,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="str">
-        <f>IF('Current Assessment'!A13&lt;&gt;"", 'Current Assessment'!A13, "")</f>
+        <f>IF(Input!A13&lt;&gt;"", Input!A13, "")</f>
         <v/>
       </c>
       <c r="B13" s="12"/>
@@ -15690,7 +15762,7 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="e">
-        <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
+        <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
         <v>#REF!</v>
       </c>
       <c r="B14" s="12"/>
@@ -15716,7 +15788,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="e">
-        <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
+        <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
         <v>#REF!</v>
       </c>
       <c r="B15" s="12"/>
@@ -15742,7 +15814,7 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="e">
-        <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
+        <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
         <v>#REF!</v>
       </c>
       <c r="B16" s="12"/>
@@ -15768,7 +15840,7 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="e">
-        <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
+        <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
         <v>#REF!</v>
       </c>
       <c r="B17" s="12"/>
@@ -15794,7 +15866,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="e">
-        <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
+        <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
         <v>#REF!</v>
       </c>
       <c r="B18" s="12"/>
@@ -15820,7 +15892,7 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="e">
-        <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
+        <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
         <v>#REF!</v>
       </c>
       <c r="B19" s="12"/>
@@ -15846,7 +15918,7 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="e">
-        <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
+        <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
         <v>#REF!</v>
       </c>
       <c r="B20" s="12"/>
@@ -15872,7 +15944,7 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="e">
-        <f>IF('Current Assessment'!#REF!&lt;&gt;"", 'Current Assessment'!#REF!, "")</f>
+        <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
         <v>#REF!</v>
       </c>
       <c r="B21" s="12"/>
@@ -15898,7 +15970,7 @@
     </row>
     <row r="23" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -16071,7 +16143,7 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B26" s="7">
         <f>Willingness_Calcs!B2</f>
@@ -16156,7 +16228,7 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B27" s="7">
         <f>Willingness_Calcs!B3</f>
@@ -16284,8 +16356,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16302,7 +16375,7 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B1">
         <f>IF(B$4&lt;&gt;"",COUNTIF(B$5:B$24, "&gt;= 3"),"")</f>
@@ -16387,7 +16460,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <f>IF(B$4&lt;&gt;"",COUNTIF(B$5:B$24, "&gt;= 2"),"")</f>
@@ -16472,7 +16545,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <f>IF(B$4&lt;&gt;"",COUNTIF(B$5:B$24, "= 1"),"")</f>
@@ -16557,89 +16630,89 @@
     </row>
     <row r="4" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="str">
-        <f>IF('Current Assessment'!B1&lt;&gt;"",'Current Assessment'!B1,"")</f>
+        <f>IF(Input!B1&lt;&gt;"",Input!B1,"")</f>
         <v>CSS</v>
       </c>
       <c r="C4" s="9" t="str">
-        <f>IF('Current Assessment'!C1&lt;&gt;"",'Current Assessment'!C1,"")</f>
+        <f>IF(Input!C1&lt;&gt;"",Input!C1,"")</f>
         <v>Javascript</v>
       </c>
       <c r="D4" s="9" t="str">
-        <f>IF('Current Assessment'!D1&lt;&gt;"",'Current Assessment'!D1,"")</f>
+        <f>IF(Input!D1&lt;&gt;"",Input!D1,"")</f>
         <v>DB Backup/Restore</v>
       </c>
       <c r="E4" s="9" t="str">
-        <f>IF('Current Assessment'!E1&lt;&gt;"",'Current Assessment'!E1,"")</f>
+        <f>IF(Input!E1&lt;&gt;"",Input!E1,"")</f>
         <v/>
       </c>
       <c r="F4" s="9" t="str">
-        <f>IF('Current Assessment'!F1&lt;&gt;"",'Current Assessment'!F1,"")</f>
+        <f>IF(Input!F1&lt;&gt;"",Input!F1,"")</f>
         <v/>
       </c>
       <c r="G4" s="9" t="str">
-        <f>IF('Current Assessment'!G1&lt;&gt;"",'Current Assessment'!G1,"")</f>
+        <f>IF(Input!G1&lt;&gt;"",Input!G1,"")</f>
         <v/>
       </c>
       <c r="H4" s="9" t="str">
-        <f>IF('Current Assessment'!H1&lt;&gt;"",'Current Assessment'!H1,"")</f>
+        <f>IF(Input!H1&lt;&gt;"",Input!H1,"")</f>
         <v/>
       </c>
       <c r="I4" s="9" t="str">
-        <f>IF('Current Assessment'!I1&lt;&gt;"",'Current Assessment'!I1,"")</f>
+        <f>IF(Input!I1&lt;&gt;"",Input!I1,"")</f>
         <v/>
       </c>
       <c r="J4" s="9" t="str">
-        <f>IF('Current Assessment'!J1&lt;&gt;"",'Current Assessment'!J1,"")</f>
+        <f>IF(Input!J1&lt;&gt;"",Input!J1,"")</f>
         <v/>
       </c>
       <c r="K4" s="9" t="str">
-        <f>IF('Current Assessment'!K1&lt;&gt;"",'Current Assessment'!K1,"")</f>
+        <f>IF(Input!K1&lt;&gt;"",Input!K1,"")</f>
         <v/>
       </c>
       <c r="L4" s="9" t="str">
-        <f>IF('Current Assessment'!L1&lt;&gt;"",'Current Assessment'!L1,"")</f>
+        <f>IF(Input!L1&lt;&gt;"",Input!L1,"")</f>
         <v/>
       </c>
       <c r="M4" s="9" t="str">
-        <f>IF('Current Assessment'!M1&lt;&gt;"",'Current Assessment'!M1,"")</f>
+        <f>IF(Input!M1&lt;&gt;"",Input!M1,"")</f>
         <v/>
       </c>
       <c r="N4" s="9" t="str">
-        <f>IF('Current Assessment'!N1&lt;&gt;"",'Current Assessment'!N1,"")</f>
+        <f>IF(Input!N1&lt;&gt;"",Input!N1,"")</f>
         <v/>
       </c>
       <c r="O4" s="9" t="str">
-        <f>IF('Current Assessment'!O1&lt;&gt;"",'Current Assessment'!O1,"")</f>
+        <f>IF(Input!O1&lt;&gt;"",Input!O1,"")</f>
         <v/>
       </c>
       <c r="P4" s="9" t="str">
-        <f>IF('Current Assessment'!P1&lt;&gt;"",'Current Assessment'!P1,"")</f>
+        <f>IF(Input!P1&lt;&gt;"",Input!P1,"")</f>
         <v/>
       </c>
       <c r="Q4" s="9" t="str">
-        <f>IF('Current Assessment'!Q1&lt;&gt;"",'Current Assessment'!Q1,"")</f>
+        <f>IF(Input!Q1&lt;&gt;"",Input!Q1,"")</f>
         <v/>
       </c>
       <c r="R4" s="9" t="str">
-        <f>IF('Current Assessment'!R1&lt;&gt;"",'Current Assessment'!R1,"")</f>
+        <f>IF(Input!R1&lt;&gt;"",Input!R1,"")</f>
         <v/>
       </c>
       <c r="S4" s="9" t="e">
-        <f>IF('Current Assessment'!#REF!&lt;&gt;"",'Current Assessment'!#REF!,"")</f>
+        <f>IF(Input!#REF!&lt;&gt;"",Input!#REF!,"")</f>
         <v>#REF!</v>
       </c>
       <c r="T4" s="9" t="e">
-        <f>IF('Current Assessment'!#REF!&lt;&gt;"",'Current Assessment'!#REF!,"")</f>
+        <f>IF(Input!#REF!&lt;&gt;"",Input!#REF!,"")</f>
         <v>#REF!</v>
       </c>
       <c r="U4" s="9" t="e">
-        <f>IF('Current Assessment'!#REF!&lt;&gt;"",'Current Assessment'!#REF!,"")</f>
+        <f>IF(Input!#REF!&lt;&gt;"",Input!#REF!,"")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="str">
-        <f>'Current Assessment'!A2</f>
+        <f>Input!A2</f>
         <v>Person 1</v>
       </c>
       <c r="B5">
@@ -16725,7 +16798,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="str">
-        <f>'Current Assessment'!A3</f>
+        <f>Input!A3</f>
         <v>Person 2</v>
       </c>
       <c r="B6">
@@ -16811,7 +16884,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="str">
-        <f>'Current Assessment'!A4</f>
+        <f>Input!A4</f>
         <v>Team 1</v>
       </c>
       <c r="B7">
@@ -16897,7 +16970,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="str">
-        <f>'Current Assessment'!A5</f>
+        <f>Input!A5</f>
         <v/>
       </c>
       <c r="B8">
@@ -16983,7 +17056,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="str">
-        <f>'Current Assessment'!A6</f>
+        <f>Input!A6</f>
         <v/>
       </c>
       <c r="B9">
@@ -17069,7 +17142,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="str">
-        <f>'Current Assessment'!A7</f>
+        <f>Input!A7</f>
         <v/>
       </c>
       <c r="B10">
@@ -17155,7 +17228,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="str">
-        <f>'Current Assessment'!A8</f>
+        <f>Input!A8</f>
         <v/>
       </c>
       <c r="B11">
@@ -17241,7 +17314,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="str">
-        <f>'Current Assessment'!A9</f>
+        <f>Input!A9</f>
         <v/>
       </c>
       <c r="B12">
@@ -17327,7 +17400,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="str">
-        <f>'Current Assessment'!A10</f>
+        <f>Input!A10</f>
         <v/>
       </c>
       <c r="B13">
@@ -17413,7 +17486,7 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="str">
-        <f>'Current Assessment'!A11</f>
+        <f>Input!A11</f>
         <v/>
       </c>
       <c r="B14">
@@ -17499,7 +17572,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="str">
-        <f>'Current Assessment'!A12</f>
+        <f>Input!A12</f>
         <v/>
       </c>
       <c r="B15">
@@ -17585,7 +17658,7 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="str">
-        <f>'Current Assessment'!A13</f>
+        <f>Input!A13</f>
         <v/>
       </c>
       <c r="B16">
@@ -17671,7 +17744,7 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="e">
-        <f>'Current Assessment'!#REF!</f>
+        <f>Input!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B17">
@@ -17757,7 +17830,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="e">
-        <f>'Current Assessment'!#REF!</f>
+        <f>Input!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B18">
@@ -17843,7 +17916,7 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="e">
-        <f>'Current Assessment'!#REF!</f>
+        <f>Input!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B19">
@@ -17929,7 +18002,7 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="e">
-        <f>'Current Assessment'!#REF!</f>
+        <f>Input!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B20">
@@ -18015,7 +18088,7 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="e">
-        <f>'Current Assessment'!#REF!</f>
+        <f>Input!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B21">
@@ -18101,7 +18174,7 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="e">
-        <f>'Current Assessment'!#REF!</f>
+        <f>Input!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B22">
@@ -18187,7 +18260,7 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="e">
-        <f>'Current Assessment'!#REF!</f>
+        <f>Input!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B23">
@@ -18273,7 +18346,7 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="e">
-        <f>'Current Assessment'!#REF!</f>
+        <f>Input!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B24">

</xml_diff>

<commit_message>
Moved advice starter to the heat map page.
</commit_message>
<xml_diff>
--- a/Spreadsheets/Capability Matrix.xlsx
+++ b/Spreadsheets/Capability Matrix.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="90" yWindow="765" windowWidth="19140" windowHeight="9525" activeTab="3"/>
+    <workbookView xWindow="90" yWindow="1110" windowWidth="19140" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
   <si>
     <t>Willing</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>For each skill, choose from the list of DESIREABLE values. If in doubt, err high (right)!</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>People / Teams</t>
@@ -12233,6 +12230,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -12268,6 +12282,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -12447,7 +12478,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:Q23"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
@@ -12455,7 +12486,7 @@
   <sheetData>
     <row r="1" spans="2:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C1" s="37"/>
       <c r="D1" s="37"/>
@@ -12472,7 +12503,7 @@
     </row>
     <row r="2" spans="2:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="P2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
@@ -12480,7 +12511,7 @@
         <v>1</v>
       </c>
       <c r="Q4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
@@ -12488,7 +12519,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="Q5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
@@ -12580,18 +12611,18 @@
   <sheetData>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="24" t="s">
         <v>24</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>25</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K5" s="2"/>
     </row>
@@ -12611,7 +12642,7 @@
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="25" t="s">
         <v>4</v>
@@ -12628,7 +12659,7 @@
         <v>15</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G8" s="25" t="s">
         <v>19</v>
@@ -12651,7 +12682,7 @@
       <c r="B10" s="26"/>
       <c r="D10" s="25"/>
       <c r="G10" s="25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I10" s="25" t="s">
         <v>2</v>
@@ -12728,7 +12759,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -13198,10 +13229,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:R33"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView showGridLines="0" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13580,7 +13611,7 @@
     <row r="14" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -13656,7 +13687,7 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="28">
         <f>Heatmap!B1</f>
@@ -13729,7 +13760,7 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="28">
         <f>Heatmap!B2</f>
@@ -13802,7 +13833,7 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="28">
         <f>Heatmap!B3</f>
@@ -13871,72 +13902,6 @@
       <c r="R19" s="29" t="str">
         <f>Heatmap!R3</f>
         <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28">
-        <v>3</v>
-      </c>
-      <c r="D28" t="s">
-        <v>40</v>
-      </c>
-      <c r="E28" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29">
-        <v>6</v>
-      </c>
-      <c r="D29" t="s">
-        <v>46</v>
-      </c>
-      <c r="E29" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="D30" t="s">
-        <v>48</v>
-      </c>
-      <c r="E30" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -13991,10 +13956,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:R22"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14007,7 +13972,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1">
         <f t="shared" ref="B1:R1" si="0">IF(B$5&lt;&gt;"",COUNTIF(B$6:B$17, "&gt;= 3"),"")</f>
@@ -14080,7 +14045,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <f t="shared" ref="B2:R2" si="1">IF(B$5&lt;&gt;"",COUNTIF(B$6:B$17, "&gt;= 2"),"")</f>
@@ -14153,7 +14118,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <f t="shared" ref="B3:R3" si="2">IF(B$5&lt;&gt;"",COUNTIF(B$6:B$17, "= 1"),"")</f>
@@ -15256,26 +15221,83 @@
       </c>
     </row>
     <row r="19" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B20" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>23</v>
+      <c r="B21" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21">
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>23</v>
-      </c>
+      <c r="B22" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B23" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B24" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B25" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B26" s="9"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B27" s="9"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B28" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B18:R18">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -15283,6 +15305,14 @@
         <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>

</xml_diff>

<commit_message>
Added advice worksheet and legend to the heat map.
</commit_message>
<xml_diff>
--- a/Spreadsheets/Capability Matrix.xlsx
+++ b/Spreadsheets/Capability Matrix.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Private\GitHub\FocusedObjective.Resources\Spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troy/Dropbox/Private/GitHub/FocusedObjective.Resources/Spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="90" yWindow="1110" windowWidth="19140" windowHeight="9525"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="6" r:id="rId1"/>
     <sheet name="Settings" sheetId="2" r:id="rId2"/>
     <sheet name="Survey Sheet" sheetId="5" r:id="rId3"/>
     <sheet name="Input" sheetId="1" r:id="rId4"/>
-    <sheet name="Heatmap" sheetId="4" r:id="rId5"/>
-    <sheet name="Splitability" sheetId="8" r:id="rId6"/>
+    <sheet name="Skill Heatmap" sheetId="4" r:id="rId5"/>
+    <sheet name="Planning and Stabilizing Teams" sheetId="9" r:id="rId6"/>
     <sheet name="Willingness" sheetId="3" state="hidden" r:id="rId7"/>
     <sheet name="Willingness_Calcs" sheetId="7" state="hidden" r:id="rId8"/>
   </sheets>
@@ -25,12 +25,17 @@
     <definedName name="Skills_Header" localSheetId="7">Settings!#REF!</definedName>
     <definedName name="Skills_Header">Settings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="82">
   <si>
     <t>Willing</t>
   </si>
@@ -149,44 +154,140 @@
     <t>Made all settings definable in the Setting tab.</t>
   </si>
   <si>
-    <t>no teacher</t>
+    <t>Will this skill be needed more in the future?</t>
   </si>
   <si>
-    <t>1 teacher</t>
+    <t>How many people are needed to maintain the rate of production support?</t>
   </si>
   <si>
-    <t>no doer</t>
+    <t>Is there a Teacher level person in each location, or at least within the same timezone if a Doer has questions?</t>
   </si>
   <si>
-    <t>1 doer</t>
+    <t>Will this skill be needed by other important projects if they get into difficulty?</t>
   </si>
   <si>
-    <t>no novice</t>
+    <t>How long does it take a teacher to train a novice into Doer level?</t>
   </si>
   <si>
-    <t>1 novice</t>
+    <t>How much effort does it take a teacher to create a doer from a novice, Do I lose the Teacher completely?</t>
   </si>
   <si>
-    <t>no doer. 1 Novice</t>
+    <t>Do we need teacher level on-staff, or can we obtain the training from external consultant?</t>
   </si>
   <si>
-    <t>teach novice into doer - URGENT</t>
+    <t>Is this skill growing in numbers on the hiring community, or decreasing?</t>
   </si>
   <si>
-    <t>1 doer, 1 novice</t>
+    <t>What skills might be needed in higher numbers for stabilization or initial production support? (where will the bug load come from)</t>
   </si>
   <si>
-    <t>teach novice into doer - SOON</t>
+    <t>How can onboarding be accelerated for this skill.</t>
   </si>
   <si>
-    <t>hire teacher level or  external consultant. Create doers, then train one into teacher</t>
+    <t>Is support for this skill needed 24/7 or just during normal hours?</t>
+  </si>
+  <si>
+    <t>How long as a Doer does it take to be a Teacher? Can this be accelerated?</t>
+  </si>
+  <si>
+    <t>2+</t>
+  </si>
+  <si>
+    <t>Teacher</t>
+  </si>
+  <si>
+    <t>Doer</t>
+  </si>
+  <si>
+    <t>Questions -</t>
+  </si>
+  <si>
+    <t>Urgency (Redder = more urgent)</t>
+  </si>
+  <si>
+    <t>Goals -</t>
+  </si>
+  <si>
+    <t>Know what skills might be needed to fix incoming defects or production issues when rolling to customer usage.</t>
+  </si>
+  <si>
+    <t>Know how long (and plan to reduce) the onboarding time from novice to doer levels, prioritized by the skills most anticipated in need for the future.</t>
+  </si>
+  <si>
+    <t>If a skill is in demand, have at least 1 (preferably 2) teachers on the team (or available), and know who is willing (or able) to be a novice in training to doer.</t>
+  </si>
+  <si>
+    <t>Know what skills might be needed elsewhere in the company, as your team members might be pulled off at short notice.</t>
+  </si>
+  <si>
+    <t>Its *not* a goal to have everyone at Teacher level for every skill; Your goal is to have a resiliant team given un-planned disruptions and the next feature demands.</t>
+  </si>
+  <si>
+    <t>Stage 1 - Getting to an Effective and Resiliant Team (Stabilizing Now and Managing Risks)</t>
+  </si>
+  <si>
+    <t>Novice</t>
+  </si>
+  <si>
+    <t>If skill is growing in demand -</t>
+  </si>
+  <si>
+    <t>Have 2+ people who are Doer's for each skill on the team. If creating new innovations, have at least 1 teacher for each skill.</t>
+  </si>
+  <si>
+    <t>Grow a team to have 1 Teacher level for each skill, and 1 Doer level ready to become a Teacher.</t>
+  </si>
+  <si>
+    <t>Split the teams and revisit Stage 1 - Getting to a Stable and Resiliant Team as soon as possible.</t>
+  </si>
+  <si>
+    <t>Build the bench of Novices who can become doers, and promote senior Doers to Teachers.</t>
+  </si>
+  <si>
+    <t>Stage 2 - Gowing a Team to Split, Splitting and the Restabilizing</t>
+  </si>
+  <si>
+    <t>Which Doer's are candidates to become Teacher level for a skill?</t>
+  </si>
+  <si>
+    <t>Who is willing to learn an in-demand skill (become novices)?</t>
+  </si>
+  <si>
+    <t>Can I loan a Teacher from another team to upskill my Doer's or mentor a new Teacher after splitting the team?</t>
+  </si>
+  <si>
+    <t>How many novices do we have ready to fill needed skills?</t>
+  </si>
+  <si>
+    <t>Grow each skill to have at least 3 Doer's in all needed skill areas, even if you don't need that many. You need to be plump on skills to split!</t>
+  </si>
+  <si>
+    <t>Is one location better than another to split?</t>
+  </si>
+  <si>
+    <t>How do I protect the skilsets where the team is at bare minimum (urgency &gt; 5)</t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>Most significant gap in skills</t>
+  </si>
+  <si>
+    <t>Least significant gap in skills</t>
+  </si>
+  <si>
+    <t>Added planning and stabilizing team advice.</t>
+  </si>
+  <si>
+    <t>Todo: Planning new teams.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,8 +382,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -311,6 +442,66 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8696B"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCAA78"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB1D47F"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFA8A72"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB84"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8AC97D"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFECB7E"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD8DF81"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF63BE7B"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -337,16 +528,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -354,10 +545,10 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -375,7 +566,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -407,15 +598,15 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -423,8 +614,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -480,18 +673,66 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="4"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="4" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Calculation" xfId="6" builtinId="22"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="4" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17"/>
     <cellStyle name="Heading 4" xfId="1" builtinId="19"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="5" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="2" builtinId="21"/>
@@ -506,9 +747,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -12200,9 +12438,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -12230,31 +12468,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -12282,23 +12503,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -12475,38 +12679,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2"/>
+  <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="B1:Q23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="2:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="37" t="s">
+    <row r="1" spans="2:17" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-    </row>
-    <row r="2" spans="2:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+    </row>
+    <row r="2" spans="2:17" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="P2" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
       <c r="P4" s="27">
         <v>1</v>
       </c>
@@ -12514,7 +12718,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
       <c r="P5" s="27">
         <v>1.1000000000000001</v>
       </c>
@@ -12522,58 +12726,63 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="P6" s="27"/>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="P6" s="27">
+        <v>1.2</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
       <c r="P7" s="27"/>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
       <c r="P8" s="27"/>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
       <c r="P9" s="27"/>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
       <c r="P10" s="27"/>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
       <c r="P11" s="27"/>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
       <c r="P12" s="27"/>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
       <c r="P13" s="27"/>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
       <c r="P14" s="27"/>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
       <c r="P15" s="27"/>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
       <c r="P16" s="27"/>
     </row>
-    <row r="17" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P17" s="27"/>
     </row>
-    <row r="18" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P18" s="27"/>
     </row>
-    <row r="19" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P19" s="27"/>
     </row>
-    <row r="20" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P20" s="27"/>
     </row>
-    <row r="21" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P21" s="27"/>
     </row>
-    <row r="22" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P22" s="27"/>
     </row>
-    <row r="23" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P23" s="27"/>
     </row>
   </sheetData>
@@ -12581,35 +12790,36 @@
     <mergeCell ref="B1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet3"/>
+  <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
   <dimension ref="B5:K22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.140625" customWidth="1"/>
-    <col min="2" max="2" width="47.140625" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="56.7109375" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" customWidth="1"/>
-    <col min="7" max="7" width="39.28515625" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" customWidth="1"/>
-    <col min="9" max="9" width="48.7109375" customWidth="1"/>
-    <col min="10" max="10" width="5.28515625" customWidth="1"/>
-    <col min="11" max="11" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" customWidth="1"/>
+    <col min="2" max="2" width="47.1640625" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="56.6640625" customWidth="1"/>
+    <col min="5" max="5" width="6.1640625" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" customWidth="1"/>
+    <col min="7" max="7" width="39.33203125" customWidth="1"/>
+    <col min="8" max="8" width="5.1640625" customWidth="1"/>
+    <col min="9" max="9" width="48.6640625" customWidth="1"/>
+    <col min="10" max="10" width="5.33203125" customWidth="1"/>
+    <col min="11" max="11" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>23</v>
       </c>
@@ -12626,7 +12836,7 @@
       </c>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="26" t="s">
         <v>5</v>
       </c>
@@ -12640,7 +12850,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="26" t="s">
         <v>28</v>
       </c>
@@ -12654,7 +12864,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="26" t="s">
         <v>15</v>
       </c>
@@ -12668,7 +12878,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="26"/>
       <c r="D9" s="25"/>
       <c r="G9" s="25" t="s">
@@ -12678,7 +12888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="26"/>
       <c r="D10" s="25"/>
       <c r="G10" s="25" t="s">
@@ -12688,47 +12898,47 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="26"/>
       <c r="D11" s="25"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="26"/>
       <c r="D12" s="25"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13" s="26"/>
       <c r="D13" s="25"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B14" s="26"/>
       <c r="D14" s="25"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B15" s="26"/>
       <c r="D15" s="25"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B16" s="26"/>
       <c r="D16" s="25"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="26"/>
       <c r="D17" s="25"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D18" s="25"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D19" s="25"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D20" s="25"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D21" s="25"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D22" s="25"/>
     </row>
   </sheetData>
@@ -12740,34 +12950,34 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" style="15" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="15" customWidth="1"/>
-    <col min="3" max="4" width="14.28515625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="15" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" style="15" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="15"/>
+    <col min="1" max="1" width="24.5" style="15" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="15" customWidth="1"/>
+    <col min="3" max="4" width="14.33203125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="15" customWidth="1"/>
+    <col min="6" max="6" width="15.5" style="15" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-    </row>
-    <row r="2" spans="1:6" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+    </row>
+    <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
         <v>16</v>
@@ -12788,7 +12998,7 @@
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="14"/>
     </row>
-    <row r="7" spans="1:6" s="22" customFormat="1" ht="34.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" s="22" customFormat="1" ht="34.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="23" t="str">
         <f>Settings!$G$6</f>
         <v>Know nothing</v>
@@ -12997,12 +13207,12 @@
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
     </row>
-    <row r="25" spans="1:6" ht="31.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" s="18" customFormat="1" ht="28" x14ac:dyDescent="0.2">
       <c r="A27" s="22"/>
       <c r="B27" s="23" t="str">
         <f>Settings!$I$6</f>
@@ -13228,22 +13438,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet4"/>
+  <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:E36"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="29.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="29.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="35.28515625" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="35.33203125" customWidth="1"/>
+    <col min="3" max="3" width="32.83203125" customWidth="1"/>
     <col min="4" max="4" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="30"/>
       <c r="B1" s="31" t="str">
         <f>IF(ISBLANK(Settings!$D6),"",Settings!$D6)</f>
@@ -13314,7 +13524,7 @@
         <v/>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="str">
         <f>IF(ISBLANK(Settings!B6),"",Settings!B6)</f>
         <v>Person 1</v>
@@ -13343,7 +13553,7 @@
       <c r="Q2" s="25"/>
       <c r="R2" s="25"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="str">
         <f>IF(ISBLANK(Settings!B7),"",Settings!B7)</f>
         <v>Person 2</v>
@@ -13372,7 +13582,7 @@
       <c r="Q3" s="25"/>
       <c r="R3" s="25"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="str">
         <f>IF(ISBLANK(Settings!B8),"",Settings!B8)</f>
         <v>Team 1</v>
@@ -13401,7 +13611,7 @@
       <c r="Q4" s="25"/>
       <c r="R4" s="25"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="str">
         <f>IF(ISBLANK(Settings!B9),"",Settings!B9)</f>
         <v/>
@@ -13424,7 +13634,7 @@
       <c r="Q5" s="25"/>
       <c r="R5" s="25"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="31" t="str">
         <f>IF(ISBLANK(Settings!B10),"",Settings!B10)</f>
         <v/>
@@ -13447,7 +13657,7 @@
       <c r="Q6" s="25"/>
       <c r="R6" s="25"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="31" t="str">
         <f>IF(ISBLANK(Settings!B11),"",Settings!B11)</f>
         <v/>
@@ -13470,7 +13680,7 @@
       <c r="Q7" s="25"/>
       <c r="R7" s="25"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="31" t="str">
         <f>IF(ISBLANK(Settings!B12),"",Settings!B12)</f>
         <v/>
@@ -13493,7 +13703,7 @@
       <c r="Q8" s="25"/>
       <c r="R8" s="25"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="31" t="str">
         <f>IF(ISBLANK(Settings!B13),"",Settings!B13)</f>
         <v/>
@@ -13516,7 +13726,7 @@
       <c r="Q9" s="25"/>
       <c r="R9" s="25"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="31" t="str">
         <f>IF(ISBLANK(Settings!B14),"",Settings!B14)</f>
         <v/>
@@ -13539,7 +13749,7 @@
       <c r="Q10" s="25"/>
       <c r="R10" s="25"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="31" t="str">
         <f>IF(ISBLANK(Settings!B15),"",Settings!B15)</f>
         <v/>
@@ -13562,7 +13772,7 @@
       <c r="Q11" s="25"/>
       <c r="R11" s="25"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="31" t="str">
         <f>IF(ISBLANK(Settings!B16),"",Settings!B16)</f>
         <v/>
@@ -13585,7 +13795,7 @@
       <c r="Q12" s="25"/>
       <c r="R12" s="25"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="31" t="str">
         <f>IF(ISBLANK(Settings!B17),"",Settings!B17)</f>
         <v/>
@@ -13608,13 +13818,13 @@
       <c r="Q13" s="25"/>
       <c r="R13" s="25"/>
     </row>
-    <row r="14" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="12.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="32"/>
       <c r="B16" s="34" t="str">
         <f>IF(B1&lt;&gt;"",B1,"")</f>
@@ -13685,222 +13895,222 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="33" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="28">
-        <f>Heatmap!B1</f>
+        <f>'Skill Heatmap'!B1</f>
         <v>0</v>
       </c>
       <c r="C17" s="28">
-        <f>Heatmap!C1</f>
+        <f>'Skill Heatmap'!C1</f>
         <v>1</v>
       </c>
       <c r="D17" s="28">
-        <f>Heatmap!D1</f>
+        <f>'Skill Heatmap'!D1</f>
         <v>1</v>
       </c>
       <c r="E17" s="28" t="str">
-        <f>Heatmap!E1</f>
+        <f>'Skill Heatmap'!E1</f>
         <v/>
       </c>
       <c r="F17" s="29" t="str">
-        <f>Heatmap!F1</f>
+        <f>'Skill Heatmap'!F1</f>
         <v/>
       </c>
       <c r="G17" s="29" t="str">
-        <f>Heatmap!G1</f>
+        <f>'Skill Heatmap'!G1</f>
         <v/>
       </c>
       <c r="H17" s="29" t="str">
-        <f>Heatmap!H1</f>
+        <f>'Skill Heatmap'!H1</f>
         <v/>
       </c>
       <c r="I17" s="29" t="str">
-        <f>Heatmap!I1</f>
+        <f>'Skill Heatmap'!I1</f>
         <v/>
       </c>
       <c r="J17" s="29" t="str">
-        <f>Heatmap!J1</f>
+        <f>'Skill Heatmap'!J1</f>
         <v/>
       </c>
       <c r="K17" s="29" t="str">
-        <f>Heatmap!K1</f>
+        <f>'Skill Heatmap'!K1</f>
         <v/>
       </c>
       <c r="L17" s="29" t="str">
-        <f>Heatmap!L1</f>
+        <f>'Skill Heatmap'!L1</f>
         <v/>
       </c>
       <c r="M17" s="29" t="str">
-        <f>Heatmap!M1</f>
+        <f>'Skill Heatmap'!M1</f>
         <v/>
       </c>
       <c r="N17" s="29" t="str">
-        <f>Heatmap!N1</f>
+        <f>'Skill Heatmap'!N1</f>
         <v/>
       </c>
       <c r="O17" s="29" t="str">
-        <f>Heatmap!O1</f>
+        <f>'Skill Heatmap'!O1</f>
         <v/>
       </c>
       <c r="P17" s="29" t="str">
-        <f>Heatmap!P1</f>
+        <f>'Skill Heatmap'!P1</f>
         <v/>
       </c>
       <c r="Q17" s="29" t="str">
-        <f>Heatmap!Q1</f>
+        <f>'Skill Heatmap'!Q1</f>
         <v/>
       </c>
       <c r="R17" s="29" t="str">
-        <f>Heatmap!R1</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+        <f>'Skill Heatmap'!R1</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="33" t="s">
         <v>29</v>
       </c>
       <c r="B18" s="28">
-        <f>Heatmap!B2</f>
+        <f>'Skill Heatmap'!B2</f>
         <v>1</v>
       </c>
       <c r="C18" s="28">
-        <f>Heatmap!C2</f>
+        <f>'Skill Heatmap'!C2</f>
         <v>1</v>
       </c>
       <c r="D18" s="28">
-        <f>Heatmap!D2</f>
+        <f>'Skill Heatmap'!D2</f>
         <v>2</v>
       </c>
       <c r="E18" s="28" t="str">
-        <f>Heatmap!E2</f>
+        <f>'Skill Heatmap'!E2</f>
         <v/>
       </c>
       <c r="F18" s="29" t="str">
-        <f>Heatmap!F2</f>
+        <f>'Skill Heatmap'!F2</f>
         <v/>
       </c>
       <c r="G18" s="29" t="str">
-        <f>Heatmap!G2</f>
+        <f>'Skill Heatmap'!G2</f>
         <v/>
       </c>
       <c r="H18" s="29" t="str">
-        <f>Heatmap!H2</f>
+        <f>'Skill Heatmap'!H2</f>
         <v/>
       </c>
       <c r="I18" s="29" t="str">
-        <f>Heatmap!I2</f>
+        <f>'Skill Heatmap'!I2</f>
         <v/>
       </c>
       <c r="J18" s="29" t="str">
-        <f>Heatmap!J2</f>
+        <f>'Skill Heatmap'!J2</f>
         <v/>
       </c>
       <c r="K18" s="29" t="str">
-        <f>Heatmap!K2</f>
+        <f>'Skill Heatmap'!K2</f>
         <v/>
       </c>
       <c r="L18" s="29" t="str">
-        <f>Heatmap!L2</f>
+        <f>'Skill Heatmap'!L2</f>
         <v/>
       </c>
       <c r="M18" s="29" t="str">
-        <f>Heatmap!M2</f>
+        <f>'Skill Heatmap'!M2</f>
         <v/>
       </c>
       <c r="N18" s="29" t="str">
-        <f>Heatmap!N2</f>
+        <f>'Skill Heatmap'!N2</f>
         <v/>
       </c>
       <c r="O18" s="29" t="str">
-        <f>Heatmap!O2</f>
+        <f>'Skill Heatmap'!O2</f>
         <v/>
       </c>
       <c r="P18" s="29" t="str">
-        <f>Heatmap!P2</f>
+        <f>'Skill Heatmap'!P2</f>
         <v/>
       </c>
       <c r="Q18" s="29" t="str">
-        <f>Heatmap!Q2</f>
+        <f>'Skill Heatmap'!Q2</f>
         <v/>
       </c>
       <c r="R18" s="29" t="str">
-        <f>Heatmap!R2</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+        <f>'Skill Heatmap'!R2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="33" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="28">
-        <f>Heatmap!B3</f>
+        <f>'Skill Heatmap'!B3</f>
         <v>0</v>
       </c>
       <c r="C19" s="28">
-        <f>Heatmap!C3</f>
+        <f>'Skill Heatmap'!C3</f>
         <v>0</v>
       </c>
       <c r="D19" s="28">
-        <f>Heatmap!D3</f>
+        <f>'Skill Heatmap'!D3</f>
         <v>1</v>
       </c>
       <c r="E19" s="28" t="str">
-        <f>Heatmap!E3</f>
+        <f>'Skill Heatmap'!E3</f>
         <v/>
       </c>
       <c r="F19" s="29" t="str">
-        <f>Heatmap!F3</f>
+        <f>'Skill Heatmap'!F3</f>
         <v/>
       </c>
       <c r="G19" s="29" t="str">
-        <f>Heatmap!G3</f>
+        <f>'Skill Heatmap'!G3</f>
         <v/>
       </c>
       <c r="H19" s="29" t="str">
-        <f>Heatmap!H3</f>
+        <f>'Skill Heatmap'!H3</f>
         <v/>
       </c>
       <c r="I19" s="29" t="str">
-        <f>Heatmap!I3</f>
+        <f>'Skill Heatmap'!I3</f>
         <v/>
       </c>
       <c r="J19" s="29" t="str">
-        <f>Heatmap!J3</f>
+        <f>'Skill Heatmap'!J3</f>
         <v/>
       </c>
       <c r="K19" s="29" t="str">
-        <f>Heatmap!K3</f>
+        <f>'Skill Heatmap'!K3</f>
         <v/>
       </c>
       <c r="L19" s="29" t="str">
-        <f>Heatmap!L3</f>
+        <f>'Skill Heatmap'!L3</f>
         <v/>
       </c>
       <c r="M19" s="29" t="str">
-        <f>Heatmap!M3</f>
+        <f>'Skill Heatmap'!M3</f>
         <v/>
       </c>
       <c r="N19" s="29" t="str">
-        <f>Heatmap!N3</f>
+        <f>'Skill Heatmap'!N3</f>
         <v/>
       </c>
       <c r="O19" s="29" t="str">
-        <f>Heatmap!O3</f>
+        <f>'Skill Heatmap'!O3</f>
         <v/>
       </c>
       <c r="P19" s="29" t="str">
-        <f>Heatmap!P3</f>
+        <f>'Skill Heatmap'!P3</f>
         <v/>
       </c>
       <c r="Q19" s="29" t="str">
-        <f>Heatmap!Q3</f>
+        <f>'Skill Heatmap'!Q3</f>
         <v/>
       </c>
       <c r="R19" s="29" t="str">
-        <f>Heatmap!R3</f>
+        <f>'Skill Heatmap'!R3</f>
         <v/>
       </c>
     </row>
@@ -13955,22 +14165,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:R28"/>
+  <sheetPr codeName="Sheet5" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -14043,7 +14253,7 @@
         <v/>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>29</v>
       </c>
@@ -14116,7 +14326,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
@@ -14189,10 +14399,10 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:18" s="35" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" s="35" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="36" t="str">
         <f>IF(Input!B1&lt;&gt;"",Input!B1,"")</f>
         <v>CSS</v>
@@ -14262,7 +14472,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="str">
         <f>Input!A2</f>
         <v>Person 1</v>
@@ -14336,7 +14546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="str">
         <f>Input!A3</f>
         <v>Person 2</v>
@@ -14410,7 +14620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="str">
         <f>Input!A4</f>
         <v>Team 1</v>
@@ -14484,7 +14694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="str">
         <f>Input!A5</f>
         <v/>
@@ -14558,7 +14768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="str">
         <f>Input!A6</f>
         <v/>
@@ -14632,7 +14842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="str">
         <f>Input!A7</f>
         <v/>
@@ -14706,7 +14916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="str">
         <f>Input!A8</f>
         <v/>
@@ -14780,7 +14990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="str">
         <f>Input!A9</f>
         <v/>
@@ -14854,7 +15064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="str">
         <f>Input!A10</f>
         <v/>
@@ -14928,7 +15138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="str">
         <f>Input!A11</f>
         <v/>
@@ -15002,7 +15212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="str">
         <f>Input!A12</f>
         <v/>
@@ -15076,7 +15286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="str">
         <f>Input!A13</f>
         <v/>
@@ -15150,7 +15360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="6">
         <f t="shared" ref="B18:R18" si="3">SUM(B6:B17)</f>
         <v>2</v>
@@ -15220,84 +15430,82 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B20" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20">
+    <row r="19" spans="1:20" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B20" s="9"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B21" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B22" s="56">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B23" s="56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B24" s="56">
         <v>3</v>
       </c>
-      <c r="E20" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21">
-        <v>6</v>
-      </c>
-      <c r="E21" t="s">
-        <v>45</v>
-      </c>
-      <c r="F21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B22" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B23" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B24" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24">
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B25" s="56">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B25" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B26" s="56">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B26" s="9"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B27" s="9"/>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B28" s="9"/>
+      <c r="C26" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S27" s="37"/>
+      <c r="T27" s="37"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B18:R18">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:R17">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B22:B26">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -15308,31 +15516,14 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6:R17">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="8" id="{339E999E-0713-46E1-92D7-78E999ECB110}">
+          <x14:cfRule type="iconSet" priority="11" id="{339E999E-0713-46E1-92D7-78E999ECB110}">
             <x14:iconSet iconSet="4TrafficLights" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -15362,32 +15553,454 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="41"/>
+    </row>
+    <row r="2" spans="1:9" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="38"/>
+      <c r="B5" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="39">
+        <v>0</v>
+      </c>
+      <c r="C6" s="39">
+        <v>1</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="38">
+        <v>0</v>
+      </c>
+      <c r="H6" s="38">
+        <v>1</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="38">
+        <v>0</v>
+      </c>
+      <c r="B7" s="7">
+        <v>9</v>
+      </c>
+      <c r="C7" s="7">
+        <v>7</v>
+      </c>
+      <c r="D7" s="7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="38">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7">
+        <v>9</v>
+      </c>
+      <c r="H7" s="7">
+        <v>7</v>
+      </c>
+      <c r="I7" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="38">
+        <v>1</v>
+      </c>
+      <c r="B8" s="7">
+        <v>8</v>
+      </c>
+      <c r="C8" s="7">
+        <v>5</v>
+      </c>
+      <c r="D8" s="7">
+        <v>2</v>
+      </c>
+      <c r="F8" s="38">
+        <v>1</v>
+      </c>
+      <c r="G8" s="7">
+        <v>8</v>
+      </c>
+      <c r="H8" s="7">
+        <v>5</v>
+      </c>
+      <c r="I8" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="7">
+        <v>6</v>
+      </c>
+      <c r="C9" s="7">
+        <v>4</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1</v>
+      </c>
+      <c r="F9" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="7">
+        <v>6</v>
+      </c>
+      <c r="H9" s="7">
+        <v>4</v>
+      </c>
+      <c r="I9" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="40" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="40" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="40" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="40" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="40" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="40" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="40" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="40" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="40" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="40" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="40" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="40" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="40" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="40" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="40" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="44"/>
+      <c r="C35" s="44"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="41"/>
+    </row>
+    <row r="36" spans="1:14" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A39" s="38"/>
+      <c r="B39" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A40" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="38">
+        <v>0</v>
+      </c>
+      <c r="C40" s="38">
+        <v>1</v>
+      </c>
+      <c r="D40" s="38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41" s="38">
+        <v>0</v>
+      </c>
+      <c r="B41" s="47">
+        <v>9</v>
+      </c>
+      <c r="C41" s="48">
+        <v>7</v>
+      </c>
+      <c r="D41" s="49">
+        <v>3</v>
+      </c>
+      <c r="H41" s="37"/>
+      <c r="I41" s="37"/>
+      <c r="J41" s="37"/>
+      <c r="K41" s="37"/>
+      <c r="L41" s="37"/>
+      <c r="M41" s="37"/>
+      <c r="N41" s="37"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A42" s="38">
+        <v>1</v>
+      </c>
+      <c r="B42" s="50">
+        <v>8</v>
+      </c>
+      <c r="C42" s="51">
+        <v>5</v>
+      </c>
+      <c r="D42" s="52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" s="53">
+        <v>6</v>
+      </c>
+      <c r="C43" s="54">
+        <v>4</v>
+      </c>
+      <c r="D43" s="55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A46" s="40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47" s="40" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A48" s="40" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="40" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="46" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="40" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="40" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="40" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="40" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="45" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B7:D9">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7:I9">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet7"/>
+  <sheetPr codeName="Sheet7" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="24.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" style="9"/>
+    <col min="1" max="1" width="24.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="13"/>
       <c r="B1" s="13" t="str">
         <f>IF(Input!B1&lt;&gt;"",Input!B1,"")</f>
@@ -15470,7 +16083,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="str">
         <f>IF(Input!A2&lt;&gt;"", Input!A2, "")</f>
         <v>Person 1</v>
@@ -15502,7 +16115,7 @@
       <c r="T2" s="12"/>
       <c r="U2" s="12"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="str">
         <f>IF(Input!A3&lt;&gt;"", Input!A3, "")</f>
         <v>Person 2</v>
@@ -15530,7 +16143,7 @@
       <c r="T3" s="12"/>
       <c r="U3" s="12"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="str">
         <f>IF(Input!A4&lt;&gt;"", Input!A4, "")</f>
         <v>Team 1</v>
@@ -15556,7 +16169,7 @@
       <c r="T4" s="12"/>
       <c r="U4" s="12"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="str">
         <f>IF(Input!A5&lt;&gt;"", Input!A5, "")</f>
         <v/>
@@ -15582,7 +16195,7 @@
       <c r="T5" s="12"/>
       <c r="U5" s="12"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="str">
         <f>IF(Input!A6&lt;&gt;"", Input!A6, "")</f>
         <v/>
@@ -15608,7 +16221,7 @@
       <c r="T6" s="12"/>
       <c r="U6" s="12"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="str">
         <f>IF(Input!A7&lt;&gt;"", Input!A7, "")</f>
         <v/>
@@ -15634,7 +16247,7 @@
       <c r="T7" s="12"/>
       <c r="U7" s="12"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="str">
         <f>IF(Input!A8&lt;&gt;"", Input!A8, "")</f>
         <v/>
@@ -15660,7 +16273,7 @@
       <c r="T8" s="12"/>
       <c r="U8" s="12"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="str">
         <f>IF(Input!A9&lt;&gt;"", Input!A9, "")</f>
         <v/>
@@ -15686,7 +16299,7 @@
       <c r="T9" s="12"/>
       <c r="U9" s="12"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="str">
         <f>IF(Input!A10&lt;&gt;"", Input!A10, "")</f>
         <v/>
@@ -15712,7 +16325,7 @@
       <c r="T10" s="12"/>
       <c r="U10" s="12"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="str">
         <f>IF(Input!A11&lt;&gt;"", Input!A11, "")</f>
         <v/>
@@ -15738,7 +16351,7 @@
       <c r="T11" s="12"/>
       <c r="U11" s="12"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="str">
         <f>IF(Input!A12&lt;&gt;"", Input!A12, "")</f>
         <v/>
@@ -15764,7 +16377,7 @@
       <c r="T12" s="12"/>
       <c r="U12" s="12"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="str">
         <f>IF(Input!A13&lt;&gt;"", Input!A13, "")</f>
         <v/>
@@ -15790,7 +16403,7 @@
       <c r="T13" s="12"/>
       <c r="U13" s="12"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="e">
         <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
         <v>#REF!</v>
@@ -15816,7 +16429,7 @@
       <c r="T14" s="12"/>
       <c r="U14" s="12"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="e">
         <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
         <v>#REF!</v>
@@ -15842,7 +16455,7 @@
       <c r="T15" s="12"/>
       <c r="U15" s="12"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="e">
         <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
         <v>#REF!</v>
@@ -15868,7 +16481,7 @@
       <c r="T16" s="12"/>
       <c r="U16" s="12"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="e">
         <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
         <v>#REF!</v>
@@ -15894,7 +16507,7 @@
       <c r="T17" s="12"/>
       <c r="U17" s="12"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="e">
         <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
         <v>#REF!</v>
@@ -15920,7 +16533,7 @@
       <c r="T18" s="12"/>
       <c r="U18" s="12"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="e">
         <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
         <v>#REF!</v>
@@ -15946,7 +16559,7 @@
       <c r="T19" s="12"/>
       <c r="U19" s="12"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="e">
         <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
         <v>#REF!</v>
@@ -15972,7 +16585,7 @@
       <c r="T20" s="12"/>
       <c r="U20" s="12"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="e">
         <f>IF(Input!#REF!&lt;&gt;"", Input!#REF!, "")</f>
         <v>#REF!</v>
@@ -15998,12 +16611,12 @@
       <c r="T21" s="12"/>
       <c r="U21" s="12"/>
     </row>
-    <row r="23" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10"/>
       <c r="B24" s="3" t="str">
         <f>IF(B1&lt;&gt;"",B1,"")</f>
@@ -16086,7 +16699,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>0</v>
       </c>
@@ -16171,7 +16784,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
         <v>14</v>
       </c>
@@ -16256,7 +16869,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
         <v>13</v>
       </c>
@@ -16388,22 +17001,22 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet8"/>
+  <sheetPr codeName="Sheet8" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.5" customWidth="1"/>
+    <col min="6" max="6" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -16488,7 +17101,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -16573,7 +17186,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -16658,7 +17271,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="9" t="str">
         <f>IF(Input!B1&lt;&gt;"",Input!B1,"")</f>
         <v>CSS</v>
@@ -16740,7 +17353,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="str">
         <f>Input!A2</f>
         <v>Person 1</v>
@@ -16826,7 +17439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="str">
         <f>Input!A3</f>
         <v>Person 2</v>
@@ -16912,7 +17525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="str">
         <f>Input!A4</f>
         <v>Team 1</v>
@@ -16998,7 +17611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="str">
         <f>Input!A5</f>
         <v/>
@@ -17084,7 +17697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="str">
         <f>Input!A6</f>
         <v/>
@@ -17170,7 +17783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="str">
         <f>Input!A7</f>
         <v/>
@@ -17256,7 +17869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="str">
         <f>Input!A8</f>
         <v/>
@@ -17342,7 +17955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="str">
         <f>Input!A9</f>
         <v/>
@@ -17428,7 +18041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="str">
         <f>Input!A10</f>
         <v/>
@@ -17514,7 +18127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="str">
         <f>Input!A11</f>
         <v/>
@@ -17600,7 +18213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="str">
         <f>Input!A12</f>
         <v/>
@@ -17686,7 +18299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="str">
         <f>Input!A13</f>
         <v/>
@@ -17772,7 +18385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="e">
         <f>Input!#REF!</f>
         <v>#REF!</v>
@@ -17858,7 +18471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="e">
         <f>Input!#REF!</f>
         <v>#REF!</v>
@@ -17944,7 +18557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="e">
         <f>Input!#REF!</f>
         <v>#REF!</v>
@@ -18030,7 +18643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="e">
         <f>Input!#REF!</f>
         <v>#REF!</v>
@@ -18116,7 +18729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="e">
         <f>Input!#REF!</f>
         <v>#REF!</v>
@@ -18202,7 +18815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="e">
         <f>Input!#REF!</f>
         <v>#REF!</v>
@@ -18288,7 +18901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="e">
         <f>Input!#REF!</f>
         <v>#REF!</v>
@@ -18374,7 +18987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="e">
         <f>Input!#REF!</f>
         <v>#REF!</v>
@@ -18460,7 +19073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="6">
         <f>SUM(B5:B24)</f>
         <v>4</v>
@@ -18542,7 +19155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:21" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <conditionalFormatting sqref="B5:U24">
     <cfRule type="colorScale" priority="3">

</xml_diff>